<commit_message>
10/11/16 open-close browser main scpt file ( don't know what chaged or why, also desk top short cuts
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28740" yWindow="720" windowWidth="29660" windowHeight="17460" tabRatio="650" firstSheet="14" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13960" tabRatio="650" firstSheet="15" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,10 @@
     <sheet name="humm" sheetId="38" r:id="rId26"/>
     <sheet name="8.19" sheetId="39" r:id="rId27"/>
     <sheet name="9.20" sheetId="41" r:id="rId28"/>
+    <sheet name="10.3" sheetId="42" r:id="rId29"/>
   </sheets>
   <definedNames>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="9">'3.25'!$A$1:$L$16</definedName>
@@ -153,29 +155,32 @@
   <connection id="26" name="Connection31" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="27" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="27" name="Connection32" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="28" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/index/12800?metric=tests/profiles/changelog?key=xml-murano-services-xml-profile-81269&amp;since=2015-09-02T19%3A11%3A38%2B0000&amp;to=2016-01-14T22%3A14%3A37%2B0000" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="28" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="29" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="29" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="30" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="30" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="31" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="31" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="32" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="32" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="33" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-mjenk01.dev.svbank.com:8080/job/T2%20web-payment-test-master/lastBuild/consoleText" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="336">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1163,6 +1168,27 @@
   <si>
     <t>~/svb-web-payments/integration$ grep -r "\sit(" * |  wc</t>
   </si>
+  <si>
+    <t>Mur Service OOBA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> results</t>
+  </si>
+  <si>
+    <t>Component Test</t>
+  </si>
+  <si>
+    <t>utB</t>
+  </si>
+  <si>
+    <t>Application Level</t>
+  </si>
+  <si>
+    <t>Mock and Backend</t>
+  </si>
+  <si>
+    <t>Oct 3, 2016</t>
+  </si>
 </sst>
 </file>
 
@@ -1717,7 +1743,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="64">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1782,8 +1808,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2063,6 +2099,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2083,8 +2125,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="64">
+  <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2147,6 +2199,16 @@
     <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2248,7 +2310,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2292,7 +2354,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2323,8 +2385,12 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+</file>
+
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2675,8 +2741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1034"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="Q63" sqref="Q63"/>
+    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -8413,13 +8479,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8456,9 +8522,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9040,20 +9106,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9516,13 +9582,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9559,9 +9625,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10143,20 +10209,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10351,13 +10417,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="143" t="s">
+      <c r="U25" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="144"/>
-      <c r="W25" s="144"/>
-      <c r="X25" s="144"/>
-      <c r="Y25" s="145"/>
+      <c r="V25" s="146"/>
+      <c r="W25" s="146"/>
+      <c r="X25" s="146"/>
+      <c r="Y25" s="147"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10370,9 +10436,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="146"/>
-      <c r="V26" s="147"/>
-      <c r="W26" s="147"/>
+      <c r="U26" s="148"/>
+      <c r="V26" s="149"/>
+      <c r="W26" s="149"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10766,13 +10832,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -10809,9 +10875,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11401,20 +11467,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -11937,13 +12003,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -11980,9 +12046,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12583,20 +12649,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13141,13 +13207,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13184,9 +13250,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -13797,20 +13863,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14347,13 +14413,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14390,9 +14456,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15003,20 +15069,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15553,13 +15619,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15596,9 +15662,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16209,20 +16275,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16759,13 +16825,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -16802,9 +16868,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17415,20 +17481,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -17968,13 +18034,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18011,9 +18077,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18627,20 +18693,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19117,13 +19183,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19160,9 +19226,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19776,20 +19842,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -20763,7 +20829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -20931,13 +20997,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -20974,9 +21040,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21590,20 +21656,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -22693,20 +22759,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -23789,20 +23855,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="142" t="s">
+      <c r="A15" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="142"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="142"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="142"/>
-      <c r="L15" s="142"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="144"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="144"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -25783,21 +25849,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
-      <c r="M16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
+      <c r="M16" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -25843,8 +25909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="Q23" sqref="O23:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -26661,21 +26727,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
-      <c r="M16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
+      <c r="M16" s="144"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27556,20 +27622,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -28266,8 +28332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -29008,20 +29074,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -29318,8 +29384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -30055,20 +30121,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="142" t="s">
+      <c r="A17" s="144" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="142"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="142"/>
-      <c r="H17" s="142"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="142"/>
-      <c r="L17" s="142"/>
+      <c r="B17" s="144"/>
+      <c r="C17" s="144"/>
+      <c r="D17" s="144"/>
+      <c r="E17" s="144"/>
+      <c r="F17" s="144"/>
+      <c r="G17" s="144"/>
+      <c r="H17" s="144"/>
+      <c r="I17" s="144"/>
+      <c r="J17" s="144"/>
+      <c r="K17" s="144"/>
+      <c r="L17" s="144"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30079,13 +30145,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="148" t="s">
+      <c r="O19" s="150" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="149"/>
-      <c r="Q19" s="149"/>
-      <c r="R19" s="149"/>
-      <c r="S19" s="150"/>
+      <c r="P19" s="151"/>
+      <c r="Q19" s="151"/>
+      <c r="R19" s="151"/>
+      <c r="S19" s="152"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -30343,6 +30409,1137 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18:U30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1"/>
+    <col min="17" max="17" width="25.5" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="45">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>266</v>
+      </c>
+      <c r="R1" t="s">
+        <v>160</v>
+      </c>
+      <c r="S1">
+        <f>SUM(R3:R10)</f>
+        <v>223</v>
+      </c>
+      <c r="T1" t="str">
+        <f>C1</f>
+        <v xml:space="preserve">UTs </v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="142">
+        <v>581</v>
+      </c>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="23">
+        <v>6209</v>
+      </c>
+      <c r="G2" s="142" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="26">
+        <v>0.52916666666666667</v>
+      </c>
+      <c r="I2" s="25">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="J2" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K2" s="142">
+        <v>0</v>
+      </c>
+      <c r="L2" s="142">
+        <v>0</v>
+      </c>
+      <c r="M2" s="142">
+        <v>2</v>
+      </c>
+      <c r="N2" s="142">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2:T17" si="0">C2</f>
+        <v>581</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="142">
+        <v>194</v>
+      </c>
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="23">
+        <v>1760</v>
+      </c>
+      <c r="G3" s="142" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="26">
+        <v>0.6020833333333333</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J3" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K3" s="142">
+        <v>0</v>
+      </c>
+      <c r="L3" s="142">
+        <v>0</v>
+      </c>
+      <c r="M3" s="142">
+        <v>2</v>
+      </c>
+      <c r="N3" s="142">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>265</v>
+      </c>
+      <c r="R3">
+        <v>26</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="142">
+        <v>132</v>
+      </c>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="142">
+        <v>871</v>
+      </c>
+      <c r="G4" s="142" t="s">
+        <v>226</v>
+      </c>
+      <c r="H4" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0.95</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K4" s="142">
+        <v>0</v>
+      </c>
+      <c r="L4" s="142">
+        <v>0</v>
+      </c>
+      <c r="M4" s="142">
+        <v>2</v>
+      </c>
+      <c r="N4" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>258</v>
+      </c>
+      <c r="R4">
+        <v>150</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="142">
+        <v>114</v>
+      </c>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
+      <c r="F5" s="23">
+        <v>1577</v>
+      </c>
+      <c r="G5" s="142" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="K5" s="142">
+        <v>0</v>
+      </c>
+      <c r="L5" s="142">
+        <v>0</v>
+      </c>
+      <c r="M5" s="142">
+        <v>0</v>
+      </c>
+      <c r="N5" s="142">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>259</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="142">
+        <v>76</v>
+      </c>
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="142">
+        <v>563</v>
+      </c>
+      <c r="G6" s="142" t="s">
+        <v>248</v>
+      </c>
+      <c r="H6" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="K6" s="142">
+        <v>0</v>
+      </c>
+      <c r="L6" s="142">
+        <v>0</v>
+      </c>
+      <c r="M6" s="142">
+        <v>1</v>
+      </c>
+      <c r="N6" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
+      <c r="A7" s="20"/>
+      <c r="B7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="142">
+        <v>69</v>
+      </c>
+      <c r="D7" s="143"/>
+      <c r="E7" s="143"/>
+      <c r="F7" s="142">
+        <v>839</v>
+      </c>
+      <c r="G7" s="142" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="J7" s="25">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="K7" s="142">
+        <v>0</v>
+      </c>
+      <c r="L7" s="142">
+        <v>0</v>
+      </c>
+      <c r="M7" s="142">
+        <v>2</v>
+      </c>
+      <c r="N7" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>268</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="142">
+        <v>61</v>
+      </c>
+      <c r="D8" s="143"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="142">
+        <v>693</v>
+      </c>
+      <c r="G8" s="142" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0.65138888888888891</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="J8" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="K8" s="142">
+        <v>0</v>
+      </c>
+      <c r="L8" s="142">
+        <v>0</v>
+      </c>
+      <c r="M8" s="142">
+        <v>0</v>
+      </c>
+      <c r="N8" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R8">
+        <v>25</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="142">
+        <v>59</v>
+      </c>
+      <c r="D9" s="143"/>
+      <c r="E9" s="143"/>
+      <c r="F9" s="142">
+        <v>344</v>
+      </c>
+      <c r="G9" s="142">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J9" s="25">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="K9" s="142">
+        <v>0</v>
+      </c>
+      <c r="L9" s="142">
+        <v>0</v>
+      </c>
+      <c r="M9" s="142">
+        <v>0</v>
+      </c>
+      <c r="N9" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>263</v>
+      </c>
+      <c r="R9">
+        <v>5</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="142">
+        <v>44</v>
+      </c>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="142">
+        <v>573</v>
+      </c>
+      <c r="G10" s="142" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="24">
+        <v>42643</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="K10" s="142">
+        <v>0</v>
+      </c>
+      <c r="L10" s="142">
+        <v>0</v>
+      </c>
+      <c r="M10" s="142">
+        <v>1</v>
+      </c>
+      <c r="N10" s="142">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>264</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="142">
+        <v>36</v>
+      </c>
+      <c r="D11" s="143"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="142">
+        <v>195</v>
+      </c>
+      <c r="G11" s="142">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J11" s="25">
+        <v>1</v>
+      </c>
+      <c r="K11" s="142">
+        <v>0</v>
+      </c>
+      <c r="L11" s="142">
+        <v>0</v>
+      </c>
+      <c r="M11" s="142">
+        <v>0</v>
+      </c>
+      <c r="N11" s="142">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="142">
+        <v>31</v>
+      </c>
+      <c r="D12" s="143"/>
+      <c r="E12" s="143"/>
+      <c r="F12" s="142">
+        <v>378</v>
+      </c>
+      <c r="G12" s="142" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K12" s="142">
+        <v>0</v>
+      </c>
+      <c r="L12" s="142">
+        <v>0</v>
+      </c>
+      <c r="M12" s="142">
+        <v>1</v>
+      </c>
+      <c r="N12" s="142">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" s="142">
+        <v>22</v>
+      </c>
+      <c r="D13" s="143"/>
+      <c r="E13" s="143"/>
+      <c r="F13" s="142">
+        <v>318</v>
+      </c>
+      <c r="G13" s="142" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="26">
+        <v>0.69652777777777775</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="142">
+        <v>0</v>
+      </c>
+      <c r="L13" s="142">
+        <v>0</v>
+      </c>
+      <c r="M13" s="142">
+        <v>1</v>
+      </c>
+      <c r="N13" s="142">
+        <v>2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="142">
+        <v>18</v>
+      </c>
+      <c r="D14" s="143"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="142">
+        <v>172</v>
+      </c>
+      <c r="G14" s="142">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="K14" s="142">
+        <v>0</v>
+      </c>
+      <c r="L14" s="142">
+        <v>0</v>
+      </c>
+      <c r="M14" s="142">
+        <v>0</v>
+      </c>
+      <c r="N14" s="142">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="U14">
+        <f>SUM(T2:T15)</f>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="142">
+        <v>13</v>
+      </c>
+      <c r="D15" s="143"/>
+      <c r="E15" s="143"/>
+      <c r="F15" s="142">
+        <v>218</v>
+      </c>
+      <c r="G15" s="142">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>42640</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K15" s="142">
+        <v>0</v>
+      </c>
+      <c r="L15" s="142">
+        <v>0</v>
+      </c>
+      <c r="M15" s="142">
+        <v>0</v>
+      </c>
+      <c r="N15" s="142">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="31">
+        <f>C22</f>
+        <v>91</v>
+      </c>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="23">
+        <v>3041</v>
+      </c>
+      <c r="G16" s="142">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
+        <v>42578</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K16" s="142">
+        <v>0</v>
+      </c>
+      <c r="L16" s="142">
+        <v>0</v>
+      </c>
+      <c r="M16" s="142">
+        <v>0</v>
+      </c>
+      <c r="N16" s="142">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="U16">
+        <f>SUM(T16:T17)</f>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="31">
+        <f>C24</f>
+        <v>491</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="23">
+        <v>10346</v>
+      </c>
+      <c r="G17" s="142" t="s">
+        <v>154</v>
+      </c>
+      <c r="H17" s="26">
+        <v>0.4368055555555555</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K17" s="142">
+        <v>0</v>
+      </c>
+      <c r="L17" s="142">
+        <v>0</v>
+      </c>
+      <c r="M17" s="142">
+        <v>0</v>
+      </c>
+      <c r="N17" s="142">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" thickBot="1">
+      <c r="A18" s="144" t="s">
+        <v>330</v>
+      </c>
+      <c r="B18" s="144"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="144"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="144"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="144"/>
+      <c r="K18" s="144"/>
+      <c r="L18" s="144"/>
+      <c r="M18" s="144"/>
+      <c r="N18" s="144"/>
+    </row>
+    <row r="19" spans="1:21" ht="15" thickBot="1">
+      <c r="B19" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q19" s="150" t="s">
+        <v>164</v>
+      </c>
+      <c r="R19" s="151"/>
+      <c r="S19" s="151"/>
+      <c r="T19" s="151"/>
+      <c r="U19" s="152"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="B20" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q20" s="124"/>
+      <c r="R20" s="125"/>
+      <c r="S20" s="125"/>
+      <c r="T20" s="153" t="s">
+        <v>165</v>
+      </c>
+      <c r="U20" s="154" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="Q21" s="128"/>
+      <c r="R21" s="129"/>
+      <c r="S21" s="129"/>
+      <c r="T21" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="U21" s="155"/>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="B22" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22">
+        <v>91</v>
+      </c>
+      <c r="F22" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q22" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="133"/>
+      <c r="S22" s="134"/>
+      <c r="T22" s="135">
+        <f>S1</f>
+        <v>223</v>
+      </c>
+      <c r="U22" s="156">
+        <f>T22/$T$29</f>
+        <v>9.1281211625051165E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="F23" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q23" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="R23" s="133" t="s">
+        <v>333</v>
+      </c>
+      <c r="S23" s="134" t="s">
+        <v>334</v>
+      </c>
+      <c r="T23" s="135">
+        <f>C38</f>
+        <v>188</v>
+      </c>
+      <c r="U23" s="156">
+        <f t="shared" ref="U23:U28" si="1">T23/$T$29</f>
+        <v>7.6954564060581251E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="B24" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24">
+        <v>491</v>
+      </c>
+      <c r="F24" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q24" s="132"/>
+      <c r="R24" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="S24" s="134"/>
+      <c r="T24" s="135">
+        <v>0</v>
+      </c>
+      <c r="U24" s="156"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="F25" s="58"/>
+      <c r="Q25" s="132"/>
+      <c r="R25" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="S25" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T25" s="135">
+        <f>U14</f>
+        <v>1450</v>
+      </c>
+      <c r="U25" s="156">
+        <f t="shared" si="1"/>
+        <v>0.59353254195661076</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="B26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q26" s="132"/>
+      <c r="R26" s="133" t="s">
+        <v>331</v>
+      </c>
+      <c r="S26" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T26" s="158"/>
+      <c r="U26" s="156"/>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="C27" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q27" s="132"/>
+      <c r="R27" s="133"/>
+      <c r="S27" s="134" t="s">
+        <v>171</v>
+      </c>
+      <c r="T27" s="135">
+        <f>U16</f>
+        <v>582</v>
+      </c>
+      <c r="U27" s="156">
+        <f t="shared" si="1"/>
+        <v>0.23823168235775685</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="C28" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q28" s="132"/>
+      <c r="R28" s="133"/>
+      <c r="S28" s="134"/>
+      <c r="T28" s="135"/>
+      <c r="U28" s="156"/>
+    </row>
+    <row r="29" spans="1:21" ht="15" thickBot="1">
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q29" s="137"/>
+      <c r="R29" s="138"/>
+      <c r="S29" s="139"/>
+      <c r="T29" s="140">
+        <f>SUM(T22:T27)</f>
+        <v>2443</v>
+      </c>
+      <c r="U29" s="157">
+        <f>SUM(U22:U28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="C30" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="B32" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" s="122"/>
+      <c r="D32" s="122"/>
+      <c r="E32" s="122"/>
+      <c r="F32" s="123" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="H32" s="122"/>
+      <c r="I32" s="122"/>
+      <c r="J32" s="122"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
+      <c r="M32" s="122"/>
+      <c r="N32" s="122"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" t="s">
+        <v>277</v>
+      </c>
+      <c r="C33">
+        <v>188</v>
+      </c>
+      <c r="F33" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="F34" s="59"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="F35" s="59"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="F37" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="C38">
+        <f>C33</f>
+        <v>188</v>
+      </c>
+      <c r="F38" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="Q19:U19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
+    <hyperlink ref="B1" tooltip="Name" display="Name"/>
+    <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
+    <hyperlink ref="F1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="G1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="H1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="I1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="J1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="K1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="L1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="M1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="N1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="mur-java-lib-httpclient"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="svb-scheduler-payments"/>
+    <hyperlink ref="B6" r:id="rId5" tooltip="mur-java-lib-auth"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="svb-service-accounts"/>
+    <hyperlink ref="B8" r:id="rId7" tooltip="svb-service-csrf"/>
+    <hyperlink ref="B9" r:id="rId8" tooltip="mur-java-lib-dbconnector"/>
+    <hyperlink ref="B10" r:id="rId9" tooltip="svb-service-client"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="mur-java-lib-logger"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="mur-java-lib-monitoring"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="svb-service-ooba"/>
+    <hyperlink ref="B14" r:id="rId13" tooltip="mur-java-lib-exception"/>
+    <hyperlink ref="B15" r:id="rId14" tooltip="mur-java-lib-mappers"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="svb-web-core-ui"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="svb-web-payment"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="T29:U29" emptyCellReference="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -31465,20 +32662,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="142" t="s">
+      <c r="A15" s="144" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="142"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="142"/>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="142"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="142"/>
-      <c r="J15" s="142"/>
-      <c r="K15" s="142"/>
-      <c r="L15" s="142"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="144"/>
+      <c r="F15" s="144"/>
+      <c r="G15" s="144"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="144"/>
+      <c r="J15" s="144"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="144"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -31683,18 +32880,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="142"/>
-      <c r="B40" s="142"/>
-      <c r="C40" s="142"/>
-      <c r="D40" s="142"/>
-      <c r="E40" s="142"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="142"/>
-      <c r="H40" s="142"/>
-      <c r="I40" s="142"/>
-      <c r="J40" s="142"/>
-      <c r="K40" s="142"/>
-      <c r="L40" s="142"/>
+      <c r="A40" s="144"/>
+      <c r="B40" s="144"/>
+      <c r="C40" s="144"/>
+      <c r="D40" s="144"/>
+      <c r="E40" s="144"/>
+      <c r="F40" s="144"/>
+      <c r="G40" s="144"/>
+      <c r="H40" s="144"/>
+      <c r="I40" s="144"/>
+      <c r="J40" s="144"/>
+      <c r="K40" s="144"/>
+      <c r="L40" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -32328,20 +33525,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -32945,20 +34142,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -33568,20 +34765,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -33803,13 +35000,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="143" t="s">
+      <c r="U4" s="145" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="145"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="147"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -33846,9 +35043,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="146"/>
-      <c r="V5" s="147"/>
-      <c r="W5" s="147"/>
+      <c r="U5" s="148"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -34438,20 +35635,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -35232,20 +36429,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="144" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="142"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="142"/>
-      <c r="J16" s="142"/>
-      <c r="K16" s="142"/>
-      <c r="L16" s="142"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
+      <c r="K16" s="144"/>
+      <c r="L16" s="144"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
10/12/16 Dot files Completed the repo Integrate count Func, etc.
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13960" tabRatio="650" firstSheet="15" activeTab="24"/>
+    <workbookView xWindow="30080" yWindow="680" windowWidth="29520" windowHeight="16900" tabRatio="817" firstSheet="11" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -28,16 +28,18 @@
     <sheet name="6.24" sheetId="30" r:id="rId19"/>
     <sheet name="7.1" sheetId="31" r:id="rId20"/>
     <sheet name="Layout Chg" sheetId="33" r:id="rId21"/>
-    <sheet name="July 8" sheetId="34" r:id="rId22"/>
-    <sheet name="July 15" sheetId="35" r:id="rId23"/>
+    <sheet name="7.8" sheetId="34" r:id="rId22"/>
+    <sheet name="7.15" sheetId="35" r:id="rId23"/>
     <sheet name="Unit&amp;Integration" sheetId="36" r:id="rId24"/>
     <sheet name="7.25" sheetId="37" r:id="rId25"/>
     <sheet name="humm" sheetId="38" r:id="rId26"/>
     <sheet name="8.19" sheetId="39" r:id="rId27"/>
     <sheet name="9.20" sheetId="41" r:id="rId28"/>
     <sheet name="10.3" sheetId="42" r:id="rId29"/>
+    <sheet name="10.12" sheetId="43" r:id="rId30"/>
   </sheets>
   <definedNames>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="29">'10.12'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
@@ -52,12 +54,12 @@
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="17">'6.17'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="18">'6.24'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="19">'7.1'!$A$1:$L$16</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="22">'7.15'!$A$1:$L$17</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="24">'7.25'!$A$1:$M$16</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="21">'7.8'!$A$1:$L$15</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="26">'8.19'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="27">'9.20'!$A$1:$L$17</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="25">humm!$A$1:$L$16</definedName>
-    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="22">'July 15'!$A$1:$L$17</definedName>
-    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="21">'July 8'!$A$1:$L$15</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="20">'Layout Chg'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="5">'S4'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="6">'S7'!$A$1:$L$16</definedName>
@@ -158,29 +160,35 @@
   <connection id="27" name="Connection32" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="28" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="28" name="Connection33" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="29" name="Connection34" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="30" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/index/12800?metric=tests/profiles/changelog?key=xml-murano-services-xml-profile-81269&amp;since=2015-09-02T19%3A11%3A38%2B0000&amp;to=2016-01-14T22%3A14%3A37%2B0000" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="29" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="31" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="30" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="32" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="31" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="33" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="32" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="34" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="33" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="35" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-mjenk01.dev.svbank.com:8080/job/T2%20web-payment-test-master/lastBuild/consoleText" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="351">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1189,6 +1197,53 @@
   <si>
     <t>Oct 3, 2016</t>
   </si>
+  <si>
+    <t>Mur Service BankInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2d 2h </t>
+  </si>
+  <si>
+    <t>20 results</t>
+  </si>
+  <si>
+    <t>Protractor E2E Integration tests</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Column E "int" represents repository count of integration or component level tests</t>
+  </si>
+  <si>
+    <t>These tests are all writtin Java and run against *.jars hosted on the GlassFish/Jersey/Grizzly2 web app test environment</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>There should be a change of the repo names so that they are all Mur Service &lt;function/feature&gt;  vs mur client service and one other</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>Application Front End</t>
+  </si>
+  <si>
+    <t>Manual
+Releases</t>
+  </si>
+  <si>
+    <t>Test Cases
+Count</t>
+  </si>
+  <si>
+    <t>Oct 12 2016</t>
+  </si>
 </sst>
 </file>
 
@@ -1819,7 +1874,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2102,6 +2157,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2125,16 +2193,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="12" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2389,8 +2450,12 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+</file>
+
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8479,13 +8544,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8522,9 +8587,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9106,20 +9171,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9582,13 +9647,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9625,9 +9690,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10209,20 +10274,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10417,13 +10482,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="145" t="s">
+      <c r="U25" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="146"/>
-      <c r="W25" s="146"/>
-      <c r="X25" s="146"/>
-      <c r="Y25" s="147"/>
+      <c r="V25" s="153"/>
+      <c r="W25" s="153"/>
+      <c r="X25" s="153"/>
+      <c r="Y25" s="154"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10436,9 +10501,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="148"/>
-      <c r="V26" s="149"/>
-      <c r="W26" s="149"/>
+      <c r="U26" s="155"/>
+      <c r="V26" s="156"/>
+      <c r="W26" s="156"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10832,13 +10897,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -10875,9 +10940,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11467,20 +11532,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12003,13 +12068,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -12046,9 +12111,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12649,20 +12714,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13207,13 +13272,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13250,9 +13315,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -13863,20 +13928,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14413,13 +14478,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14456,9 +14521,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15069,20 +15134,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15619,13 +15684,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15662,9 +15727,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16275,20 +16340,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16825,13 +16890,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -16868,9 +16933,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17481,20 +17546,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18034,13 +18099,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18077,9 +18142,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18693,20 +18758,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19183,13 +19248,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19226,9 +19291,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19842,20 +19907,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -20997,13 +21062,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -21040,9 +21105,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21656,20 +21721,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21974,7 +22039,7 @@
   <dimension ref="A1:Y34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -22759,20 +22824,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -23855,20 +23920,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="151" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="144"/>
-      <c r="F15" s="144"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="144"/>
-      <c r="K15" s="144"/>
-      <c r="L15" s="144"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -24200,7 +24265,7 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -25849,21 +25914,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
-      <c r="M16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -25909,8 +25974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="Q23" sqref="O23:Q23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -26727,21 +26792,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
-      <c r="M16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="151"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27622,20 +27687,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -29074,20 +29139,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -29384,7 +29449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
@@ -30121,20 +30186,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="151" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="144"/>
-      <c r="C17" s="144"/>
-      <c r="D17" s="144"/>
-      <c r="E17" s="144"/>
-      <c r="F17" s="144"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
-      <c r="K17" s="144"/>
-      <c r="L17" s="144"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="151"/>
+      <c r="D17" s="151"/>
+      <c r="E17" s="151"/>
+      <c r="F17" s="151"/>
+      <c r="G17" s="151"/>
+      <c r="H17" s="151"/>
+      <c r="I17" s="151"/>
+      <c r="J17" s="151"/>
+      <c r="K17" s="151"/>
+      <c r="L17" s="151"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30145,13 +30210,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="150" t="s">
+      <c r="O19" s="157" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="151"/>
-      <c r="Q19" s="151"/>
-      <c r="R19" s="151"/>
-      <c r="S19" s="152"/>
+      <c r="P19" s="158"/>
+      <c r="Q19" s="158"/>
+      <c r="R19" s="158"/>
+      <c r="S19" s="159"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -30421,8 +30486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18:U30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -30515,7 +30580,9 @@
         <v>581</v>
       </c>
       <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
+      <c r="E2" s="143">
+        <v>123</v>
+      </c>
       <c r="F2" s="23">
         <v>6209</v>
       </c>
@@ -30557,7 +30624,9 @@
         <v>194</v>
       </c>
       <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
+      <c r="E3" s="143">
+        <v>34</v>
+      </c>
       <c r="F3" s="23">
         <v>1760</v>
       </c>
@@ -31237,34 +31306,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="144" t="s">
+      <c r="A18" s="151" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="144"/>
-      <c r="C18" s="144"/>
-      <c r="D18" s="144"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
-      <c r="K18" s="144"/>
-      <c r="L18" s="144"/>
-      <c r="M18" s="144"/>
-      <c r="N18" s="144"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="151"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="151"/>
+      <c r="K18" s="151"/>
+      <c r="L18" s="151"/>
+      <c r="M18" s="151"/>
+      <c r="N18" s="151"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="150" t="s">
+      <c r="Q19" s="157" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="151"/>
-      <c r="S19" s="151"/>
-      <c r="T19" s="151"/>
-      <c r="U19" s="152"/>
+      <c r="R19" s="158"/>
+      <c r="S19" s="158"/>
+      <c r="T19" s="158"/>
+      <c r="U19" s="159"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -31273,10 +31342,10 @@
       <c r="Q20" s="124"/>
       <c r="R20" s="125"/>
       <c r="S20" s="125"/>
-      <c r="T20" s="153" t="s">
+      <c r="T20" s="144" t="s">
         <v>165</v>
       </c>
-      <c r="U20" s="154" t="s">
+      <c r="U20" s="145" t="s">
         <v>335</v>
       </c>
     </row>
@@ -31287,7 +31356,7 @@
       <c r="T21" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="U21" s="155"/>
+      <c r="U21" s="146"/>
     </row>
     <row r="22" spans="1:21">
       <c r="B22" t="s">
@@ -31311,7 +31380,7 @@
         <f>S1</f>
         <v>223</v>
       </c>
-      <c r="U22" s="156">
+      <c r="U22" s="147">
         <f>T22/$T$29</f>
         <v>9.1281211625051165E-2</v>
       </c>
@@ -31333,8 +31402,8 @@
         <f>C38</f>
         <v>188</v>
       </c>
-      <c r="U23" s="156">
-        <f t="shared" ref="U23:U28" si="1">T23/$T$29</f>
+      <c r="U23" s="147">
+        <f t="shared" ref="U23:U27" si="1">T23/$T$29</f>
         <v>7.6954564060581251E-2</v>
       </c>
     </row>
@@ -31359,7 +31428,7 @@
       <c r="T24" s="135">
         <v>0</v>
       </c>
-      <c r="U24" s="156"/>
+      <c r="U24" s="147"/>
     </row>
     <row r="25" spans="1:21">
       <c r="F25" s="58"/>
@@ -31374,7 +31443,7 @@
         <f>U14</f>
         <v>1450</v>
       </c>
-      <c r="U25" s="156">
+      <c r="U25" s="147">
         <f t="shared" si="1"/>
         <v>0.59353254195661076</v>
       </c>
@@ -31393,8 +31462,8 @@
       <c r="S26" s="134" t="s">
         <v>170</v>
       </c>
-      <c r="T26" s="158"/>
-      <c r="U26" s="156"/>
+      <c r="T26" s="149"/>
+      <c r="U26" s="147"/>
     </row>
     <row r="27" spans="1:21">
       <c r="C27" t="s">
@@ -31409,7 +31478,7 @@
         <f>U16</f>
         <v>582</v>
       </c>
-      <c r="U27" s="156">
+      <c r="U27" s="147">
         <f t="shared" si="1"/>
         <v>0.23823168235775685</v>
       </c>
@@ -31422,7 +31491,7 @@
       <c r="R28" s="133"/>
       <c r="S28" s="134"/>
       <c r="T28" s="135"/>
-      <c r="U28" s="156"/>
+      <c r="U28" s="147"/>
     </row>
     <row r="29" spans="1:21" ht="15" thickBot="1">
       <c r="C29" t="s">
@@ -31435,7 +31504,7 @@
         <f>SUM(T22:T27)</f>
         <v>2443</v>
       </c>
-      <c r="U29" s="157">
+      <c r="U29" s="148">
         <f>SUM(U22:U28)</f>
         <v>1</v>
       </c>
@@ -32139,6 +32208,1680 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U172"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="45">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="160" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" s="160" t="s">
+        <v>349</v>
+      </c>
+      <c r="S1" s="59" t="str">
+        <f>C1</f>
+        <v xml:space="preserve">UTs </v>
+      </c>
+      <c r="T1" s="59" t="str">
+        <f>E1</f>
+        <v>Int</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="150">
+        <v>581</v>
+      </c>
+      <c r="D2" s="150"/>
+      <c r="E2" s="150">
+        <v>123</v>
+      </c>
+      <c r="F2" s="23">
+        <v>6215</v>
+      </c>
+      <c r="G2" s="150" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="26">
+        <v>0.56319444444444444</v>
+      </c>
+      <c r="I2" s="25">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="J2" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K2" s="150">
+        <v>0</v>
+      </c>
+      <c r="L2" s="150">
+        <v>0</v>
+      </c>
+      <c r="M2" s="150">
+        <v>2</v>
+      </c>
+      <c r="N2" s="150">
+        <v>0</v>
+      </c>
+      <c r="S2" s="59">
+        <f>C2-E2</f>
+        <v>458</v>
+      </c>
+      <c r="T2" s="59">
+        <f t="shared" ref="T2:T18" si="0">E2</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="150">
+        <v>194</v>
+      </c>
+      <c r="D3" s="150"/>
+      <c r="E3" s="150">
+        <v>34</v>
+      </c>
+      <c r="F3" s="23">
+        <v>1760</v>
+      </c>
+      <c r="G3" s="150" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="26">
+        <v>0.54097222222222219</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J3" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K3" s="150">
+        <v>0</v>
+      </c>
+      <c r="L3" s="150">
+        <v>0</v>
+      </c>
+      <c r="M3" s="150">
+        <v>2</v>
+      </c>
+      <c r="N3" s="150">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>265</v>
+      </c>
+      <c r="R3">
+        <v>13</v>
+      </c>
+      <c r="S3" s="59">
+        <f t="shared" ref="S3:S18" si="1">C3-E3</f>
+        <v>160</v>
+      </c>
+      <c r="T3" s="59">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="150">
+        <v>132</v>
+      </c>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150">
+        <v>871</v>
+      </c>
+      <c r="G4" s="150" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0.95</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K4" s="150">
+        <v>0</v>
+      </c>
+      <c r="L4" s="150">
+        <v>0</v>
+      </c>
+      <c r="M4" s="150">
+        <v>1</v>
+      </c>
+      <c r="N4" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>258</v>
+      </c>
+      <c r="R4">
+        <v>153</v>
+      </c>
+      <c r="S4" s="59">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="T4" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="150">
+        <v>114</v>
+      </c>
+      <c r="D5" s="150"/>
+      <c r="E5" s="150"/>
+      <c r="F5" s="23">
+        <v>1611</v>
+      </c>
+      <c r="G5" s="150" t="s">
+        <v>255</v>
+      </c>
+      <c r="H5" s="24">
+        <v>42649</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="K5" s="150">
+        <v>0</v>
+      </c>
+      <c r="L5" s="150">
+        <v>0</v>
+      </c>
+      <c r="M5" s="150">
+        <v>0</v>
+      </c>
+      <c r="N5" s="150">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>259</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="59">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="T5" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="150">
+        <v>76</v>
+      </c>
+      <c r="D6" s="150"/>
+      <c r="E6" s="150"/>
+      <c r="F6" s="150">
+        <v>563</v>
+      </c>
+      <c r="G6" s="150" t="s">
+        <v>248</v>
+      </c>
+      <c r="H6" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="K6" s="150">
+        <v>0</v>
+      </c>
+      <c r="L6" s="150">
+        <v>0</v>
+      </c>
+      <c r="M6" s="150">
+        <v>1</v>
+      </c>
+      <c r="N6" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" s="59">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+      <c r="T6" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
+      <c r="A7" s="20"/>
+      <c r="B7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="150">
+        <v>69</v>
+      </c>
+      <c r="D7" s="150"/>
+      <c r="E7" s="150">
+        <v>16</v>
+      </c>
+      <c r="F7" s="150">
+        <v>839</v>
+      </c>
+      <c r="G7" s="150" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" s="24">
+        <v>42646</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="J7" s="25">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="K7" s="150">
+        <v>0</v>
+      </c>
+      <c r="L7" s="150">
+        <v>0</v>
+      </c>
+      <c r="M7" s="150">
+        <v>2</v>
+      </c>
+      <c r="N7" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>268</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7" s="59">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="T7" s="59">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="150">
+        <v>61</v>
+      </c>
+      <c r="D8" s="150"/>
+      <c r="E8" s="150">
+        <v>11</v>
+      </c>
+      <c r="F8" s="150">
+        <v>693</v>
+      </c>
+      <c r="G8" s="150" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="24">
+        <v>42646</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="J8" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="K8" s="150">
+        <v>0</v>
+      </c>
+      <c r="L8" s="150">
+        <v>0</v>
+      </c>
+      <c r="M8" s="150">
+        <v>0</v>
+      </c>
+      <c r="N8" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R8">
+        <v>27</v>
+      </c>
+      <c r="S8" s="59">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="T8" s="59">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="150">
+        <v>59</v>
+      </c>
+      <c r="D9" s="150"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="150">
+        <v>344</v>
+      </c>
+      <c r="G9" s="150">
+        <v>0</v>
+      </c>
+      <c r="H9" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J9" s="25">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="K9" s="150">
+        <v>0</v>
+      </c>
+      <c r="L9" s="150">
+        <v>0</v>
+      </c>
+      <c r="M9" s="150">
+        <v>0</v>
+      </c>
+      <c r="N9" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>263</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9" s="59">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="T9" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" s="150">
+        <v>44</v>
+      </c>
+      <c r="D10" s="150"/>
+      <c r="E10" s="150">
+        <v>5</v>
+      </c>
+      <c r="F10" s="150">
+        <v>573</v>
+      </c>
+      <c r="G10" s="150" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" s="26">
+        <v>0.46875</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="K10" s="150">
+        <v>0</v>
+      </c>
+      <c r="L10" s="150">
+        <v>0</v>
+      </c>
+      <c r="M10" s="150">
+        <v>1</v>
+      </c>
+      <c r="N10" s="150">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>264</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="59">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="T10" s="59">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="150">
+        <v>36</v>
+      </c>
+      <c r="D11" s="150"/>
+      <c r="E11" s="150"/>
+      <c r="F11" s="150">
+        <v>195</v>
+      </c>
+      <c r="G11" s="150">
+        <v>0</v>
+      </c>
+      <c r="H11" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J11" s="25">
+        <v>1</v>
+      </c>
+      <c r="K11" s="150">
+        <v>0</v>
+      </c>
+      <c r="L11" s="150">
+        <v>0</v>
+      </c>
+      <c r="M11" s="150">
+        <v>0</v>
+      </c>
+      <c r="N11" s="150">
+        <v>0</v>
+      </c>
+      <c r="S11" s="59">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="T11" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="150">
+        <v>31</v>
+      </c>
+      <c r="D12" s="150"/>
+      <c r="E12" s="150"/>
+      <c r="F12" s="150">
+        <v>378</v>
+      </c>
+      <c r="G12" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K12" s="150">
+        <v>0</v>
+      </c>
+      <c r="L12" s="150">
+        <v>0</v>
+      </c>
+      <c r="M12" s="150">
+        <v>1</v>
+      </c>
+      <c r="N12" s="150">
+        <v>0</v>
+      </c>
+      <c r="S12" s="59">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="T12" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" s="150">
+        <v>22</v>
+      </c>
+      <c r="D13" s="150"/>
+      <c r="E13" s="150"/>
+      <c r="F13" s="150">
+        <v>318</v>
+      </c>
+      <c r="G13" s="150" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="J13" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="K13" s="150">
+        <v>0</v>
+      </c>
+      <c r="L13" s="150">
+        <v>0</v>
+      </c>
+      <c r="M13" s="150">
+        <v>1</v>
+      </c>
+      <c r="N13" s="150">
+        <v>2</v>
+      </c>
+      <c r="S13" s="59">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="T13" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" s="150">
+        <v>22</v>
+      </c>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150">
+        <v>8</v>
+      </c>
+      <c r="F14" s="150">
+        <v>319</v>
+      </c>
+      <c r="G14" s="150" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="24">
+        <v>42654</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="150">
+        <v>0</v>
+      </c>
+      <c r="L14" s="150">
+        <v>0</v>
+      </c>
+      <c r="M14" s="150">
+        <v>1</v>
+      </c>
+      <c r="N14" s="150">
+        <v>0</v>
+      </c>
+      <c r="S14" s="59">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="T14" s="59">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="U14">
+        <f>SUM(S2:S16)</f>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="150">
+        <v>18</v>
+      </c>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150">
+        <v>172</v>
+      </c>
+      <c r="G15" s="150">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="K15" s="150">
+        <v>0</v>
+      </c>
+      <c r="L15" s="150">
+        <v>0</v>
+      </c>
+      <c r="M15" s="150">
+        <v>0</v>
+      </c>
+      <c r="N15" s="150">
+        <v>0</v>
+      </c>
+      <c r="S15" s="59">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T15" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>SUM(T2:T18)</f>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="150">
+        <v>13</v>
+      </c>
+      <c r="D16" s="150"/>
+      <c r="E16" s="150"/>
+      <c r="F16" s="150">
+        <v>218</v>
+      </c>
+      <c r="G16" s="150">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
+        <v>42647</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K16" s="150">
+        <v>0</v>
+      </c>
+      <c r="L16" s="150">
+        <v>0</v>
+      </c>
+      <c r="M16" s="150">
+        <v>0</v>
+      </c>
+      <c r="N16" s="150">
+        <v>0</v>
+      </c>
+      <c r="S16" s="59">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="T16" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>SUM(S17:S18)</f>
+        <v>582</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="31">
+        <v>91</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="23">
+        <v>3041</v>
+      </c>
+      <c r="G17" s="150">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>42578</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K17" s="150">
+        <v>0</v>
+      </c>
+      <c r="L17" s="150">
+        <v>0</v>
+      </c>
+      <c r="M17" s="150">
+        <v>0</v>
+      </c>
+      <c r="N17" s="150">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>SUM(R3:R10)</f>
+        <v>217</v>
+      </c>
+      <c r="S17" s="59">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="T17" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="18" customHeight="1">
+      <c r="A18" s="19"/>
+      <c r="B18" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="31">
+        <v>491</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="23">
+        <v>10132</v>
+      </c>
+      <c r="G18" s="150" t="s">
+        <v>337</v>
+      </c>
+      <c r="H18" s="24">
+        <v>42607</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="J18" s="25">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="K18" s="150">
+        <v>0</v>
+      </c>
+      <c r="L18" s="150">
+        <v>0</v>
+      </c>
+      <c r="M18" s="150">
+        <v>19</v>
+      </c>
+      <c r="N18" s="150">
+        <v>104</v>
+      </c>
+      <c r="S18" s="59">
+        <f t="shared" si="1"/>
+        <v>491</v>
+      </c>
+      <c r="T18" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="150" t="s">
+        <v>338</v>
+      </c>
+      <c r="B19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="150"/>
+      <c r="H19" s="150"/>
+      <c r="I19" s="150"/>
+      <c r="J19" s="150"/>
+      <c r="K19" s="150"/>
+      <c r="L19" s="150"/>
+      <c r="M19" s="150"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="B20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" thickBot="1">
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" thickBot="1">
+      <c r="Q22" s="157" t="s">
+        <v>164</v>
+      </c>
+      <c r="R22" s="158"/>
+      <c r="S22" s="158"/>
+      <c r="T22" s="158"/>
+      <c r="U22" s="159"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>91</v>
+      </c>
+      <c r="F23" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G23" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q23" s="124"/>
+      <c r="R23" s="125"/>
+      <c r="S23" s="125"/>
+      <c r="T23" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="U23" s="145" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="F24" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="129"/>
+      <c r="S24" s="129"/>
+      <c r="T24" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="146"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25">
+        <v>491</v>
+      </c>
+      <c r="F25" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q25" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="133"/>
+      <c r="S25" s="134"/>
+      <c r="T25" s="135">
+        <f>R17</f>
+        <v>217</v>
+      </c>
+      <c r="U25" s="147">
+        <f>T25/$T$32</f>
+        <v>8.8247254981699871E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="F26" s="58"/>
+      <c r="Q26" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="R26" s="133" t="s">
+        <v>333</v>
+      </c>
+      <c r="S26" s="134" t="s">
+        <v>334</v>
+      </c>
+      <c r="T26" s="135">
+        <f>C34</f>
+        <v>188</v>
+      </c>
+      <c r="U26" s="147">
+        <f t="shared" ref="U26:U30" si="2">T26/$T$32</f>
+        <v>7.6453843025620166E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="B27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q27" s="132"/>
+      <c r="R27" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="S27" s="134"/>
+      <c r="T27" s="135">
+        <v>0</v>
+      </c>
+      <c r="U27" s="147"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="C28" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q28" s="132"/>
+      <c r="R28" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="S28" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T28" s="135">
+        <f>U14</f>
+        <v>1275</v>
+      </c>
+      <c r="U28" s="147">
+        <f t="shared" si="2"/>
+        <v>0.51850345668971132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="C29" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q29" s="132"/>
+      <c r="R29" s="133" t="s">
+        <v>331</v>
+      </c>
+      <c r="S29" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T29" s="135">
+        <f>U15</f>
+        <v>197</v>
+      </c>
+      <c r="U29" s="147">
+        <f t="shared" si="2"/>
+        <v>8.0113867425782845E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="C30" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q30" s="132"/>
+      <c r="R30" s="133"/>
+      <c r="S30" s="134" t="s">
+        <v>347</v>
+      </c>
+      <c r="T30" s="135">
+        <f>U16</f>
+        <v>582</v>
+      </c>
+      <c r="U30" s="147">
+        <f t="shared" si="2"/>
+        <v>0.23668157787718586</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q31" s="132"/>
+      <c r="R31" s="133"/>
+      <c r="S31" s="134"/>
+      <c r="T31" s="135"/>
+      <c r="U31" s="147"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" thickBot="1">
+      <c r="Q32" s="137"/>
+      <c r="R32" s="138"/>
+      <c r="S32" s="139"/>
+      <c r="T32" s="140">
+        <f>SUM(T25:T30)</f>
+        <v>2459</v>
+      </c>
+      <c r="U32" s="148">
+        <f>SUM(U25:U31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="B33" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="123" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="122"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="B34" t="s">
+        <v>339</v>
+      </c>
+      <c r="C34">
+        <v>188</v>
+      </c>
+      <c r="F34" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="62" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B37" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="62"/>
+      <c r="B38" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="62" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="62" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="62"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="62"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="62"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="62"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="62"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="62"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="62"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="62"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="62"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="62"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="62"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="62"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="62"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="62"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="62"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="62"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="62"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="62"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="62"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="62"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="62"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="62"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="62"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="62"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="62"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="62"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="62"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="62"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="62"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="62"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="62"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="62"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="62"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="62"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="62"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="62"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="62"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="62"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="62"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="62"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="62"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="62"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="62"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="62"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="62"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="62"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="62"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="62"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="62"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="62"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="62"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="62"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="62"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="62"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="62"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="62"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="62"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="62"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="62"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="62"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="62"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="62"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="62"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="62"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="62"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="62"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="62"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="62"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="62"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="62"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="62"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="62"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="62"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="62"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="62"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="62"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="62"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="62"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="62"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="62"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="62"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="62"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="62"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="62"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="62"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="62"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="62"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="62"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="62"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="62"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="62"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="62"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="62"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="62"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="62"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="62"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="62"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="62"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="62"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="62"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="62"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="62"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="62"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="62"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="62"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="62"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="62"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="62"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="62"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="62"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="62"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="62"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="62"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="62"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="62"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="62"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="62"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="62"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="62"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="62"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="62"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="62"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="62"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="62"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="62"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="62"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="62"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="62"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="62"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="62"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="62"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Q22:U22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
+    <hyperlink ref="B1" tooltip="Name" display="Name"/>
+    <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
+    <hyperlink ref="F1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="G1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="H1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="I1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="J1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="K1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="L1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="M1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="N1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="mur-java-lib-httpclient"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="svb-scheduler-payments"/>
+    <hyperlink ref="B6" r:id="rId5" tooltip="mur-java-lib-auth"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="svb-service-accounts"/>
+    <hyperlink ref="B8" r:id="rId7" tooltip="svb-service-csrf"/>
+    <hyperlink ref="B9" r:id="rId8" tooltip="mur-java-lib-dbconnector"/>
+    <hyperlink ref="B10" r:id="rId9" tooltip="svb-service-client"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="mur-java-lib-logger"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="mur-java-lib-monitoring"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="svb-service-ooba"/>
+    <hyperlink ref="B14" r:id="rId13" tooltip="svb-service-bankinfo"/>
+    <hyperlink ref="B15" r:id="rId14" tooltip="mur-java-lib-exception"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="mur-java-lib-mappers"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="svb-web-core-ui"/>
+    <hyperlink ref="B18" r:id="rId17" tooltip="svb-web-payment:master" display="Mur Web Payment master"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="U32" emptyCellReference="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
@@ -32662,20 +34405,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="151" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="144"/>
-      <c r="C15" s="144"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="144"/>
-      <c r="F15" s="144"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="144"/>
-      <c r="K15" s="144"/>
-      <c r="L15" s="144"/>
+      <c r="B15" s="151"/>
+      <c r="C15" s="151"/>
+      <c r="D15" s="151"/>
+      <c r="E15" s="151"/>
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="151"/>
+      <c r="L15" s="151"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -32880,18 +34623,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="144"/>
-      <c r="B40" s="144"/>
-      <c r="C40" s="144"/>
-      <c r="D40" s="144"/>
-      <c r="E40" s="144"/>
-      <c r="F40" s="144"/>
-      <c r="G40" s="144"/>
-      <c r="H40" s="144"/>
-      <c r="I40" s="144"/>
-      <c r="J40" s="144"/>
-      <c r="K40" s="144"/>
-      <c r="L40" s="144"/>
+      <c r="A40" s="151"/>
+      <c r="B40" s="151"/>
+      <c r="C40" s="151"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="151"/>
+      <c r="F40" s="151"/>
+      <c r="G40" s="151"/>
+      <c r="H40" s="151"/>
+      <c r="I40" s="151"/>
+      <c r="J40" s="151"/>
+      <c r="K40" s="151"/>
+      <c r="L40" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -33525,20 +35268,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -34142,20 +35885,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -34765,20 +36508,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -35000,13 +36743,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="145" t="s">
+      <c r="U4" s="152" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="147"/>
+      <c r="V4" s="153"/>
+      <c r="W4" s="153"/>
+      <c r="X4" s="153"/>
+      <c r="Y4" s="154"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -35043,9 +36786,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="148"/>
-      <c r="V5" s="149"/>
-      <c r="W5" s="149"/>
+      <c r="U5" s="155"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -35635,20 +37378,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -36429,20 +38172,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="144" t="s">
+      <c r="A16" s="151" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="144"/>
-      <c r="C16" s="144"/>
-      <c r="D16" s="144"/>
-      <c r="E16" s="144"/>
-      <c r="F16" s="144"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
-      <c r="K16" s="144"/>
-      <c r="L16" s="144"/>
+      <c r="B16" s="151"/>
+      <c r="C16" s="151"/>
+      <c r="D16" s="151"/>
+      <c r="E16" s="151"/>
+      <c r="F16" s="151"/>
+      <c r="G16" s="151"/>
+      <c r="H16" s="151"/>
+      <c r="I16" s="151"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151"/>
+      <c r="L16" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
10/20/16 dots, Exce files
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="120" windowWidth="28420" windowHeight="17420" tabRatio="817" firstSheet="21" activeTab="30"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17060" windowHeight="16880" tabRatio="559" firstSheet="27" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2444" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="355">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1258,6 +1258,9 @@
   <si>
     <t>Oct 18 2016</t>
   </si>
+  <si>
+    <t>B34  Prot E2E Integration test is both ../integration/mock &amp; ../integration/scenarios</t>
+  </si>
 </sst>
 </file>
 
@@ -2193,6 +2196,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2215,9 +2221,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="76">
@@ -2396,7 +2399,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2440,7 +2443,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8573,13 +8576,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8616,9 +8619,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9200,20 +9203,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9676,13 +9679,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9719,9 +9722,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10303,20 +10306,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10511,13 +10514,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="154" t="s">
+      <c r="U25" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="155"/>
-      <c r="W25" s="155"/>
-      <c r="X25" s="155"/>
-      <c r="Y25" s="156"/>
+      <c r="V25" s="156"/>
+      <c r="W25" s="156"/>
+      <c r="X25" s="156"/>
+      <c r="Y25" s="157"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10530,9 +10533,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="157"/>
-      <c r="V26" s="158"/>
-      <c r="W26" s="158"/>
+      <c r="U26" s="158"/>
+      <c r="V26" s="159"/>
+      <c r="W26" s="159"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10926,13 +10929,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -10969,9 +10972,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11561,20 +11564,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12097,13 +12100,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -12140,9 +12143,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12743,20 +12746,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13301,13 +13304,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13344,9 +13347,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -13957,20 +13960,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14507,13 +14510,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14550,9 +14553,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15163,20 +15166,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15713,13 +15716,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15756,9 +15759,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16369,20 +16372,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16919,13 +16922,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -16962,9 +16965,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17575,20 +17578,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18128,13 +18131,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18171,9 +18174,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18787,20 +18790,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19277,13 +19280,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19320,9 +19323,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19936,20 +19939,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21091,13 +21094,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -21134,9 +21137,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21750,20 +21753,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -22853,20 +22856,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -23949,20 +23952,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="153" t="s">
+      <c r="A15" s="154" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="153"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
-      <c r="L15" s="153"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="154"/>
+      <c r="D15" s="154"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="154"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="154"/>
+      <c r="L15" s="154"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -25943,21 +25946,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
-      <c r="M16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
+      <c r="M16" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -26821,21 +26824,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
-      <c r="M16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
+      <c r="M16" s="154"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27716,20 +27719,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -29168,20 +29171,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -29478,8 +29481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -30215,20 +30218,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="153" t="s">
+      <c r="A17" s="154" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="153"/>
-      <c r="C17" s="153"/>
-      <c r="D17" s="153"/>
-      <c r="E17" s="153"/>
-      <c r="F17" s="153"/>
-      <c r="G17" s="153"/>
-      <c r="H17" s="153"/>
-      <c r="I17" s="153"/>
-      <c r="J17" s="153"/>
-      <c r="K17" s="153"/>
-      <c r="L17" s="153"/>
+      <c r="B17" s="154"/>
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="154"/>
+      <c r="F17" s="154"/>
+      <c r="G17" s="154"/>
+      <c r="H17" s="154"/>
+      <c r="I17" s="154"/>
+      <c r="J17" s="154"/>
+      <c r="K17" s="154"/>
+      <c r="L17" s="154"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30239,13 +30242,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="159" t="s">
+      <c r="O19" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="160"/>
-      <c r="Q19" s="160"/>
-      <c r="R19" s="160"/>
-      <c r="S19" s="161"/>
+      <c r="P19" s="161"/>
+      <c r="Q19" s="161"/>
+      <c r="R19" s="161"/>
+      <c r="S19" s="162"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -31335,34 +31338,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="153" t="s">
+      <c r="A18" s="154" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="153"/>
-      <c r="C18" s="153"/>
-      <c r="D18" s="153"/>
-      <c r="E18" s="153"/>
-      <c r="F18" s="153"/>
-      <c r="G18" s="153"/>
-      <c r="H18" s="153"/>
-      <c r="I18" s="153"/>
-      <c r="J18" s="153"/>
-      <c r="K18" s="153"/>
-      <c r="L18" s="153"/>
-      <c r="M18" s="153"/>
-      <c r="N18" s="153"/>
+      <c r="B18" s="154"/>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="154"/>
+      <c r="F18" s="154"/>
+      <c r="G18" s="154"/>
+      <c r="H18" s="154"/>
+      <c r="I18" s="154"/>
+      <c r="J18" s="154"/>
+      <c r="K18" s="154"/>
+      <c r="L18" s="154"/>
+      <c r="M18" s="154"/>
+      <c r="N18" s="154"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="159" t="s">
+      <c r="Q19" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="160"/>
-      <c r="S19" s="160"/>
-      <c r="T19" s="160"/>
-      <c r="U19" s="161"/>
+      <c r="R19" s="161"/>
+      <c r="S19" s="161"/>
+      <c r="T19" s="161"/>
+      <c r="U19" s="162"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -32242,7 +32245,7 @@
   <dimension ref="A1:U172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -32272,7 +32275,7 @@
       <c r="A1" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="162" t="s">
+      <c r="B1" s="153" t="s">
         <v>104</v>
       </c>
       <c r="C1" s="18" t="s">
@@ -33212,13 +33215,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="159" t="s">
+      <c r="Q22" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="160"/>
-      <c r="S22" s="160"/>
-      <c r="T22" s="160"/>
-      <c r="U22" s="161"/>
+      <c r="R22" s="161"/>
+      <c r="S22" s="161"/>
+      <c r="T22" s="161"/>
+      <c r="U22" s="162"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -33915,14 +33918,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="4.33203125" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
@@ -33939,7 +33942,7 @@
     <col min="18" max="18" width="17.1640625" customWidth="1"/>
     <col min="19" max="19" width="22.33203125" customWidth="1"/>
     <col min="20" max="20" width="19.1640625" customWidth="1"/>
-    <col min="21" max="21" width="12.5" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45">
@@ -34006,9 +34009,11 @@
       <c r="C2" s="151">
         <v>591</v>
       </c>
-      <c r="D2" s="151"/>
+      <c r="D2" s="151">
+        <v>608</v>
+      </c>
       <c r="E2" s="151">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F2" s="23">
         <v>6330</v>
@@ -34039,11 +34044,11 @@
       </c>
       <c r="S2" s="59">
         <f>C2-E2</f>
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="T2" s="59">
-        <f t="shared" ref="T2:T18" si="0">E2</f>
-        <v>123</v>
+        <f t="shared" ref="T2:T16" si="0">E2</f>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15">
@@ -34052,11 +34057,13 @@
         <v>117</v>
       </c>
       <c r="C3" s="151">
-        <v>194</v>
-      </c>
-      <c r="D3" s="151"/>
+        <v>210</v>
+      </c>
+      <c r="D3" s="151">
+        <v>239</v>
+      </c>
       <c r="E3" s="151">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F3" s="23">
         <v>1760</v>
@@ -34093,11 +34100,11 @@
       </c>
       <c r="S3" s="59">
         <f t="shared" ref="S3:S16" si="1">C3-E3</f>
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="T3" s="59">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15">
@@ -34106,10 +34113,14 @@
         <v>329</v>
       </c>
       <c r="C4" s="151">
-        <v>28</v>
-      </c>
-      <c r="D4" s="151"/>
-      <c r="E4" s="151"/>
+        <v>172</v>
+      </c>
+      <c r="D4" s="151">
+        <v>165</v>
+      </c>
+      <c r="E4" s="151">
+        <v>39</v>
+      </c>
       <c r="F4" s="23">
         <v>2230</v>
       </c>
@@ -34145,11 +34156,11 @@
       </c>
       <c r="S4" s="59">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="T4" s="59">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15">
@@ -34160,7 +34171,9 @@
       <c r="C5" s="151">
         <v>132</v>
       </c>
-      <c r="D5" s="151"/>
+      <c r="D5" s="151">
+        <v>134</v>
+      </c>
       <c r="E5" s="151"/>
       <c r="F5" s="151">
         <v>871</v>
@@ -34212,7 +34225,9 @@
       <c r="C6" s="151">
         <v>114</v>
       </c>
-      <c r="D6" s="151"/>
+      <c r="D6" s="151">
+        <v>115</v>
+      </c>
       <c r="E6" s="151"/>
       <c r="F6" s="23">
         <v>1607</v>
@@ -34264,7 +34279,9 @@
       <c r="C7" s="151">
         <v>82</v>
       </c>
-      <c r="D7" s="151"/>
+      <c r="D7" s="151">
+        <v>84</v>
+      </c>
       <c r="E7" s="151"/>
       <c r="F7" s="151">
         <v>677</v>
@@ -34316,7 +34333,9 @@
       <c r="C8" s="151">
         <v>69</v>
       </c>
-      <c r="D8" s="151"/>
+      <c r="D8" s="151">
+        <v>80</v>
+      </c>
       <c r="E8" s="151">
         <v>16</v>
       </c>
@@ -34370,7 +34389,9 @@
       <c r="C9" s="151">
         <v>61</v>
       </c>
-      <c r="D9" s="151"/>
+      <c r="D9" s="151">
+        <v>77</v>
+      </c>
       <c r="E9" s="151">
         <v>11</v>
       </c>
@@ -34424,7 +34445,9 @@
       <c r="C10" s="151">
         <v>59</v>
       </c>
-      <c r="D10" s="151"/>
+      <c r="D10" s="151">
+        <v>60</v>
+      </c>
       <c r="E10" s="151"/>
       <c r="F10" s="151">
         <v>344</v>
@@ -34476,7 +34499,9 @@
       <c r="C11" s="151">
         <v>44</v>
       </c>
-      <c r="D11" s="151"/>
+      <c r="D11" s="151">
+        <v>38</v>
+      </c>
       <c r="E11" s="151">
         <v>5</v>
       </c>
@@ -34524,9 +34549,11 @@
       <c r="C12" s="151">
         <v>41</v>
       </c>
-      <c r="D12" s="151"/>
+      <c r="D12" s="151">
+        <v>48</v>
+      </c>
       <c r="E12" s="151">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F12" s="151">
         <v>567</v>
@@ -34557,11 +34584,11 @@
       </c>
       <c r="S12" s="59">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="T12" s="59">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15">
@@ -34572,7 +34599,9 @@
       <c r="C13" s="151">
         <v>36</v>
       </c>
-      <c r="D13" s="151"/>
+      <c r="D13" s="151">
+        <v>36</v>
+      </c>
       <c r="E13" s="151"/>
       <c r="F13" s="151">
         <v>195</v>
@@ -34618,7 +34647,9 @@
       <c r="C14" s="151">
         <v>31</v>
       </c>
-      <c r="D14" s="151"/>
+      <c r="D14" s="151">
+        <v>32</v>
+      </c>
       <c r="E14" s="151"/>
       <c r="F14" s="151">
         <v>378</v>
@@ -34657,7 +34688,7 @@
       </c>
       <c r="U14">
         <f>SUM(S2:S16)</f>
-        <v>1316</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15">
@@ -34668,7 +34699,9 @@
       <c r="C15" s="151">
         <v>18</v>
       </c>
-      <c r="D15" s="151"/>
+      <c r="D15" s="151">
+        <v>21</v>
+      </c>
       <c r="E15" s="151"/>
       <c r="F15" s="151">
         <v>172</v>
@@ -34707,7 +34740,7 @@
       </c>
       <c r="U15">
         <f>SUM(T2:T18)</f>
-        <v>197</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15">
@@ -34718,7 +34751,9 @@
       <c r="C16" s="151">
         <v>13</v>
       </c>
-      <c r="D16" s="151"/>
+      <c r="D16" s="151">
+        <v>18</v>
+      </c>
       <c r="E16" s="151"/>
       <c r="F16" s="151">
         <v>218</v>
@@ -34802,7 +34837,7 @@
         <v>219</v>
       </c>
       <c r="S17" s="59">
-        <f t="shared" ref="S2:S18" si="2">C17</f>
+        <f t="shared" ref="S17:S18" si="2">C17</f>
         <v>85</v>
       </c>
       <c r="T17" s="59"/>
@@ -34851,22 +34886,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="153" t="s">
+      <c r="A19" s="154" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="153"/>
-      <c r="C19" s="153"/>
-      <c r="D19" s="153"/>
-      <c r="E19" s="153"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="153"/>
-      <c r="H19" s="153"/>
-      <c r="I19" s="153"/>
-      <c r="J19" s="153"/>
-      <c r="K19" s="153"/>
-      <c r="L19" s="153"/>
-      <c r="M19" s="153"/>
-      <c r="N19" s="153"/>
+      <c r="B19" s="154"/>
+      <c r="C19" s="154"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="154"/>
+      <c r="F19" s="154"/>
+      <c r="G19" s="154"/>
+      <c r="H19" s="154"/>
+      <c r="I19" s="154"/>
+      <c r="J19" s="154"/>
+      <c r="K19" s="154"/>
+      <c r="L19" s="154"/>
+      <c r="M19" s="154"/>
+      <c r="N19" s="154"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -34879,13 +34914,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="159" t="s">
+      <c r="Q22" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="160"/>
-      <c r="S22" s="160"/>
-      <c r="T22" s="160"/>
-      <c r="U22" s="161"/>
+      <c r="R22" s="161"/>
+      <c r="S22" s="161"/>
+      <c r="T22" s="161"/>
+      <c r="U22" s="162"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -34946,7 +34981,7 @@
       </c>
       <c r="U25" s="147">
         <f>T25/$T$32</f>
-        <v>8.7740384615384609E-2</v>
+        <v>8.2454819277108432E-2</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -34966,7 +35001,7 @@
       </c>
       <c r="U26" s="147">
         <f t="shared" ref="U26:U30" si="3">T26/$T$32</f>
-        <v>7.5320512820512817E-2</v>
+        <v>7.0783132530120488E-2</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -34999,11 +35034,11 @@
       </c>
       <c r="T28" s="135">
         <f>U14</f>
-        <v>1316</v>
+        <v>1434</v>
       </c>
       <c r="U28" s="147">
         <f t="shared" si="3"/>
-        <v>0.52724358974358976</v>
+        <v>0.53990963855421692</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -35019,11 +35054,11 @@
       </c>
       <c r="T29" s="135">
         <f>U15</f>
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="U29" s="147">
         <f t="shared" si="3"/>
-        <v>7.8926282051282048E-2</v>
+        <v>8.9984939759036139E-2</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -35041,7 +35076,7 @@
       </c>
       <c r="U30" s="147">
         <f t="shared" si="3"/>
-        <v>0.23076923076923078</v>
+        <v>0.21686746987951808</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -35060,7 +35095,7 @@
       <c r="S32" s="139"/>
       <c r="T32" s="140">
         <f>SUM(T25:T30)</f>
-        <v>2496</v>
+        <v>2656</v>
       </c>
       <c r="U32" s="148">
         <f>SUM(U25:U31)</f>
@@ -35132,6 +35167,9 @@
     <row r="40" spans="1:14">
       <c r="A40" s="62" t="s">
         <v>346</v>
+      </c>
+      <c r="B40" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -35188,7 +35226,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="T4:T16 S17:S18 S4:S16" emptyCellReference="1"/>
+    <ignoredError sqref="T4:T16 S17:S18 S4:S16 U32" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -35721,20 +35759,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="153" t="s">
+      <c r="A15" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="153"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="153"/>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
-      <c r="L15" s="153"/>
+      <c r="B15" s="154"/>
+      <c r="C15" s="154"/>
+      <c r="D15" s="154"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="154"/>
+      <c r="G15" s="154"/>
+      <c r="H15" s="154"/>
+      <c r="I15" s="154"/>
+      <c r="J15" s="154"/>
+      <c r="K15" s="154"/>
+      <c r="L15" s="154"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -35939,18 +35977,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="153"/>
-      <c r="B40" s="153"/>
-      <c r="C40" s="153"/>
-      <c r="D40" s="153"/>
-      <c r="E40" s="153"/>
-      <c r="F40" s="153"/>
-      <c r="G40" s="153"/>
-      <c r="H40" s="153"/>
-      <c r="I40" s="153"/>
-      <c r="J40" s="153"/>
-      <c r="K40" s="153"/>
-      <c r="L40" s="153"/>
+      <c r="A40" s="154"/>
+      <c r="B40" s="154"/>
+      <c r="C40" s="154"/>
+      <c r="D40" s="154"/>
+      <c r="E40" s="154"/>
+      <c r="F40" s="154"/>
+      <c r="G40" s="154"/>
+      <c r="H40" s="154"/>
+      <c r="I40" s="154"/>
+      <c r="J40" s="154"/>
+      <c r="K40" s="154"/>
+      <c r="L40" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -36584,20 +36622,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -37201,20 +37239,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -37824,20 +37862,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -38059,13 +38097,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="154" t="s">
+      <c r="U4" s="155" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="155"/>
-      <c r="W4" s="155"/>
-      <c r="X4" s="155"/>
-      <c r="Y4" s="156"/>
+      <c r="V4" s="156"/>
+      <c r="W4" s="156"/>
+      <c r="X4" s="156"/>
+      <c r="Y4" s="157"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -38102,9 +38140,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="157"/>
-      <c r="V5" s="158"/>
-      <c r="W5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -38694,20 +38732,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -39488,20 +39526,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="153" t="s">
+      <c r="A16" s="154" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="153"/>
-      <c r="C16" s="153"/>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
-      <c r="F16" s="153"/>
-      <c r="G16" s="153"/>
-      <c r="H16" s="153"/>
-      <c r="I16" s="153"/>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="153"/>
+      <c r="B16" s="154"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
+      <c r="H16" s="154"/>
+      <c r="I16" s="154"/>
+      <c r="J16" s="154"/>
+      <c r="K16" s="154"/>
+      <c r="L16" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mods and some v8 dot file deletions
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17060" windowHeight="16880" tabRatio="559" firstSheet="27" activeTab="30"/>
+    <workbookView xWindow="62400" yWindow="260" windowWidth="31320" windowHeight="20160" tabRatio="559" firstSheet="19" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,12 @@
     <sheet name="10.3" sheetId="42" r:id="rId29"/>
     <sheet name="10.12" sheetId="43" r:id="rId30"/>
     <sheet name="10.18" sheetId="44" r:id="rId31"/>
+    <sheet name="10.28" sheetId="45" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="29">'10.12'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="30">'10.18'!$A$1:$N$19</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="31">'10.28'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
@@ -171,29 +173,32 @@
   <connection id="30" name="Connection35" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="31" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="31" name="Connection36" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="32" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/index/12800?metric=tests/profiles/changelog?key=xml-murano-services-xml-profile-81269&amp;since=2015-09-02T19%3A11%3A38%2B0000&amp;to=2016-01-14T22%3A14%3A37%2B0000" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="32" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="33" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="33" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="34" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="34" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="35" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="35" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="36" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="36" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="37" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-mjenk01.dev.svbank.com:8080/job/T2%20web-payment-test-master/lastBuild/consoleText" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2445" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="357">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1261,6 +1266,12 @@
   <si>
     <t>B34  Prot E2E Integration test is both ../integration/mock &amp; ../integration/scenarios</t>
   </si>
+  <si>
+    <t xml:space="preserve">26min </t>
+  </si>
+  <si>
+    <t>Oct 28 2016</t>
+  </si>
 </sst>
 </file>
 
@@ -1894,7 +1905,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2202,6 +2213,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2399,7 +2413,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2443,7 +2457,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2487,7 +2501,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2838,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1034"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView topLeftCell="F24" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="V59" sqref="V59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -8576,13 +8594,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8619,9 +8637,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9203,20 +9221,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9679,13 +9697,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9722,9 +9740,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10306,20 +10324,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10514,13 +10532,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="155" t="s">
+      <c r="U25" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="156"/>
-      <c r="W25" s="156"/>
-      <c r="X25" s="156"/>
-      <c r="Y25" s="157"/>
+      <c r="V25" s="157"/>
+      <c r="W25" s="157"/>
+      <c r="X25" s="157"/>
+      <c r="Y25" s="158"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10533,9 +10551,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="158"/>
-      <c r="V26" s="159"/>
-      <c r="W26" s="159"/>
+      <c r="U26" s="159"/>
+      <c r="V26" s="160"/>
+      <c r="W26" s="160"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10929,13 +10947,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -10972,9 +10990,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11564,20 +11582,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12100,13 +12118,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -12143,9 +12161,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12746,20 +12764,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13304,13 +13322,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13347,9 +13365,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -13960,20 +13978,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14510,13 +14528,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14553,9 +14571,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15166,20 +15184,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15716,13 +15734,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15759,9 +15777,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16372,20 +16390,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16922,13 +16940,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -16965,9 +16983,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17578,20 +17596,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18131,13 +18149,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18174,9 +18192,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18790,20 +18808,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19280,13 +19298,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19323,9 +19341,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19939,20 +19957,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21094,13 +21112,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -21137,9 +21155,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21753,20 +21771,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -22856,20 +22874,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -23952,20 +23970,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="155" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="154"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="155"/>
+      <c r="F15" s="155"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
+      <c r="K15" s="155"/>
+      <c r="L15" s="155"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -25946,21 +25964,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
-      <c r="M16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
+      <c r="M16" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -26824,21 +26842,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
-      <c r="M16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
+      <c r="M16" s="155"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27719,20 +27737,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -29171,20 +29189,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -29481,7 +29499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
@@ -30218,20 +30236,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="154" t="s">
+      <c r="A17" s="155" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="154"/>
-      <c r="C17" s="154"/>
-      <c r="D17" s="154"/>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
-      <c r="L17" s="154"/>
+      <c r="B17" s="155"/>
+      <c r="C17" s="155"/>
+      <c r="D17" s="155"/>
+      <c r="E17" s="155"/>
+      <c r="F17" s="155"/>
+      <c r="G17" s="155"/>
+      <c r="H17" s="155"/>
+      <c r="I17" s="155"/>
+      <c r="J17" s="155"/>
+      <c r="K17" s="155"/>
+      <c r="L17" s="155"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30242,13 +30260,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="160" t="s">
+      <c r="O19" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="161"/>
-      <c r="Q19" s="161"/>
-      <c r="R19" s="161"/>
-      <c r="S19" s="162"/>
+      <c r="P19" s="162"/>
+      <c r="Q19" s="162"/>
+      <c r="R19" s="162"/>
+      <c r="S19" s="163"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -31338,34 +31356,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="154" t="s">
+      <c r="A18" s="155" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="154"/>
-      <c r="C18" s="154"/>
-      <c r="D18" s="154"/>
-      <c r="E18" s="154"/>
-      <c r="F18" s="154"/>
-      <c r="G18" s="154"/>
-      <c r="H18" s="154"/>
-      <c r="I18" s="154"/>
-      <c r="J18" s="154"/>
-      <c r="K18" s="154"/>
-      <c r="L18" s="154"/>
-      <c r="M18" s="154"/>
-      <c r="N18" s="154"/>
+      <c r="B18" s="155"/>
+      <c r="C18" s="155"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="155"/>
+      <c r="F18" s="155"/>
+      <c r="G18" s="155"/>
+      <c r="H18" s="155"/>
+      <c r="I18" s="155"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="155"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="155"/>
+      <c r="N18" s="155"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="160" t="s">
+      <c r="Q19" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="161"/>
-      <c r="S19" s="161"/>
-      <c r="T19" s="161"/>
-      <c r="U19" s="162"/>
+      <c r="R19" s="162"/>
+      <c r="S19" s="162"/>
+      <c r="T19" s="162"/>
+      <c r="U19" s="163"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -32244,8 +32262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -33215,13 +33233,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="160" t="s">
+      <c r="Q22" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="161"/>
-      <c r="S22" s="161"/>
-      <c r="T22" s="161"/>
-      <c r="U22" s="162"/>
+      <c r="R22" s="162"/>
+      <c r="S22" s="162"/>
+      <c r="T22" s="162"/>
+      <c r="U22" s="163"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -33916,10 +33934,10 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U45"/>
+  <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L7" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T28" sqref="T28:T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -33945,7 +33963,7 @@
     <col min="21" max="21" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="45">
+    <row r="1" spans="1:22" ht="45">
       <c r="A1" s="18" t="s">
         <v>103</v>
       </c>
@@ -34001,7 +34019,7 @@
         <v>Int</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15">
+    <row r="2" spans="1:22" ht="15">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>119</v>
@@ -34050,8 +34068,11 @@
         <f t="shared" ref="T2:T16" si="0">E2</f>
         <v>124</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" ht="15">
+      <c r="V2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="15">
       <c r="A3" s="20"/>
       <c r="B3" s="22" t="s">
         <v>117</v>
@@ -34106,8 +34127,11 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="15">
+      <c r="V3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15">
       <c r="A4" s="19"/>
       <c r="B4" s="22" t="s">
         <v>329</v>
@@ -34162,8 +34186,11 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" ht="15">
+      <c r="V4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15">
       <c r="A5" s="20"/>
       <c r="B5" s="22" t="s">
         <v>128</v>
@@ -34216,8 +34243,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15">
+      <c r="V5">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="22" t="s">
         <v>114</v>
@@ -34270,8 +34300,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="15">
+      <c r="V6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15">
       <c r="A7" s="19"/>
       <c r="B7" s="22" t="s">
         <v>133</v>
@@ -34324,8 +34357,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="15">
+      <c r="V7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="22" t="s">
         <v>123</v>
@@ -34380,8 +34416,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="15">
+      <c r="V8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="22" t="s">
         <v>139</v>
@@ -34437,7 +34476,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15">
+    <row r="10" spans="1:22" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="22" t="s">
         <v>127</v>
@@ -34491,7 +34530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15">
+    <row r="11" spans="1:22" ht="15">
       <c r="A11" s="20"/>
       <c r="B11" s="22" t="s">
         <v>292</v>
@@ -34541,7 +34580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15">
+    <row r="12" spans="1:22" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="22" t="s">
         <v>336</v>
@@ -34591,7 +34630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15">
+    <row r="13" spans="1:22" ht="15">
       <c r="A13" s="20"/>
       <c r="B13" s="22" t="s">
         <v>126</v>
@@ -34639,7 +34678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15">
+    <row r="14" spans="1:22" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="22" t="s">
         <v>131</v>
@@ -34691,7 +34730,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15">
+    <row r="15" spans="1:22" ht="15">
       <c r="A15" s="20"/>
       <c r="B15" s="22" t="s">
         <v>125</v>
@@ -34743,7 +34782,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15">
+    <row r="16" spans="1:22" ht="15">
       <c r="A16" s="20"/>
       <c r="B16" s="22" t="s">
         <v>130</v>
@@ -34886,22 +34925,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="154" t="s">
+      <c r="A19" s="155" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="154"/>
-      <c r="C19" s="154"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="154"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="154"/>
-      <c r="H19" s="154"/>
-      <c r="I19" s="154"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="154"/>
-      <c r="M19" s="154"/>
-      <c r="N19" s="154"/>
+      <c r="B19" s="155"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="155"/>
+      <c r="G19" s="155"/>
+      <c r="H19" s="155"/>
+      <c r="I19" s="155"/>
+      <c r="J19" s="155"/>
+      <c r="K19" s="155"/>
+      <c r="L19" s="155"/>
+      <c r="M19" s="155"/>
+      <c r="N19" s="155"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -34914,13 +34953,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="160" t="s">
+      <c r="Q22" s="161" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="161"/>
-      <c r="S22" s="161"/>
-      <c r="T22" s="161"/>
-      <c r="U22" s="162"/>
+      <c r="R22" s="162"/>
+      <c r="S22" s="162"/>
+      <c r="T22" s="162"/>
+      <c r="U22" s="163"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -35236,6 +35275,1356 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="45">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="152" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" s="152" t="s">
+        <v>349</v>
+      </c>
+      <c r="S1" s="59" t="str">
+        <f>C1</f>
+        <v xml:space="preserve">UTs </v>
+      </c>
+      <c r="T1" s="59" t="str">
+        <f>E1</f>
+        <v>Int</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="154">
+        <v>591</v>
+      </c>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154">
+        <v>127</v>
+      </c>
+      <c r="F2" s="23">
+        <v>6330</v>
+      </c>
+      <c r="G2" s="154" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="26">
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="I2" s="25">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="J2" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="K2" s="154">
+        <v>0</v>
+      </c>
+      <c r="L2" s="154">
+        <v>0</v>
+      </c>
+      <c r="M2" s="154">
+        <v>2</v>
+      </c>
+      <c r="N2" s="154">
+        <v>0</v>
+      </c>
+      <c r="S2" s="59">
+        <f>C2-E2</f>
+        <v>464</v>
+      </c>
+      <c r="T2" s="59">
+        <f t="shared" ref="T2:T16" si="0">E2</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="154">
+        <v>194</v>
+      </c>
+      <c r="D3" s="154"/>
+      <c r="E3" s="154">
+        <v>40</v>
+      </c>
+      <c r="F3" s="23">
+        <v>1760</v>
+      </c>
+      <c r="G3" s="154" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="26">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="J3" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="K3" s="154">
+        <v>0</v>
+      </c>
+      <c r="L3" s="154">
+        <v>0</v>
+      </c>
+      <c r="M3" s="154">
+        <v>2</v>
+      </c>
+      <c r="N3" s="154">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>265</v>
+      </c>
+      <c r="R3">
+        <v>14</v>
+      </c>
+      <c r="S3" s="59">
+        <f t="shared" ref="S3:S18" si="1">C3-E3</f>
+        <v>154</v>
+      </c>
+      <c r="T3" s="59">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15">
+      <c r="A4" s="19"/>
+      <c r="B4" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="154">
+        <v>172</v>
+      </c>
+      <c r="D4" s="154"/>
+      <c r="E4" s="154">
+        <v>43</v>
+      </c>
+      <c r="F4" s="23">
+        <v>2233</v>
+      </c>
+      <c r="G4" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="24">
+        <v>42667</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J4" s="25">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="K4" s="154">
+        <v>0</v>
+      </c>
+      <c r="L4" s="154">
+        <v>0</v>
+      </c>
+      <c r="M4" s="154">
+        <v>1</v>
+      </c>
+      <c r="N4" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>258</v>
+      </c>
+      <c r="R4">
+        <v>153</v>
+      </c>
+      <c r="S4" s="59">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="T4" s="59">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="154">
+        <v>132</v>
+      </c>
+      <c r="D5" s="154"/>
+      <c r="E5" s="154"/>
+      <c r="F5" s="154">
+        <v>871</v>
+      </c>
+      <c r="G5" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0.95</v>
+      </c>
+      <c r="J5" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K5" s="154">
+        <v>0</v>
+      </c>
+      <c r="L5" s="154">
+        <v>0</v>
+      </c>
+      <c r="M5" s="154">
+        <v>1</v>
+      </c>
+      <c r="N5" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>259</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="59">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="T5" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="154">
+        <v>114</v>
+      </c>
+      <c r="D6" s="154"/>
+      <c r="E6" s="154"/>
+      <c r="F6" s="23">
+        <v>1638</v>
+      </c>
+      <c r="G6" s="154" t="s">
+        <v>355</v>
+      </c>
+      <c r="H6" s="24">
+        <v>42667</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="J6" s="25">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="K6" s="154">
+        <v>0</v>
+      </c>
+      <c r="L6" s="154">
+        <v>0</v>
+      </c>
+      <c r="M6" s="154">
+        <v>2</v>
+      </c>
+      <c r="N6" s="154">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" s="59">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="T6" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
+      <c r="A7" s="19"/>
+      <c r="B7" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="154">
+        <v>82</v>
+      </c>
+      <c r="D7" s="154"/>
+      <c r="E7" s="154"/>
+      <c r="F7" s="154">
+        <v>677</v>
+      </c>
+      <c r="G7" s="154" t="s">
+        <v>351</v>
+      </c>
+      <c r="H7" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="J7" s="25">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="K7" s="154">
+        <v>0</v>
+      </c>
+      <c r="L7" s="154">
+        <v>0</v>
+      </c>
+      <c r="M7" s="154">
+        <v>1</v>
+      </c>
+      <c r="N7" s="154">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>268</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7" s="59">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="T7" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="154">
+        <v>69</v>
+      </c>
+      <c r="D8" s="154"/>
+      <c r="E8" s="154">
+        <v>16</v>
+      </c>
+      <c r="F8" s="154">
+        <v>839</v>
+      </c>
+      <c r="G8" s="154" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" s="24">
+        <v>42657</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="J8" s="25">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="K8" s="154">
+        <v>0</v>
+      </c>
+      <c r="L8" s="154">
+        <v>0</v>
+      </c>
+      <c r="M8" s="154">
+        <v>2</v>
+      </c>
+      <c r="N8" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R8">
+        <v>27</v>
+      </c>
+      <c r="S8" s="59">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="T8" s="59">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="154">
+        <v>61</v>
+      </c>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154">
+        <v>11</v>
+      </c>
+      <c r="F9" s="154">
+        <v>693</v>
+      </c>
+      <c r="G9" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="24">
+        <v>42661</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="J9" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="K9" s="154">
+        <v>0</v>
+      </c>
+      <c r="L9" s="154">
+        <v>0</v>
+      </c>
+      <c r="M9" s="154">
+        <v>0</v>
+      </c>
+      <c r="N9" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>263</v>
+      </c>
+      <c r="R9">
+        <v>7</v>
+      </c>
+      <c r="S9" s="59">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="T9" s="59">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="154">
+        <v>59</v>
+      </c>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="154">
+        <v>344</v>
+      </c>
+      <c r="G10" s="154">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="J10" s="25">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="K10" s="154">
+        <v>0</v>
+      </c>
+      <c r="L10" s="154">
+        <v>0</v>
+      </c>
+      <c r="M10" s="154">
+        <v>0</v>
+      </c>
+      <c r="N10" s="154">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>264</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="59">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="T10" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="154">
+        <v>44</v>
+      </c>
+      <c r="D11" s="154"/>
+      <c r="E11" s="154">
+        <v>5</v>
+      </c>
+      <c r="F11" s="154">
+        <v>573</v>
+      </c>
+      <c r="G11" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="24">
+        <v>42657</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="J11" s="25">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="K11" s="154">
+        <v>0</v>
+      </c>
+      <c r="L11" s="154">
+        <v>0</v>
+      </c>
+      <c r="M11" s="154">
+        <v>1</v>
+      </c>
+      <c r="N11" s="154">
+        <v>0</v>
+      </c>
+      <c r="S11" s="59">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="T11" s="59">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="154">
+        <v>41</v>
+      </c>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154">
+        <v>4</v>
+      </c>
+      <c r="F12" s="154">
+        <v>567</v>
+      </c>
+      <c r="G12" s="154" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" s="24">
+        <v>42657</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="K12" s="154">
+        <v>0</v>
+      </c>
+      <c r="L12" s="154">
+        <v>0</v>
+      </c>
+      <c r="M12" s="154">
+        <v>1</v>
+      </c>
+      <c r="N12" s="154">
+        <v>0</v>
+      </c>
+      <c r="S12" s="59">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="T12" s="59">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="154">
+        <v>36</v>
+      </c>
+      <c r="D13" s="154"/>
+      <c r="E13" s="154"/>
+      <c r="F13" s="154">
+        <v>195</v>
+      </c>
+      <c r="G13" s="154">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="J13" s="25">
+        <v>1</v>
+      </c>
+      <c r="K13" s="154">
+        <v>0</v>
+      </c>
+      <c r="L13" s="154">
+        <v>0</v>
+      </c>
+      <c r="M13" s="154">
+        <v>0</v>
+      </c>
+      <c r="N13" s="154">
+        <v>0</v>
+      </c>
+      <c r="S13" s="59">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="T13" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="154">
+        <v>31</v>
+      </c>
+      <c r="D14" s="154"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="154">
+        <v>378</v>
+      </c>
+      <c r="G14" s="154" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="K14" s="154">
+        <v>0</v>
+      </c>
+      <c r="L14" s="154">
+        <v>0</v>
+      </c>
+      <c r="M14" s="154">
+        <v>1</v>
+      </c>
+      <c r="N14" s="154">
+        <v>0</v>
+      </c>
+      <c r="S14" s="59">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="T14" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f>SUM(S2:S16)</f>
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="154">
+        <v>18</v>
+      </c>
+      <c r="D15" s="154"/>
+      <c r="E15" s="154"/>
+      <c r="F15" s="154">
+        <v>172</v>
+      </c>
+      <c r="G15" s="154">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="K15" s="154">
+        <v>0</v>
+      </c>
+      <c r="L15" s="154">
+        <v>0</v>
+      </c>
+      <c r="M15" s="154">
+        <v>0</v>
+      </c>
+      <c r="N15" s="154">
+        <v>0</v>
+      </c>
+      <c r="S15" s="59">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T15" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>SUM(T2:T18)</f>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="154">
+        <v>13</v>
+      </c>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154">
+        <v>218</v>
+      </c>
+      <c r="G16" s="154">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
+        <v>42660</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="J16" s="25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="K16" s="154">
+        <v>0</v>
+      </c>
+      <c r="L16" s="154">
+        <v>0</v>
+      </c>
+      <c r="M16" s="154">
+        <v>0</v>
+      </c>
+      <c r="N16" s="154">
+        <v>0</v>
+      </c>
+      <c r="S16" s="59">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="T16" s="59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>SUM(S17:S18)</f>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="31">
+        <f>C23</f>
+        <v>113</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="23">
+        <v>3041</v>
+      </c>
+      <c r="G17" s="154">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
+        <v>42578</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="J17" s="25">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="K17" s="154">
+        <v>0</v>
+      </c>
+      <c r="L17" s="154">
+        <v>0</v>
+      </c>
+      <c r="M17" s="154">
+        <v>0</v>
+      </c>
+      <c r="N17" s="154">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>SUM(R3:R10)</f>
+        <v>219</v>
+      </c>
+      <c r="S17" s="59">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="T17" s="59"/>
+    </row>
+    <row r="18" spans="1:21" ht="15">
+      <c r="A18" s="20"/>
+      <c r="B18" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="31">
+        <f>C25</f>
+        <v>491</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="23">
+        <v>10346</v>
+      </c>
+      <c r="G18" s="154" t="s">
+        <v>154</v>
+      </c>
+      <c r="H18" s="24">
+        <v>42663</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="J18" s="25">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K18" s="154">
+        <v>0</v>
+      </c>
+      <c r="L18" s="154">
+        <v>0</v>
+      </c>
+      <c r="M18" s="154">
+        <v>0</v>
+      </c>
+      <c r="N18" s="154">
+        <v>0</v>
+      </c>
+      <c r="S18" s="59">
+        <f t="shared" si="1"/>
+        <v>491</v>
+      </c>
+      <c r="T18" s="59"/>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="155" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19" s="155"/>
+      <c r="C19" s="155"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="155"/>
+      <c r="F19" s="155"/>
+      <c r="G19" s="155"/>
+      <c r="H19" s="155"/>
+      <c r="I19" s="155"/>
+      <c r="J19" s="155"/>
+      <c r="K19" s="155"/>
+      <c r="L19" s="155"/>
+      <c r="M19" s="155"/>
+      <c r="N19" s="155"/>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="B20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15" thickBot="1">
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" thickBot="1">
+      <c r="Q22" s="161" t="s">
+        <v>164</v>
+      </c>
+      <c r="R22" s="162"/>
+      <c r="S22" s="162"/>
+      <c r="T22" s="162"/>
+      <c r="U22" s="163"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>113</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="H23" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q23" s="124"/>
+      <c r="R23" s="125"/>
+      <c r="S23" s="125"/>
+      <c r="T23" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="U23" s="145" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="G24" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="129"/>
+      <c r="S24" s="129"/>
+      <c r="T24" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="146"/>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25">
+        <v>491</v>
+      </c>
+      <c r="G25" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="H25" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q25" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="133"/>
+      <c r="S25" s="134"/>
+      <c r="T25" s="135">
+        <f>R17</f>
+        <v>219</v>
+      </c>
+      <c r="U25" s="147">
+        <f>T25/$T$32</f>
+        <v>8.20839580209895E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="G26" s="58"/>
+      <c r="Q26" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="R26" s="133" t="s">
+        <v>333</v>
+      </c>
+      <c r="S26" s="134" t="s">
+        <v>334</v>
+      </c>
+      <c r="T26" s="135">
+        <f>C34</f>
+        <v>188</v>
+      </c>
+      <c r="U26" s="147">
+        <f t="shared" ref="U26:U30" si="2">T26/$T$32</f>
+        <v>7.0464767616191901E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="B27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q27" s="132"/>
+      <c r="R27" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="S27" s="134"/>
+      <c r="T27" s="135">
+        <v>0</v>
+      </c>
+      <c r="U27" s="147"/>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="C28" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q28" s="132"/>
+      <c r="R28" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="S28" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T28" s="135">
+        <f>U14</f>
+        <v>1411</v>
+      </c>
+      <c r="U28" s="147">
+        <f t="shared" si="2"/>
+        <v>0.52886056971514239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="C29" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q29" s="132"/>
+      <c r="R29" s="133" t="s">
+        <v>331</v>
+      </c>
+      <c r="S29" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T29" s="135">
+        <f>U15</f>
+        <v>246</v>
+      </c>
+      <c r="U29" s="147">
+        <f t="shared" si="2"/>
+        <v>9.2203898050974509E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="C30" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q30" s="132"/>
+      <c r="R30" s="133"/>
+      <c r="S30" s="134" t="s">
+        <v>347</v>
+      </c>
+      <c r="T30" s="135">
+        <f>U16</f>
+        <v>604</v>
+      </c>
+      <c r="U30" s="147">
+        <f t="shared" si="2"/>
+        <v>0.22638680659670166</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q31" s="132"/>
+      <c r="R31" s="133"/>
+      <c r="S31" s="134"/>
+      <c r="T31" s="135"/>
+      <c r="U31" s="147"/>
+    </row>
+    <row r="32" spans="1:21" ht="15" thickBot="1">
+      <c r="Q32" s="137"/>
+      <c r="R32" s="138"/>
+      <c r="S32" s="139"/>
+      <c r="T32" s="140">
+        <f>SUM(T25:T30)</f>
+        <v>2668</v>
+      </c>
+      <c r="U32" s="148">
+        <f>SUM(U25:U31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="B33" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="123" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="122"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="B34" t="s">
+        <v>339</v>
+      </c>
+      <c r="C34">
+        <v>188</v>
+      </c>
+      <c r="G34" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="H34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" s="62" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" s="62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B37" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" s="62"/>
+      <c r="B38" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="A39" s="62" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="A40" s="62" t="s">
+        <v>346</v>
+      </c>
+      <c r="B40" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" s="62"/>
+      <c r="Q41">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" s="62"/>
+      <c r="Q42">
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="Q43">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="Q44">
+        <v>52.89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="F45">
+        <f>C5</f>
+        <v>132</v>
+      </c>
+      <c r="Q45">
+        <v>22.64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="F46">
+        <f>C7</f>
+        <v>82</v>
+      </c>
+      <c r="Q46">
+        <f>Q41-SUM(Q42:Q45)</f>
+        <v>9.2099999999999937</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="F47">
+        <f>C10</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="F48">
+        <f>C13</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6">
+      <c r="F49">
+        <f t="shared" ref="F49:F56" si="3">C14</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6">
+      <c r="F50">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6">
+      <c r="F51">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="Q22:U22"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
+    <hyperlink ref="B1" tooltip="Name" display="Name"/>
+    <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
+    <hyperlink ref="F1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="G1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="H1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="I1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="J1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="K1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="L1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="M1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="N1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="svb-service-ooba"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="mur-java-lib-httpclient"/>
+    <hyperlink ref="B6" r:id="rId5" tooltip="svb-scheduler-payments"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="mur-java-lib-auth"/>
+    <hyperlink ref="B8" r:id="rId7" tooltip="svb-service-accounts"/>
+    <hyperlink ref="B9" r:id="rId8" tooltip="svb-service-csrf"/>
+    <hyperlink ref="B10" r:id="rId9" tooltip="mur-java-lib-dbconnector"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="svb-service-client"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="svb-service-bankinfo"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="mur-java-lib-logger"/>
+    <hyperlink ref="B14" r:id="rId13" tooltip="mur-java-lib-monitoring"/>
+    <hyperlink ref="B15" r:id="rId14" tooltip="mur-java-lib-exception"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="mur-java-lib-mappers"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="svb-web-core-ui"/>
+    <hyperlink ref="B18" r:id="rId17" tooltip="svb-web-payment"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <ignoredErrors>
+    <ignoredError sqref="T5:T16 S5:S19 U15 U32" emptyCellReference="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
@@ -35759,20 +37148,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="154" t="s">
+      <c r="A15" s="155" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="154"/>
-      <c r="C15" s="154"/>
-      <c r="D15" s="154"/>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="154"/>
+      <c r="B15" s="155"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="155"/>
+      <c r="F15" s="155"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
+      <c r="K15" s="155"/>
+      <c r="L15" s="155"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -35977,18 +37366,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="154"/>
-      <c r="B40" s="154"/>
-      <c r="C40" s="154"/>
-      <c r="D40" s="154"/>
-      <c r="E40" s="154"/>
-      <c r="F40" s="154"/>
-      <c r="G40" s="154"/>
-      <c r="H40" s="154"/>
-      <c r="I40" s="154"/>
-      <c r="J40" s="154"/>
-      <c r="K40" s="154"/>
-      <c r="L40" s="154"/>
+      <c r="A40" s="155"/>
+      <c r="B40" s="155"/>
+      <c r="C40" s="155"/>
+      <c r="D40" s="155"/>
+      <c r="E40" s="155"/>
+      <c r="F40" s="155"/>
+      <c r="G40" s="155"/>
+      <c r="H40" s="155"/>
+      <c r="I40" s="155"/>
+      <c r="J40" s="155"/>
+      <c r="K40" s="155"/>
+      <c r="L40" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -36622,20 +38011,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -37239,20 +38628,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -37862,20 +39251,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -38097,13 +39486,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="155" t="s">
+      <c r="U4" s="156" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="156"/>
-      <c r="W4" s="156"/>
-      <c r="X4" s="156"/>
-      <c r="Y4" s="157"/>
+      <c r="V4" s="157"/>
+      <c r="W4" s="157"/>
+      <c r="X4" s="157"/>
+      <c r="Y4" s="158"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -38140,9 +39529,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="158"/>
-      <c r="V5" s="159"/>
-      <c r="W5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -38732,20 +40121,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -39526,20 +40915,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="154" t="s">
+      <c r="A16" s="155" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="154"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
-      <c r="L16" s="154"/>
+      <c r="B16" s="155"/>
+      <c r="C16" s="155"/>
+      <c r="D16" s="155"/>
+      <c r="E16" s="155"/>
+      <c r="F16" s="155"/>
+      <c r="G16" s="155"/>
+      <c r="H16" s="155"/>
+      <c r="I16" s="155"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="155"/>
+      <c r="L16" s="155"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Dot Files , Mashup text, Excel files
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="28060" windowHeight="15960" tabRatio="559" firstSheet="23" activeTab="32"/>
+    <workbookView xWindow="31000" yWindow="1420" windowWidth="23980" windowHeight="13160" tabRatio="559" firstSheet="23" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -40,12 +40,14 @@
     <sheet name="10.18" sheetId="44" r:id="rId31"/>
     <sheet name="10.28" sheetId="45" r:id="rId32"/>
     <sheet name="Sheet1" sheetId="46" r:id="rId33"/>
+    <sheet name="11.14" sheetId="47" r:id="rId34"/>
   </sheets>
   <definedNames>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="29">'10.12'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="30">'10.18'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="31">'10.28'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="33">'11.14'!$A$1:$L$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="9">'3.25'!$A$1:$L$16</definedName>
@@ -185,29 +187,32 @@
   <connection id="33" name="Connection38" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="34" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="34" name="Connection39" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="35" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/index/12800?metric=tests/profiles/changelog?key=xml-murano-services-xml-profile-81269&amp;since=2015-09-02T19%3A11%3A38%2B0000&amp;to=2016-01-14T22%3A14%3A37%2B0000" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="35" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="36" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="36" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="37" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="37" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="38" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="38" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="39" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="39" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="40" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-mjenk01.dev.svbank.com:8080/job/T2%20web-payment-test-master/lastBuild/consoleText" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="360">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1287,6 +1292,9 @@
   <si>
     <t xml:space="preserve">2d 1h </t>
   </si>
+  <si>
+    <t xml:space="preserve">1h 15min </t>
+  </si>
 </sst>
 </file>
 
@@ -1920,7 +1928,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="166">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2237,6 +2245,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2434,7 +2445,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2478,7 +2489,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2522,7 +2533,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="35" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="36" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2530,11 +2541,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8623,13 +8638,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8666,9 +8681,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9250,20 +9265,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9726,13 +9741,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9769,9 +9784,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10353,20 +10368,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10561,13 +10576,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="158" t="s">
+      <c r="U25" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="159"/>
-      <c r="W25" s="159"/>
-      <c r="X25" s="159"/>
-      <c r="Y25" s="160"/>
+      <c r="V25" s="160"/>
+      <c r="W25" s="160"/>
+      <c r="X25" s="160"/>
+      <c r="Y25" s="161"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10580,9 +10595,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="161"/>
-      <c r="V26" s="162"/>
-      <c r="W26" s="162"/>
+      <c r="U26" s="162"/>
+      <c r="V26" s="163"/>
+      <c r="W26" s="163"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10976,13 +10991,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -11019,9 +11034,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11611,20 +11626,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12147,13 +12162,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -12190,9 +12205,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12793,20 +12808,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13351,13 +13366,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13394,9 +13409,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -14007,20 +14022,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14557,13 +14572,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14600,9 +14615,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15213,20 +15228,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15763,13 +15778,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15806,9 +15821,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16419,20 +16434,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16969,13 +16984,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -17012,9 +17027,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17625,20 +17640,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18178,13 +18193,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18221,9 +18236,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18837,20 +18852,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19327,13 +19342,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19370,9 +19385,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19986,20 +20001,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21141,13 +21156,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -21184,9 +21199,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21800,20 +21815,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -22903,20 +22918,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -23999,20 +24014,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="158" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="157"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="157"/>
-      <c r="J15" s="157"/>
-      <c r="K15" s="157"/>
-      <c r="L15" s="157"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="158"/>
+      <c r="H15" s="158"/>
+      <c r="I15" s="158"/>
+      <c r="J15" s="158"/>
+      <c r="K15" s="158"/>
+      <c r="L15" s="158"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -25993,21 +26008,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
-      <c r="M16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
+      <c r="M16" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -26871,21 +26886,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
-      <c r="M16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
+      <c r="M16" s="158"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27766,20 +27781,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -29218,20 +29233,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -30265,20 +30280,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="157" t="s">
+      <c r="A17" s="158" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="157"/>
-      <c r="C17" s="157"/>
-      <c r="D17" s="157"/>
-      <c r="E17" s="157"/>
-      <c r="F17" s="157"/>
-      <c r="G17" s="157"/>
-      <c r="H17" s="157"/>
-      <c r="I17" s="157"/>
-      <c r="J17" s="157"/>
-      <c r="K17" s="157"/>
-      <c r="L17" s="157"/>
+      <c r="B17" s="158"/>
+      <c r="C17" s="158"/>
+      <c r="D17" s="158"/>
+      <c r="E17" s="158"/>
+      <c r="F17" s="158"/>
+      <c r="G17" s="158"/>
+      <c r="H17" s="158"/>
+      <c r="I17" s="158"/>
+      <c r="J17" s="158"/>
+      <c r="K17" s="158"/>
+      <c r="L17" s="158"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30289,13 +30304,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="163" t="s">
+      <c r="O19" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="164"/>
-      <c r="Q19" s="164"/>
-      <c r="R19" s="164"/>
-      <c r="S19" s="165"/>
+      <c r="P19" s="165"/>
+      <c r="Q19" s="165"/>
+      <c r="R19" s="165"/>
+      <c r="S19" s="166"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -31385,34 +31400,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="157" t="s">
+      <c r="A18" s="158" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="157"/>
-      <c r="C18" s="157"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="157"/>
-      <c r="F18" s="157"/>
-      <c r="G18" s="157"/>
-      <c r="H18" s="157"/>
-      <c r="I18" s="157"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="157"/>
-      <c r="L18" s="157"/>
-      <c r="M18" s="157"/>
-      <c r="N18" s="157"/>
+      <c r="B18" s="158"/>
+      <c r="C18" s="158"/>
+      <c r="D18" s="158"/>
+      <c r="E18" s="158"/>
+      <c r="F18" s="158"/>
+      <c r="G18" s="158"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="158"/>
+      <c r="J18" s="158"/>
+      <c r="K18" s="158"/>
+      <c r="L18" s="158"/>
+      <c r="M18" s="158"/>
+      <c r="N18" s="158"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="163" t="s">
+      <c r="Q19" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="164"/>
-      <c r="S19" s="164"/>
-      <c r="T19" s="164"/>
-      <c r="U19" s="165"/>
+      <c r="R19" s="165"/>
+      <c r="S19" s="165"/>
+      <c r="T19" s="165"/>
+      <c r="U19" s="166"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -33262,13 +33277,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="163" t="s">
+      <c r="Q22" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="164"/>
-      <c r="S22" s="164"/>
-      <c r="T22" s="164"/>
-      <c r="U22" s="165"/>
+      <c r="R22" s="165"/>
+      <c r="S22" s="165"/>
+      <c r="T22" s="165"/>
+      <c r="U22" s="166"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -34954,22 +34969,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="158" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
-      <c r="H19" s="157"/>
-      <c r="I19" s="157"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="157"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="158"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -34982,13 +34997,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="163" t="s">
+      <c r="Q22" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="164"/>
-      <c r="S22" s="164"/>
-      <c r="T22" s="164"/>
-      <c r="U22" s="165"/>
+      <c r="R22" s="165"/>
+      <c r="S22" s="165"/>
+      <c r="T22" s="165"/>
+      <c r="U22" s="166"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -36249,22 +36264,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="158" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
-      <c r="H19" s="157"/>
-      <c r="I19" s="157"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="157"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="158"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -36277,13 +36292,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="163" t="s">
+      <c r="Q22" s="164" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="164"/>
-      <c r="S22" s="164"/>
-      <c r="T22" s="164"/>
-      <c r="U22" s="165"/>
+      <c r="R22" s="165"/>
+      <c r="S22" s="165"/>
+      <c r="T22" s="165"/>
+      <c r="U22" s="166"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -36658,7 +36673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
@@ -37532,24 +37547,24 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="157" t="s">
+      <c r="A19" s="158" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="157"/>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="157"/>
-      <c r="F19" s="157"/>
-      <c r="G19" s="157"/>
-      <c r="H19" s="157"/>
-      <c r="I19" s="157"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="157"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="157"/>
-      <c r="O19" s="157"/>
-      <c r="P19" s="157"/>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="158"/>
+      <c r="O19" s="158"/>
+      <c r="P19" s="158"/>
     </row>
     <row r="23" spans="1:16" ht="60">
       <c r="A23" s="18" t="s">
@@ -38350,20 +38365,20 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="157" t="s">
+      <c r="A43" s="158" t="s">
         <v>357</v>
       </c>
-      <c r="B43" s="157"/>
-      <c r="C43" s="157"/>
-      <c r="D43" s="157"/>
-      <c r="E43" s="157"/>
-      <c r="F43" s="157"/>
-      <c r="G43" s="157"/>
-      <c r="H43" s="157"/>
-      <c r="I43" s="157"/>
-      <c r="J43" s="157"/>
-      <c r="K43" s="157"/>
-      <c r="L43" s="157"/>
+      <c r="B43" s="158"/>
+      <c r="C43" s="158"/>
+      <c r="D43" s="158"/>
+      <c r="E43" s="158"/>
+      <c r="F43" s="158"/>
+      <c r="G43" s="158"/>
+      <c r="H43" s="158"/>
+      <c r="I43" s="158"/>
+      <c r="J43" s="158"/>
+      <c r="K43" s="158"/>
+      <c r="L43" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -38441,6 +38456,733 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="157">
+        <v>491</v>
+      </c>
+      <c r="D2" s="23">
+        <v>5271</v>
+      </c>
+      <c r="E2" s="157" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G2" s="25">
+        <v>0.92</v>
+      </c>
+      <c r="H2" s="25">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="I2" s="157">
+        <v>0</v>
+      </c>
+      <c r="J2" s="157">
+        <v>0</v>
+      </c>
+      <c r="K2" s="157">
+        <v>2</v>
+      </c>
+      <c r="L2" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="157">
+        <v>210</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1879</v>
+      </c>
+      <c r="E3" s="157" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="24">
+        <v>42682</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="I3" s="157">
+        <v>0</v>
+      </c>
+      <c r="J3" s="157">
+        <v>0</v>
+      </c>
+      <c r="K3" s="157">
+        <v>2</v>
+      </c>
+      <c r="L3" s="157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15">
+      <c r="A4" s="19"/>
+      <c r="B4" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="157">
+        <v>181</v>
+      </c>
+      <c r="D4" s="23">
+        <v>2270</v>
+      </c>
+      <c r="E4" s="157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F4" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G4" s="25">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="I4" s="157">
+        <v>0</v>
+      </c>
+      <c r="J4" s="157">
+        <v>0</v>
+      </c>
+      <c r="K4" s="157">
+        <v>1</v>
+      </c>
+      <c r="L4" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="157">
+        <v>133</v>
+      </c>
+      <c r="D5" s="157">
+        <v>892</v>
+      </c>
+      <c r="E5" s="157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="I5" s="157">
+        <v>0</v>
+      </c>
+      <c r="J5" s="157">
+        <v>0</v>
+      </c>
+      <c r="K5" s="157">
+        <v>1</v>
+      </c>
+      <c r="L5" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="157">
+        <v>114</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1638</v>
+      </c>
+      <c r="E6" s="157" t="s">
+        <v>355</v>
+      </c>
+      <c r="F6" s="24">
+        <v>42676</v>
+      </c>
+      <c r="G6" s="25">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="I6" s="157">
+        <v>0</v>
+      </c>
+      <c r="J6" s="157">
+        <v>0</v>
+      </c>
+      <c r="K6" s="157">
+        <v>2</v>
+      </c>
+      <c r="L6" s="157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15">
+      <c r="A7" s="19"/>
+      <c r="B7" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="157">
+        <v>83</v>
+      </c>
+      <c r="D7" s="157">
+        <v>677</v>
+      </c>
+      <c r="E7" s="157" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G7" s="25">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="H7" s="25">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="I7" s="157">
+        <v>0</v>
+      </c>
+      <c r="J7" s="157">
+        <v>0</v>
+      </c>
+      <c r="K7" s="157">
+        <v>1</v>
+      </c>
+      <c r="L7" s="157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="157">
+        <v>69</v>
+      </c>
+      <c r="D8" s="157">
+        <v>839</v>
+      </c>
+      <c r="E8" s="157" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="24">
+        <v>42657</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="I8" s="157">
+        <v>0</v>
+      </c>
+      <c r="J8" s="157">
+        <v>0</v>
+      </c>
+      <c r="K8" s="157">
+        <v>2</v>
+      </c>
+      <c r="L8" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="157">
+        <v>61</v>
+      </c>
+      <c r="D9" s="157">
+        <v>693</v>
+      </c>
+      <c r="E9" s="157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I9" s="157">
+        <v>0</v>
+      </c>
+      <c r="J9" s="157">
+        <v>0</v>
+      </c>
+      <c r="K9" s="157">
+        <v>0</v>
+      </c>
+      <c r="L9" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="157">
+        <v>59</v>
+      </c>
+      <c r="D10" s="157">
+        <v>344</v>
+      </c>
+      <c r="E10" s="157">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I10" s="157">
+        <v>0</v>
+      </c>
+      <c r="J10" s="157">
+        <v>0</v>
+      </c>
+      <c r="K10" s="157">
+        <v>0</v>
+      </c>
+      <c r="L10" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="157">
+        <v>44</v>
+      </c>
+      <c r="D11" s="157">
+        <v>573</v>
+      </c>
+      <c r="E11" s="157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="24">
+        <v>42676</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0.86099999999999999</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0.86399999999999999</v>
+      </c>
+      <c r="I11" s="157">
+        <v>0</v>
+      </c>
+      <c r="J11" s="157">
+        <v>0</v>
+      </c>
+      <c r="K11" s="157">
+        <v>1</v>
+      </c>
+      <c r="L11" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="157">
+        <v>41</v>
+      </c>
+      <c r="D12" s="157">
+        <v>567</v>
+      </c>
+      <c r="E12" s="157" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="24">
+        <v>42676</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="H12" s="25">
+        <v>0.85</v>
+      </c>
+      <c r="I12" s="157">
+        <v>0</v>
+      </c>
+      <c r="J12" s="157">
+        <v>0</v>
+      </c>
+      <c r="K12" s="157">
+        <v>1</v>
+      </c>
+      <c r="L12" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="157">
+        <v>36</v>
+      </c>
+      <c r="D13" s="157">
+        <v>195</v>
+      </c>
+      <c r="E13" s="157">
+        <v>0</v>
+      </c>
+      <c r="F13" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H13" s="25">
+        <v>1</v>
+      </c>
+      <c r="I13" s="157">
+        <v>0</v>
+      </c>
+      <c r="J13" s="157">
+        <v>0</v>
+      </c>
+      <c r="K13" s="157">
+        <v>0</v>
+      </c>
+      <c r="L13" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="157">
+        <v>31</v>
+      </c>
+      <c r="D14" s="157">
+        <v>378</v>
+      </c>
+      <c r="E14" s="157" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="I14" s="157">
+        <v>0</v>
+      </c>
+      <c r="J14" s="157">
+        <v>0</v>
+      </c>
+      <c r="K14" s="157">
+        <v>1</v>
+      </c>
+      <c r="L14" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="157">
+        <v>20</v>
+      </c>
+      <c r="D15" s="157">
+        <v>179</v>
+      </c>
+      <c r="E15" s="157">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="I15" s="157">
+        <v>0</v>
+      </c>
+      <c r="J15" s="157">
+        <v>0</v>
+      </c>
+      <c r="K15" s="157">
+        <v>0</v>
+      </c>
+      <c r="L15" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="157">
+        <v>13</v>
+      </c>
+      <c r="D16" s="157">
+        <v>218</v>
+      </c>
+      <c r="E16" s="157">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0.99099999999999999</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="I16" s="157">
+        <v>0</v>
+      </c>
+      <c r="J16" s="157">
+        <v>0</v>
+      </c>
+      <c r="K16" s="157">
+        <v>0</v>
+      </c>
+      <c r="L16" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="23">
+        <v>3041</v>
+      </c>
+      <c r="E17" s="157">
+        <v>0</v>
+      </c>
+      <c r="F17" s="24">
+        <v>42578</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="H17" s="25">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="I17" s="157">
+        <v>0</v>
+      </c>
+      <c r="J17" s="157">
+        <v>0</v>
+      </c>
+      <c r="K17" s="157">
+        <v>0</v>
+      </c>
+      <c r="L17" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15">
+      <c r="A18" s="20"/>
+      <c r="B18" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="23">
+        <v>10687</v>
+      </c>
+      <c r="E18" s="157" t="s">
+        <v>359</v>
+      </c>
+      <c r="F18" s="24">
+        <v>42684</v>
+      </c>
+      <c r="G18" s="25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="31"/>
+      <c r="I18" s="157">
+        <v>0</v>
+      </c>
+      <c r="J18" s="157">
+        <v>0</v>
+      </c>
+      <c r="K18" s="157">
+        <v>2</v>
+      </c>
+      <c r="L18" s="157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="158" t="s">
+        <v>357</v>
+      </c>
+      <c r="B19" s="158"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="158"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:L19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
+    <hyperlink ref="B1" tooltip="Name" display="Name"/>
+    <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
+    <hyperlink ref="D1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="E1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="F1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="G1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="H1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="I1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="J1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="K1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="L1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="svb-service-ooba"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="mur-java-lib-httpclient"/>
+    <hyperlink ref="B6" r:id="rId5" tooltip="svb-scheduler-payments"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="mur-java-lib-auth"/>
+    <hyperlink ref="B8" r:id="rId7" tooltip="svb-service-accounts"/>
+    <hyperlink ref="B9" r:id="rId8" tooltip="svb-service-csrf"/>
+    <hyperlink ref="B10" r:id="rId9" tooltip="mur-java-lib-dbconnector"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="svb-service-client"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="svb-service-bankinfo"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="mur-java-lib-logger"/>
+    <hyperlink ref="B14" r:id="rId13" tooltip="mur-java-lib-monitoring"/>
+    <hyperlink ref="B15" r:id="rId14" tooltip="mur-java-lib-exception"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="mur-java-lib-mappers"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="svb-web-core-ui"/>
+    <hyperlink ref="B18" r:id="rId17" tooltip="svb-web-payment"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
@@ -38964,20 +39706,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="157"/>
-      <c r="C15" s="157"/>
-      <c r="D15" s="157"/>
-      <c r="E15" s="157"/>
-      <c r="F15" s="157"/>
-      <c r="G15" s="157"/>
-      <c r="H15" s="157"/>
-      <c r="I15" s="157"/>
-      <c r="J15" s="157"/>
-      <c r="K15" s="157"/>
-      <c r="L15" s="157"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="158"/>
+      <c r="H15" s="158"/>
+      <c r="I15" s="158"/>
+      <c r="J15" s="158"/>
+      <c r="K15" s="158"/>
+      <c r="L15" s="158"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -39182,18 +39924,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="157"/>
-      <c r="B40" s="157"/>
-      <c r="C40" s="157"/>
-      <c r="D40" s="157"/>
-      <c r="E40" s="157"/>
-      <c r="F40" s="157"/>
-      <c r="G40" s="157"/>
-      <c r="H40" s="157"/>
-      <c r="I40" s="157"/>
-      <c r="J40" s="157"/>
-      <c r="K40" s="157"/>
-      <c r="L40" s="157"/>
+      <c r="A40" s="158"/>
+      <c r="B40" s="158"/>
+      <c r="C40" s="158"/>
+      <c r="D40" s="158"/>
+      <c r="E40" s="158"/>
+      <c r="F40" s="158"/>
+      <c r="G40" s="158"/>
+      <c r="H40" s="158"/>
+      <c r="I40" s="158"/>
+      <c r="J40" s="158"/>
+      <c r="K40" s="158"/>
+      <c r="L40" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -39827,20 +40569,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -40444,20 +41186,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -41067,20 +41809,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -41302,13 +42044,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="158" t="s">
+      <c r="U4" s="159" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="161"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -41345,9 +42087,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="161"/>
-      <c r="V5" s="162"/>
-      <c r="W5" s="162"/>
+      <c r="U5" s="162"/>
+      <c r="V5" s="163"/>
+      <c r="W5" s="163"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -41937,20 +42679,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -42731,20 +43473,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="158" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="157"/>
-      <c r="C16" s="157"/>
-      <c r="D16" s="157"/>
-      <c r="E16" s="157"/>
-      <c r="F16" s="157"/>
-      <c r="G16" s="157"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="157"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="157"/>
-      <c r="L16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="158"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="158"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
11/28/16 general roundup of recent work
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31000" yWindow="1420" windowWidth="23980" windowHeight="13160" tabRatio="559" firstSheet="23" activeTab="33"/>
+    <workbookView xWindow="-580" yWindow="120" windowWidth="27380" windowHeight="16440" tabRatio="498" firstSheet="24" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="30">'10.18'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="31">'10.28'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
-    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="33">'11.14'!$A$1:$L$19</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="33">'11.14'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="9">'3.25'!$A$1:$L$16</definedName>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2671" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="367">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1295,6 +1295,27 @@
   <si>
     <t xml:space="preserve">1h 15min </t>
   </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Auto E2E</t>
+  </si>
+  <si>
+    <t>Service AIP</t>
+  </si>
+  <si>
+    <t>Unit Test</t>
+  </si>
+  <si>
+    <t>2016-20</t>
+  </si>
+  <si>
+    <t>2016-21</t>
+  </si>
+  <si>
+    <t>2016-22</t>
+  </si>
 </sst>
 </file>
 
@@ -1850,7 +1871,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="76">
+  <cellStyleXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1927,8 +1948,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2248,6 +2271,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2268,8 +2294,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="76">
+  <cellStyles count="78">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2344,12 +2374,717 @@
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10.28'!$Q$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10.28'!$R$52:$V$52</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10.28'!$R$56:$V$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1216.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1231.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1714.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10.28'!$Q$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Service AIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10.28'!$R$52:$V$52</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10.28'!$R$55:$V$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>239.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>246.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10.28'!$Q$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Auto E2E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10.28'!$R$52:$V$52</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10.28'!$R$54:$V$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'10.28'!$Q$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'10.28'!$R$52:$V$52</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'10.28'!$R$53:$V$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2144292520"/>
+        <c:axId val="2144087144"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="2144292520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2144087144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2144087144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2144292520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0891374023452548"/>
+          <c:y val="0.0277777777777778"/>
+          <c:w val="0.729413840393238"/>
+          <c:h val="0.822469378827647"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$52</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$52:$W$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1216.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1231.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1714.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2010.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2015.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2131.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Service AIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$51:$W$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>232.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>239.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>246.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$50</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Auto E2E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$50:$W$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>117.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>139.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>176.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>203.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$49</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16-Mar</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16-Apr</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16-Sep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2016-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016-21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2016-22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$49:$W$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>163.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>218.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>219.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>223.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2146090136"/>
+        <c:axId val="2146333752"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="2146090136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146333752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2146333752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2146090136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.855586605469453"/>
+          <c:y val="0.314047098279382"/>
+          <c:w val="0.125214262600737"/>
+          <c:h val="0.371905803441236"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2444,8 +3179,78 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>374650</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2489,7 +3294,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2541,11 +3346,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8638,13 +9443,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -8681,9 +9486,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -9265,20 +10070,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -9741,13 +10546,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -9784,9 +10589,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10368,20 +11173,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10576,13 +11381,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="159" t="s">
+      <c r="U25" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="160"/>
-      <c r="W25" s="160"/>
-      <c r="X25" s="160"/>
-      <c r="Y25" s="161"/>
+      <c r="V25" s="161"/>
+      <c r="W25" s="161"/>
+      <c r="X25" s="161"/>
+      <c r="Y25" s="162"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -10595,9 +11400,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="162"/>
-      <c r="V26" s="163"/>
-      <c r="W26" s="163"/>
+      <c r="U26" s="163"/>
+      <c r="V26" s="164"/>
+      <c r="W26" s="164"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -10991,13 +11796,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -11034,9 +11839,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11626,20 +12431,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12162,13 +12967,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -12205,9 +13010,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12808,20 +13613,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -13366,13 +14171,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -13409,9 +14214,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -14022,20 +14827,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14572,13 +15377,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -14615,9 +15420,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -15228,20 +16033,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15778,13 +16583,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15821,9 +16626,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16434,20 +17239,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16984,13 +17789,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -17027,9 +17832,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17640,20 +18445,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18193,13 +18998,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -18236,9 +19041,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18852,20 +19657,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -19342,13 +20147,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19385,9 +20190,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -20001,20 +20806,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21156,13 +21961,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -21199,9 +22004,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -21815,20 +22620,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -22918,20 +23723,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -24014,20 +24819,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="159" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="159"/>
+      <c r="I15" s="159"/>
+      <c r="J15" s="159"/>
+      <c r="K15" s="159"/>
+      <c r="L15" s="159"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -26008,21 +26813,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
-      <c r="M16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
+      <c r="M16" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -26886,21 +27691,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
-      <c r="M16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
+      <c r="M16" s="159"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -27781,20 +28586,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -29233,20 +30038,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -30280,20 +31085,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="158" t="s">
+      <c r="A17" s="159" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="158"/>
-      <c r="C17" s="158"/>
-      <c r="D17" s="158"/>
-      <c r="E17" s="158"/>
-      <c r="F17" s="158"/>
-      <c r="G17" s="158"/>
-      <c r="H17" s="158"/>
-      <c r="I17" s="158"/>
-      <c r="J17" s="158"/>
-      <c r="K17" s="158"/>
-      <c r="L17" s="158"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="159"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="159"/>
+      <c r="I17" s="159"/>
+      <c r="J17" s="159"/>
+      <c r="K17" s="159"/>
+      <c r="L17" s="159"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -30304,13 +31109,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="164" t="s">
+      <c r="O19" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="165"/>
-      <c r="Q19" s="165"/>
-      <c r="R19" s="165"/>
-      <c r="S19" s="166"/>
+      <c r="P19" s="166"/>
+      <c r="Q19" s="166"/>
+      <c r="R19" s="166"/>
+      <c r="S19" s="167"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -31400,34 +32205,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="158" t="s">
+      <c r="A18" s="159" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="158"/>
-      <c r="C18" s="158"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="158"/>
-      <c r="G18" s="158"/>
-      <c r="H18" s="158"/>
-      <c r="I18" s="158"/>
-      <c r="J18" s="158"/>
-      <c r="K18" s="158"/>
-      <c r="L18" s="158"/>
-      <c r="M18" s="158"/>
-      <c r="N18" s="158"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="159"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
+      <c r="L18" s="159"/>
+      <c r="M18" s="159"/>
+      <c r="N18" s="159"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="164" t="s">
+      <c r="Q19" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="165"/>
-      <c r="S19" s="165"/>
-      <c r="T19" s="165"/>
-      <c r="U19" s="166"/>
+      <c r="R19" s="166"/>
+      <c r="S19" s="166"/>
+      <c r="T19" s="166"/>
+      <c r="U19" s="167"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -32306,7 +33111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U172"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
@@ -33277,13 +34082,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="164" t="s">
+      <c r="Q22" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="165"/>
-      <c r="S22" s="165"/>
-      <c r="T22" s="165"/>
-      <c r="U22" s="166"/>
+      <c r="R22" s="166"/>
+      <c r="S22" s="166"/>
+      <c r="T22" s="166"/>
+      <c r="U22" s="167"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -33980,7 +34785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -34969,22 +35774,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="158" t="s">
+      <c r="A19" s="159" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="158"/>
-      <c r="N19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="159"/>
+      <c r="N19" s="159"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -34997,13 +35802,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="164" t="s">
+      <c r="Q22" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="165"/>
-      <c r="S22" s="165"/>
-      <c r="T22" s="165"/>
-      <c r="U22" s="166"/>
+      <c r="R22" s="166"/>
+      <c r="S22" s="166"/>
+      <c r="T22" s="166"/>
+      <c r="U22" s="167"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -35321,10 +36126,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+    <sheetView topLeftCell="N43" workbookViewId="0">
+      <selection activeCell="Y64" sqref="Y64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -36264,22 +37069,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="158" t="s">
+      <c r="A19" s="159" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="158"/>
-      <c r="N19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="159"/>
+      <c r="N19" s="159"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -36292,13 +37097,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="164" t="s">
+      <c r="Q22" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="165"/>
-      <c r="S22" s="165"/>
-      <c r="T22" s="165"/>
-      <c r="U22" s="166"/>
+      <c r="R22" s="166"/>
+      <c r="S22" s="166"/>
+      <c r="T22" s="166"/>
+      <c r="U22" s="167"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -36603,22 +37408,120 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="6:6">
+    <row r="49" spans="6:23">
       <c r="F49">
         <f t="shared" ref="F49:F51" si="3">C14</f>
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="6:6">
+    <row r="50" spans="6:23">
       <c r="F50">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="6:6">
+    <row r="51" spans="6:23">
       <c r="F51">
         <f t="shared" si="3"/>
         <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="6:23">
+      <c r="R52" s="169">
+        <v>42445</v>
+      </c>
+      <c r="S52" s="169">
+        <v>42476</v>
+      </c>
+      <c r="T52" s="169">
+        <v>42629</v>
+      </c>
+      <c r="U52" s="62" t="s">
+        <v>364</v>
+      </c>
+      <c r="V52" s="62" t="s">
+        <v>365</v>
+      </c>
+      <c r="W52" s="62"/>
+    </row>
+    <row r="53" spans="6:23">
+      <c r="Q53" t="s">
+        <v>360</v>
+      </c>
+      <c r="R53">
+        <v>163</v>
+      </c>
+      <c r="S53">
+        <v>163</v>
+      </c>
+      <c r="T53">
+        <v>218</v>
+      </c>
+      <c r="U53">
+        <v>219</v>
+      </c>
+      <c r="V53">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="6:23">
+      <c r="Q54" t="s">
+        <v>361</v>
+      </c>
+      <c r="R54">
+        <v>117</v>
+      </c>
+      <c r="S54">
+        <v>139</v>
+      </c>
+      <c r="T54">
+        <v>134</v>
+      </c>
+      <c r="U54">
+        <v>176</v>
+      </c>
+      <c r="V54">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="6:23">
+      <c r="Q55" t="s">
+        <v>362</v>
+      </c>
+      <c r="R55">
+        <v>218</v>
+      </c>
+      <c r="S55">
+        <v>223</v>
+      </c>
+      <c r="T55">
+        <v>232</v>
+      </c>
+      <c r="U55">
+        <v>239</v>
+      </c>
+      <c r="V55">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="56" spans="6:23">
+      <c r="Q56" t="s">
+        <v>363</v>
+      </c>
+      <c r="R56">
+        <v>1216</v>
+      </c>
+      <c r="S56">
+        <v>1231</v>
+      </c>
+      <c r="T56">
+        <v>1714</v>
+      </c>
+      <c r="U56">
+        <v>2010</v>
+      </c>
+      <c r="V56">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>
@@ -36658,9 +37561,11 @@
     <hyperlink ref="B18" r:id="rId17" tooltip="svb-web-payment"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
     <ignoredError sqref="T5:T16 S13:S19 U15 U32" emptyCellReference="1"/>
   </ignoredErrors>
+  <drawing r:id="rId18"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -37547,24 +38452,24 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="158" t="s">
+      <c r="A19" s="159" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="158"/>
-      <c r="N19" s="158"/>
-      <c r="O19" s="158"/>
-      <c r="P19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="159"/>
+      <c r="N19" s="159"/>
+      <c r="O19" s="159"/>
+      <c r="P19" s="159"/>
     </row>
     <row r="23" spans="1:16" ht="60">
       <c r="A23" s="18" t="s">
@@ -38365,20 +39270,20 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="158" t="s">
+      <c r="A43" s="159" t="s">
         <v>357</v>
       </c>
-      <c r="B43" s="158"/>
-      <c r="C43" s="158"/>
-      <c r="D43" s="158"/>
-      <c r="E43" s="158"/>
-      <c r="F43" s="158"/>
-      <c r="G43" s="158"/>
-      <c r="H43" s="158"/>
-      <c r="I43" s="158"/>
-      <c r="J43" s="158"/>
-      <c r="K43" s="158"/>
-      <c r="L43" s="158"/>
+      <c r="B43" s="159"/>
+      <c r="C43" s="159"/>
+      <c r="D43" s="159"/>
+      <c r="E43" s="159"/>
+      <c r="F43" s="159"/>
+      <c r="G43" s="159"/>
+      <c r="H43" s="159"/>
+      <c r="I43" s="159"/>
+      <c r="J43" s="159"/>
+      <c r="K43" s="159"/>
+      <c r="L43" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -38458,28 +39363,37 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
+      <selection activeCell="R45" sqref="R45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="4.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="5.5" customWidth="1"/>
+    <col min="17" max="17" width="20.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="13.83203125" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="168"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45">
+    <row r="1" spans="1:21" ht="45">
       <c r="A1" s="18" t="s">
         <v>103</v>
       </c>
@@ -38489,35 +39403,51 @@
       <c r="C1" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15">
+      <c r="Q1" s="152" t="s">
+        <v>348</v>
+      </c>
+      <c r="R1" s="152" t="s">
+        <v>349</v>
+      </c>
+      <c r="S1" s="59" t="str">
+        <f>C1</f>
+        <v xml:space="preserve">UTs </v>
+      </c>
+      <c r="T1" s="59">
+        <f>E1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>119</v>
@@ -38525,35 +39455,47 @@
       <c r="C2" s="157">
         <v>491</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="158"/>
+      <c r="E2" s="158">
+        <v>81</v>
+      </c>
+      <c r="F2" s="23">
         <v>5271</v>
       </c>
-      <c r="E2" s="157" t="s">
+      <c r="G2" s="157" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="24">
+      <c r="H2" s="24">
         <v>42684</v>
       </c>
-      <c r="G2" s="25">
+      <c r="I2" s="25">
         <v>0.92</v>
       </c>
-      <c r="H2" s="25">
+      <c r="J2" s="25">
         <v>0.91300000000000003</v>
       </c>
-      <c r="I2" s="157">
-        <v>0</v>
-      </c>
-      <c r="J2" s="157">
-        <v>0</v>
-      </c>
       <c r="K2" s="157">
+        <v>0</v>
+      </c>
+      <c r="L2" s="157">
+        <v>0</v>
+      </c>
+      <c r="M2" s="157">
         <v>2</v>
       </c>
-      <c r="L2" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15">
+      <c r="N2" s="157">
+        <v>0</v>
+      </c>
+      <c r="S2" s="59">
+        <f t="shared" ref="S2:S18" si="0">C2-E2</f>
+        <v>410</v>
+      </c>
+      <c r="T2" s="59">
+        <f t="shared" ref="T2:T16" si="1">E2</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15">
       <c r="A3" s="20"/>
       <c r="B3" s="22" t="s">
         <v>117</v>
@@ -38561,35 +39503,53 @@
       <c r="C3" s="157">
         <v>210</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="158"/>
+      <c r="E3" s="158">
+        <v>40</v>
+      </c>
+      <c r="F3" s="23">
         <v>1879</v>
       </c>
-      <c r="E3" s="157" t="s">
+      <c r="G3" s="157" t="s">
         <v>129</v>
       </c>
-      <c r="F3" s="24">
+      <c r="H3" s="24">
         <v>42682</v>
       </c>
-      <c r="G3" s="25">
+      <c r="I3" s="25">
         <v>0.93700000000000006</v>
       </c>
-      <c r="H3" s="25">
+      <c r="J3" s="25">
         <v>0.92600000000000005</v>
       </c>
-      <c r="I3" s="157">
-        <v>0</v>
-      </c>
-      <c r="J3" s="157">
-        <v>0</v>
-      </c>
       <c r="K3" s="157">
+        <v>0</v>
+      </c>
+      <c r="L3" s="157">
+        <v>0</v>
+      </c>
+      <c r="M3" s="157">
         <v>2</v>
       </c>
-      <c r="L3" s="157">
+      <c r="N3" s="157">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15">
+      <c r="Q3" t="s">
+        <v>265</v>
+      </c>
+      <c r="R3">
+        <v>15</v>
+      </c>
+      <c r="S3" s="59">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="T3" s="59">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15">
       <c r="A4" s="19"/>
       <c r="B4" s="22" t="s">
         <v>329</v>
@@ -38597,35 +39557,53 @@
       <c r="C4" s="157">
         <v>181</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="158"/>
+      <c r="E4" s="158">
+        <v>43</v>
+      </c>
+      <c r="F4" s="23">
         <v>2270</v>
       </c>
-      <c r="E4" s="157" t="s">
+      <c r="G4" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="24">
+      <c r="H4" s="24">
         <v>42684</v>
       </c>
-      <c r="G4" s="25">
+      <c r="I4" s="25">
         <v>0.91800000000000004</v>
       </c>
-      <c r="H4" s="25">
+      <c r="J4" s="25">
         <v>0.83099999999999996</v>
       </c>
-      <c r="I4" s="157">
-        <v>0</v>
-      </c>
-      <c r="J4" s="157">
-        <v>0</v>
-      </c>
       <c r="K4" s="157">
+        <v>0</v>
+      </c>
+      <c r="L4" s="157">
+        <v>0</v>
+      </c>
+      <c r="M4" s="157">
         <v>1</v>
       </c>
-      <c r="L4" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15">
+      <c r="N4" s="157">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>258</v>
+      </c>
+      <c r="R4">
+        <v>153</v>
+      </c>
+      <c r="S4" s="59">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="T4" s="59">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15">
       <c r="A5" s="20"/>
       <c r="B5" s="22" t="s">
         <v>128</v>
@@ -38633,35 +39611,51 @@
       <c r="C5" s="157">
         <v>133</v>
       </c>
-      <c r="D5" s="157">
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="157">
         <v>892</v>
       </c>
-      <c r="E5" s="157" t="s">
+      <c r="G5" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="F5" s="24">
+      <c r="H5" s="24">
         <v>42684</v>
       </c>
-      <c r="G5" s="25">
+      <c r="I5" s="25">
         <v>0.94799999999999995</v>
       </c>
-      <c r="H5" s="25">
+      <c r="J5" s="25">
         <v>0.91</v>
       </c>
-      <c r="I5" s="157">
-        <v>0</v>
-      </c>
-      <c r="J5" s="157">
-        <v>0</v>
-      </c>
       <c r="K5" s="157">
+        <v>0</v>
+      </c>
+      <c r="L5" s="157">
+        <v>0</v>
+      </c>
+      <c r="M5" s="157">
         <v>1</v>
       </c>
-      <c r="L5" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15">
+      <c r="N5" s="157">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>259</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5" s="59">
+        <f t="shared" si="0"/>
+        <v>133</v>
+      </c>
+      <c r="T5" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15">
       <c r="A6" s="20"/>
       <c r="B6" s="22" t="s">
         <v>114</v>
@@ -38669,35 +39663,51 @@
       <c r="C6" s="157">
         <v>114</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="158"/>
+      <c r="E6" s="158"/>
+      <c r="F6" s="23">
         <v>1638</v>
       </c>
-      <c r="E6" s="157" t="s">
+      <c r="G6" s="157" t="s">
         <v>355</v>
       </c>
-      <c r="F6" s="24">
+      <c r="H6" s="24">
         <v>42676</v>
       </c>
-      <c r="G6" s="25">
+      <c r="I6" s="25">
         <v>0.95699999999999996</v>
       </c>
-      <c r="H6" s="25">
+      <c r="J6" s="25">
         <v>0.94199999999999995</v>
       </c>
-      <c r="I6" s="157">
-        <v>0</v>
-      </c>
-      <c r="J6" s="157">
-        <v>0</v>
-      </c>
       <c r="K6" s="157">
+        <v>0</v>
+      </c>
+      <c r="L6" s="157">
+        <v>0</v>
+      </c>
+      <c r="M6" s="157">
         <v>2</v>
       </c>
-      <c r="L6" s="157">
+      <c r="N6" s="157">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15">
+      <c r="Q6" t="s">
+        <v>260</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" s="59">
+        <f t="shared" si="0"/>
+        <v>114</v>
+      </c>
+      <c r="T6" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15">
       <c r="A7" s="19"/>
       <c r="B7" s="22" t="s">
         <v>133</v>
@@ -38705,35 +39715,51 @@
       <c r="C7" s="157">
         <v>83</v>
       </c>
-      <c r="D7" s="157">
+      <c r="D7" s="158"/>
+      <c r="E7" s="158"/>
+      <c r="F7" s="157">
         <v>677</v>
       </c>
-      <c r="E7" s="157" t="s">
+      <c r="G7" s="157" t="s">
         <v>351</v>
       </c>
-      <c r="F7" s="24">
+      <c r="H7" s="24">
         <v>42684</v>
       </c>
-      <c r="G7" s="25">
+      <c r="I7" s="25">
         <v>0.96699999999999997</v>
       </c>
-      <c r="H7" s="25">
+      <c r="J7" s="25">
         <v>0.94599999999999995</v>
       </c>
-      <c r="I7" s="157">
-        <v>0</v>
-      </c>
-      <c r="J7" s="157">
-        <v>0</v>
-      </c>
       <c r="K7" s="157">
+        <v>0</v>
+      </c>
+      <c r="L7" s="157">
+        <v>0</v>
+      </c>
+      <c r="M7" s="157">
         <v>1</v>
       </c>
-      <c r="L7" s="157">
+      <c r="N7" s="157">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15">
+      <c r="Q7" t="s">
+        <v>268</v>
+      </c>
+      <c r="R7">
+        <v>11</v>
+      </c>
+      <c r="S7" s="59">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="T7" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15">
       <c r="A8" s="20"/>
       <c r="B8" s="22" t="s">
         <v>123</v>
@@ -38741,35 +39767,53 @@
       <c r="C8" s="157">
         <v>69</v>
       </c>
-      <c r="D8" s="157">
+      <c r="D8" s="158"/>
+      <c r="E8" s="158">
+        <v>16</v>
+      </c>
+      <c r="F8" s="157">
         <v>839</v>
       </c>
-      <c r="E8" s="157" t="s">
+      <c r="G8" s="157" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="24">
+      <c r="H8" s="24">
         <v>42657</v>
       </c>
-      <c r="G8" s="25">
+      <c r="I8" s="25">
         <v>0.90300000000000002</v>
       </c>
-      <c r="H8" s="25">
+      <c r="J8" s="25">
         <v>0.82399999999999995</v>
       </c>
-      <c r="I8" s="157">
-        <v>0</v>
-      </c>
-      <c r="J8" s="157">
-        <v>0</v>
-      </c>
       <c r="K8" s="157">
+        <v>0</v>
+      </c>
+      <c r="L8" s="157">
+        <v>0</v>
+      </c>
+      <c r="M8" s="157">
         <v>2</v>
       </c>
-      <c r="L8" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15">
+      <c r="N8" s="157">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>262</v>
+      </c>
+      <c r="R8">
+        <v>27</v>
+      </c>
+      <c r="S8" s="59">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="T8" s="59">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15">
       <c r="A9" s="20"/>
       <c r="B9" s="22" t="s">
         <v>139</v>
@@ -38777,35 +39821,53 @@
       <c r="C9" s="157">
         <v>61</v>
       </c>
-      <c r="D9" s="157">
+      <c r="D9" s="158"/>
+      <c r="E9" s="158">
+        <v>11</v>
+      </c>
+      <c r="F9" s="157">
         <v>693</v>
       </c>
-      <c r="E9" s="157" t="s">
+      <c r="G9" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="24">
+      <c r="H9" s="24">
         <v>42684</v>
       </c>
-      <c r="G9" s="25">
+      <c r="I9" s="25">
         <v>0.91600000000000004</v>
       </c>
-      <c r="H9" s="25">
+      <c r="J9" s="25">
         <v>0.94399999999999995</v>
       </c>
-      <c r="I9" s="157">
-        <v>0</v>
-      </c>
-      <c r="J9" s="157">
-        <v>0</v>
-      </c>
       <c r="K9" s="157">
         <v>0</v>
       </c>
       <c r="L9" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15">
+      <c r="M9" s="157">
+        <v>0</v>
+      </c>
+      <c r="N9" s="157">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>263</v>
+      </c>
+      <c r="R9">
+        <v>10</v>
+      </c>
+      <c r="S9" s="59">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="T9" s="59">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15">
       <c r="A10" s="20"/>
       <c r="B10" s="22" t="s">
         <v>127</v>
@@ -38813,35 +39875,51 @@
       <c r="C10" s="157">
         <v>59</v>
       </c>
-      <c r="D10" s="157">
+      <c r="D10" s="158"/>
+      <c r="E10" s="158"/>
+      <c r="F10" s="157">
         <v>344</v>
       </c>
-      <c r="E10" s="157">
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
+      <c r="G10" s="157">
+        <v>0</v>
+      </c>
+      <c r="H10" s="24">
         <v>42684</v>
       </c>
-      <c r="G10" s="25">
+      <c r="I10" s="25">
         <v>0.92200000000000004</v>
       </c>
-      <c r="H10" s="25">
+      <c r="J10" s="25">
         <v>0.97699999999999998</v>
       </c>
-      <c r="I10" s="157">
-        <v>0</v>
-      </c>
-      <c r="J10" s="157">
-        <v>0</v>
-      </c>
       <c r="K10" s="157">
         <v>0</v>
       </c>
       <c r="L10" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15">
+      <c r="M10" s="157">
+        <v>0</v>
+      </c>
+      <c r="N10" s="157">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>264</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="59">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="T10" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15">
       <c r="A11" s="20"/>
       <c r="B11" s="22" t="s">
         <v>292</v>
@@ -38849,35 +39927,47 @@
       <c r="C11" s="157">
         <v>44</v>
       </c>
-      <c r="D11" s="157">
+      <c r="D11" s="158"/>
+      <c r="E11" s="158">
+        <v>5</v>
+      </c>
+      <c r="F11" s="157">
         <v>573</v>
       </c>
-      <c r="E11" s="157" t="s">
+      <c r="G11" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="24">
+      <c r="H11" s="24">
         <v>42676</v>
       </c>
-      <c r="G11" s="25">
+      <c r="I11" s="25">
         <v>0.86099999999999999</v>
       </c>
-      <c r="H11" s="25">
+      <c r="J11" s="25">
         <v>0.86399999999999999</v>
       </c>
-      <c r="I11" s="157">
-        <v>0</v>
-      </c>
-      <c r="J11" s="157">
-        <v>0</v>
-      </c>
       <c r="K11" s="157">
+        <v>0</v>
+      </c>
+      <c r="L11" s="157">
+        <v>0</v>
+      </c>
+      <c r="M11" s="157">
         <v>1</v>
       </c>
-      <c r="L11" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15">
+      <c r="N11" s="157">
+        <v>0</v>
+      </c>
+      <c r="S11" s="59">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="T11" s="59">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15">
       <c r="A12" s="20"/>
       <c r="B12" s="22" t="s">
         <v>336</v>
@@ -38885,35 +39975,47 @@
       <c r="C12" s="157">
         <v>41</v>
       </c>
-      <c r="D12" s="157">
+      <c r="D12" s="158"/>
+      <c r="E12" s="158">
+        <v>4</v>
+      </c>
+      <c r="F12" s="157">
         <v>567</v>
       </c>
-      <c r="E12" s="157" t="s">
+      <c r="G12" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="24">
+      <c r="H12" s="24">
         <v>42676</v>
       </c>
-      <c r="G12" s="25">
+      <c r="I12" s="25">
         <v>0.89800000000000002</v>
       </c>
-      <c r="H12" s="25">
+      <c r="J12" s="25">
         <v>0.85</v>
       </c>
-      <c r="I12" s="157">
-        <v>0</v>
-      </c>
-      <c r="J12" s="157">
-        <v>0</v>
-      </c>
       <c r="K12" s="157">
+        <v>0</v>
+      </c>
+      <c r="L12" s="157">
+        <v>0</v>
+      </c>
+      <c r="M12" s="157">
         <v>1</v>
       </c>
-      <c r="L12" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15">
+      <c r="N12" s="157">
+        <v>0</v>
+      </c>
+      <c r="S12" s="59">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="T12" s="59">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15">
       <c r="A13" s="20"/>
       <c r="B13" s="22" t="s">
         <v>126</v>
@@ -38921,35 +40023,45 @@
       <c r="C13" s="157">
         <v>36</v>
       </c>
-      <c r="D13" s="157">
+      <c r="D13" s="158"/>
+      <c r="E13" s="158"/>
+      <c r="F13" s="157">
         <v>195</v>
       </c>
-      <c r="E13" s="157">
-        <v>0</v>
-      </c>
-      <c r="F13" s="24">
+      <c r="G13" s="157">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24">
         <v>42684</v>
       </c>
-      <c r="G13" s="25">
+      <c r="I13" s="25">
         <v>0.98599999999999999</v>
       </c>
-      <c r="H13" s="25">
+      <c r="J13" s="25">
         <v>1</v>
       </c>
-      <c r="I13" s="157">
-        <v>0</v>
-      </c>
-      <c r="J13" s="157">
-        <v>0</v>
-      </c>
       <c r="K13" s="157">
         <v>0</v>
       </c>
       <c r="L13" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15">
+      <c r="M13" s="157">
+        <v>0</v>
+      </c>
+      <c r="N13" s="157">
+        <v>0</v>
+      </c>
+      <c r="S13" s="59">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="T13" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15">
       <c r="A14" s="20"/>
       <c r="B14" s="22" t="s">
         <v>131</v>
@@ -38957,35 +40069,49 @@
       <c r="C14" s="157">
         <v>31</v>
       </c>
-      <c r="D14" s="157">
+      <c r="D14" s="158"/>
+      <c r="E14" s="158"/>
+      <c r="F14" s="157">
         <v>378</v>
       </c>
-      <c r="E14" s="157" t="s">
+      <c r="G14" s="157" t="s">
         <v>132</v>
       </c>
-      <c r="F14" s="24">
+      <c r="H14" s="24">
         <v>42684</v>
       </c>
-      <c r="G14" s="25">
+      <c r="I14" s="25">
         <v>0.77100000000000002</v>
       </c>
-      <c r="H14" s="25">
+      <c r="J14" s="25">
         <v>0.51700000000000002</v>
       </c>
-      <c r="I14" s="157">
-        <v>0</v>
-      </c>
-      <c r="J14" s="157">
-        <v>0</v>
-      </c>
       <c r="K14" s="157">
+        <v>0</v>
+      </c>
+      <c r="L14" s="157">
+        <v>0</v>
+      </c>
+      <c r="M14" s="157">
         <v>1</v>
       </c>
-      <c r="L14" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15">
+      <c r="N14" s="157">
+        <v>0</v>
+      </c>
+      <c r="S14" s="59">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="T14" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f>SUM(S2:S16)</f>
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15">
       <c r="A15" s="20"/>
       <c r="B15" s="22" t="s">
         <v>125</v>
@@ -38993,35 +40119,49 @@
       <c r="C15" s="157">
         <v>20</v>
       </c>
-      <c r="D15" s="157">
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="157">
         <v>179</v>
       </c>
-      <c r="E15" s="157">
-        <v>0</v>
-      </c>
-      <c r="F15" s="24">
+      <c r="G15" s="157">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24">
         <v>42684</v>
       </c>
-      <c r="G15" s="25">
+      <c r="I15" s="25">
         <v>0.93600000000000005</v>
       </c>
-      <c r="H15" s="25">
+      <c r="J15" s="25">
         <v>0.91700000000000004</v>
       </c>
-      <c r="I15" s="157">
-        <v>0</v>
-      </c>
-      <c r="J15" s="157">
-        <v>0</v>
-      </c>
       <c r="K15" s="157">
         <v>0</v>
       </c>
       <c r="L15" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15">
+      <c r="M15" s="157">
+        <v>0</v>
+      </c>
+      <c r="N15" s="157">
+        <v>0</v>
+      </c>
+      <c r="S15" s="59">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="T15" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>SUM(T2:T18)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15">
       <c r="A16" s="20"/>
       <c r="B16" s="22" t="s">
         <v>130</v>
@@ -39029,133 +40169,598 @@
       <c r="C16" s="157">
         <v>13</v>
       </c>
-      <c r="D16" s="157">
+      <c r="D16" s="158"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="157">
         <v>218</v>
       </c>
-      <c r="E16" s="157">
-        <v>0</v>
-      </c>
-      <c r="F16" s="24">
+      <c r="G16" s="157">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24">
         <v>42684</v>
       </c>
-      <c r="G16" s="25">
+      <c r="I16" s="25">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H16" s="25">
+      <c r="J16" s="25">
         <v>0.92900000000000005</v>
       </c>
-      <c r="I16" s="157">
-        <v>0</v>
-      </c>
-      <c r="J16" s="157">
-        <v>0</v>
-      </c>
       <c r="K16" s="157">
         <v>0</v>
       </c>
       <c r="L16" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="15">
+      <c r="M16" s="157">
+        <v>0</v>
+      </c>
+      <c r="N16" s="157">
+        <v>0</v>
+      </c>
+      <c r="S16" s="59">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="T16" s="59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>SUM(S17:S18)</f>
+        <v>745</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="15">
       <c r="A17" s="20"/>
       <c r="B17" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="23">
+      <c r="C17" s="31">
+        <v>231</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="23">
         <v>3041</v>
       </c>
-      <c r="E17" s="157">
-        <v>0</v>
-      </c>
-      <c r="F17" s="24">
+      <c r="G17" s="157">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24">
         <v>42578</v>
       </c>
-      <c r="G17" s="25">
+      <c r="I17" s="25">
         <v>0.91700000000000004</v>
       </c>
-      <c r="H17" s="25">
+      <c r="J17" s="25">
         <v>0.81599999999999995</v>
       </c>
-      <c r="I17" s="157">
-        <v>0</v>
-      </c>
-      <c r="J17" s="157">
-        <v>0</v>
-      </c>
       <c r="K17" s="157">
         <v>0</v>
       </c>
       <c r="L17" s="157">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="15">
+      <c r="M17" s="157">
+        <v>0</v>
+      </c>
+      <c r="N17" s="157">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>SUM(R3:R10)</f>
+        <v>223</v>
+      </c>
+      <c r="S17" s="59">
+        <f t="shared" si="0"/>
+        <v>231</v>
+      </c>
+      <c r="T17" s="59"/>
+    </row>
+    <row r="18" spans="1:24" ht="15">
       <c r="A18" s="20"/>
       <c r="B18" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="23">
+      <c r="C18" s="31">
+        <v>514</v>
+      </c>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="23">
         <v>10687</v>
       </c>
-      <c r="E18" s="157" t="s">
+      <c r="G18" s="157" t="s">
         <v>359</v>
       </c>
-      <c r="F18" s="24">
+      <c r="H18" s="24">
         <v>42684</v>
       </c>
-      <c r="G18" s="25">
-        <v>0</v>
-      </c>
-      <c r="H18" s="31"/>
-      <c r="I18" s="157">
-        <v>0</v>
-      </c>
-      <c r="J18" s="157">
-        <v>0</v>
-      </c>
+      <c r="I18" s="25">
+        <v>0</v>
+      </c>
+      <c r="J18" s="31"/>
       <c r="K18" s="157">
+        <v>0</v>
+      </c>
+      <c r="L18" s="157">
+        <v>0</v>
+      </c>
+      <c r="M18" s="157">
         <v>2</v>
       </c>
-      <c r="L18" s="157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="158" t="s">
+      <c r="N18" s="157">
+        <v>0</v>
+      </c>
+      <c r="S18" s="59">
+        <f t="shared" si="0"/>
+        <v>514</v>
+      </c>
+      <c r="T18" s="59"/>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="159" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="158"/>
-      <c r="C19" s="158"/>
-      <c r="D19" s="158"/>
-      <c r="E19" s="158"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="158"/>
-      <c r="H19" s="158"/>
-      <c r="I19" s="158"/>
-      <c r="J19" s="158"/>
-      <c r="K19" s="158"/>
-      <c r="L19" s="158"/>
+      <c r="B19" s="159"/>
+      <c r="C19" s="159"/>
+      <c r="D19" s="159"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="159"/>
+      <c r="N19" s="159"/>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="B20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" ht="15" thickBot="1">
+      <c r="B21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="15" thickBot="1">
+      <c r="Q22" s="165" t="s">
+        <v>164</v>
+      </c>
+      <c r="R22" s="166"/>
+      <c r="S22" s="166"/>
+      <c r="T22" s="166"/>
+      <c r="U22" s="167"/>
+      <c r="W22">
+        <v>223</v>
+      </c>
+      <c r="X22" s="168">
+        <f>W22/W$26</f>
+        <v>8.0885019949220163E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>113</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="J23" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q23" s="124"/>
+      <c r="R23" s="125"/>
+      <c r="S23" s="125"/>
+      <c r="T23" s="144" t="s">
+        <v>165</v>
+      </c>
+      <c r="U23" s="145" t="s">
+        <v>356</v>
+      </c>
+      <c r="W23">
+        <v>203</v>
+      </c>
+      <c r="X23" s="168">
+        <f t="shared" ref="X23:X26" si="2">W23/W$26</f>
+        <v>7.3630758070366342E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="I24" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q24" s="128"/>
+      <c r="R24" s="129"/>
+      <c r="S24" s="129"/>
+      <c r="T24" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="U24" s="146"/>
+      <c r="W24">
+        <v>200</v>
+      </c>
+      <c r="X24" s="168">
+        <f t="shared" si="2"/>
+        <v>7.2542618788538266E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="B25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25">
+        <v>491</v>
+      </c>
+      <c r="I25" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="J25" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q25" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="133"/>
+      <c r="S25" s="134"/>
+      <c r="T25" s="135">
+        <f>R17</f>
+        <v>223</v>
+      </c>
+      <c r="U25" s="147">
+        <f>T25/$T$32</f>
+        <v>8.0885019949220163E-2</v>
+      </c>
+      <c r="W25">
+        <v>2131</v>
+      </c>
+      <c r="X25" s="168">
+        <f t="shared" si="2"/>
+        <v>0.77294160319187522</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="I26" s="58"/>
+      <c r="Q26" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="R26" s="133" t="s">
+        <v>333</v>
+      </c>
+      <c r="S26" s="134" t="s">
+        <v>334</v>
+      </c>
+      <c r="T26" s="135">
+        <f>C34</f>
+        <v>203</v>
+      </c>
+      <c r="U26" s="147">
+        <f t="shared" ref="U26:U30" si="3">T26/$T$32</f>
+        <v>7.3630758070366342E-2</v>
+      </c>
+      <c r="W26">
+        <f>SUM(W22:W25)</f>
+        <v>2757</v>
+      </c>
+      <c r="X26" s="168">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="B27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C27" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q27" s="132"/>
+      <c r="R27" s="133" t="s">
+        <v>169</v>
+      </c>
+      <c r="S27" s="134"/>
+      <c r="T27" s="135">
+        <f>U15</f>
+        <v>200</v>
+      </c>
+      <c r="U27" s="147">
+        <f t="shared" si="3"/>
+        <v>7.2542618788538266E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="C28" t="s">
+        <v>279</v>
+      </c>
+      <c r="Q28" s="132"/>
+      <c r="R28" s="133" t="s">
+        <v>9</v>
+      </c>
+      <c r="S28" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T28" s="135">
+        <f>U14</f>
+        <v>1386</v>
+      </c>
+      <c r="U28" s="147">
+        <f t="shared" si="3"/>
+        <v>0.50272034820457023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="C29" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q29" s="132"/>
+      <c r="R29" s="133" t="s">
+        <v>331</v>
+      </c>
+      <c r="S29" s="134" t="s">
+        <v>170</v>
+      </c>
+      <c r="T29" s="135">
+        <v>0</v>
+      </c>
+      <c r="U29" s="147">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="C30" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q30" s="132"/>
+      <c r="R30" s="133"/>
+      <c r="S30" s="134" t="s">
+        <v>347</v>
+      </c>
+      <c r="T30" s="135">
+        <f>U16</f>
+        <v>745</v>
+      </c>
+      <c r="U30" s="147">
+        <f t="shared" si="3"/>
+        <v>0.27022125498730504</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q31" s="132"/>
+      <c r="R31" s="133"/>
+      <c r="S31" s="134"/>
+      <c r="T31" s="135"/>
+      <c r="U31" s="147"/>
+    </row>
+    <row r="32" spans="1:24" ht="15" thickBot="1">
+      <c r="Q32" s="137"/>
+      <c r="R32" s="138"/>
+      <c r="S32" s="139"/>
+      <c r="T32" s="140">
+        <f>SUM(T25:T30)</f>
+        <v>2757</v>
+      </c>
+      <c r="U32" s="148">
+        <f>SUM(U25:U31)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="B33" s="122" t="s">
+        <v>276</v>
+      </c>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="123" t="s">
+        <v>160</v>
+      </c>
+      <c r="J33" s="122" t="s">
+        <v>274</v>
+      </c>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="122"/>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="B34" t="s">
+        <v>339</v>
+      </c>
+      <c r="C34">
+        <v>203</v>
+      </c>
+      <c r="I34" s="59" t="s">
+        <v>160</v>
+      </c>
+      <c r="J34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36" s="62" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="A37" s="62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B37" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38" s="62"/>
+      <c r="B38" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
+      <c r="A39" s="62" t="s">
+        <v>344</v>
+      </c>
+      <c r="B39" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
+      <c r="A40" s="62" t="s">
+        <v>346</v>
+      </c>
+      <c r="B40" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
+      <c r="A41" s="62"/>
+    </row>
+    <row r="42" spans="1:23">
+      <c r="A42" s="62"/>
+    </row>
+    <row r="48" spans="1:23">
+      <c r="R48" s="169">
+        <v>42445</v>
+      </c>
+      <c r="S48" s="169">
+        <v>42476</v>
+      </c>
+      <c r="T48" s="169">
+        <v>42629</v>
+      </c>
+      <c r="U48" s="62" t="s">
+        <v>364</v>
+      </c>
+      <c r="V48" s="62" t="s">
+        <v>365</v>
+      </c>
+      <c r="W48" s="62" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="49" spans="17:23">
+      <c r="Q49" t="s">
+        <v>360</v>
+      </c>
+      <c r="R49">
+        <v>163</v>
+      </c>
+      <c r="S49">
+        <v>163</v>
+      </c>
+      <c r="T49">
+        <v>218</v>
+      </c>
+      <c r="U49">
+        <v>219</v>
+      </c>
+      <c r="V49">
+        <v>220</v>
+      </c>
+      <c r="W49">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="50" spans="17:23">
+      <c r="Q50" t="s">
+        <v>361</v>
+      </c>
+      <c r="R50">
+        <v>117</v>
+      </c>
+      <c r="S50">
+        <v>139</v>
+      </c>
+      <c r="T50">
+        <v>134</v>
+      </c>
+      <c r="U50">
+        <v>176</v>
+      </c>
+      <c r="V50">
+        <v>188</v>
+      </c>
+      <c r="W50">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="51" spans="17:23">
+      <c r="Q51" t="s">
+        <v>362</v>
+      </c>
+      <c r="R51">
+        <v>218</v>
+      </c>
+      <c r="S51">
+        <v>223</v>
+      </c>
+      <c r="T51">
+        <v>232</v>
+      </c>
+      <c r="U51">
+        <v>239</v>
+      </c>
+      <c r="V51">
+        <v>246</v>
+      </c>
+      <c r="W51">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="17:23">
+      <c r="Q52" t="s">
+        <v>363</v>
+      </c>
+      <c r="R52">
+        <v>1216</v>
+      </c>
+      <c r="S52">
+        <v>1231</v>
+      </c>
+      <c r="T52">
+        <v>1714</v>
+      </c>
+      <c r="U52">
+        <v>2010</v>
+      </c>
+      <c r="V52">
+        <v>2015</v>
+      </c>
+      <c r="W52">
+        <v>2131</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A19:L19"/>
+  <mergeCells count="2">
+    <mergeCell ref="A19:N19"/>
+    <mergeCell ref="Q22:U22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
     <hyperlink ref="B1" tooltip="Name" display="Name"/>
     <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
-    <hyperlink ref="D1" tooltip="Non Commenting Lines of Code" display="LOC"/>
-    <hyperlink ref="E1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
-    <hyperlink ref="F1" tooltip="Last Analysis" display="Last Analysis"/>
-    <hyperlink ref="G1" tooltip="Coverage by unit tests" display="Coverage"/>
-    <hyperlink ref="H1" tooltip="Condition coverage" display="Condition coverage"/>
-    <hyperlink ref="I1" tooltip="Blocker issues" display="Blocker issues"/>
-    <hyperlink ref="J1" tooltip="Critical issues" display="Critical issues"/>
-    <hyperlink ref="K1" tooltip="Major issues" display="Major issues"/>
-    <hyperlink ref="L1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="F1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="G1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="H1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="I1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="J1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="K1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="L1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="M1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="N1" tooltip="Minor issues" display="Minor issues"/>
     <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
     <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
     <hyperlink ref="B4" r:id="rId3" tooltip="svb-service-ooba"/>
@@ -39175,6 +40780,11 @@
     <hyperlink ref="B18" r:id="rId17" tooltip="svb-web-payment"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="S5:U16 S18:U18 S17:T17" emptyCellReference="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId18"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -39706,20 +41316,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="159" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
-      <c r="H15" s="158"/>
-      <c r="I15" s="158"/>
-      <c r="J15" s="158"/>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="159"/>
+      <c r="I15" s="159"/>
+      <c r="J15" s="159"/>
+      <c r="K15" s="159"/>
+      <c r="L15" s="159"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -39924,18 +41534,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="158"/>
-      <c r="B40" s="158"/>
-      <c r="C40" s="158"/>
-      <c r="D40" s="158"/>
-      <c r="E40" s="158"/>
-      <c r="F40" s="158"/>
-      <c r="G40" s="158"/>
-      <c r="H40" s="158"/>
-      <c r="I40" s="158"/>
-      <c r="J40" s="158"/>
-      <c r="K40" s="158"/>
-      <c r="L40" s="158"/>
+      <c r="A40" s="159"/>
+      <c r="B40" s="159"/>
+      <c r="C40" s="159"/>
+      <c r="D40" s="159"/>
+      <c r="E40" s="159"/>
+      <c r="F40" s="159"/>
+      <c r="G40" s="159"/>
+      <c r="H40" s="159"/>
+      <c r="I40" s="159"/>
+      <c r="J40" s="159"/>
+      <c r="K40" s="159"/>
+      <c r="L40" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -40569,20 +42179,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -41186,20 +42796,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -41809,20 +43419,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -42044,13 +43654,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="159" t="s">
+      <c r="U4" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="160"/>
-      <c r="W4" s="160"/>
-      <c r="X4" s="160"/>
-      <c r="Y4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -42087,9 +43697,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="162"/>
-      <c r="V5" s="163"/>
-      <c r="W5" s="163"/>
+      <c r="U5" s="163"/>
+      <c r="V5" s="164"/>
+      <c r="W5" s="164"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -42679,20 +44289,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -43473,20 +45083,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="158" t="s">
+      <c r="A16" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="158"/>
-      <c r="C16" s="158"/>
-      <c r="D16" s="158"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="158"/>
-      <c r="G16" s="158"/>
-      <c r="H16" s="158"/>
-      <c r="I16" s="158"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
+      <c r="B16" s="159"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="159"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="159"/>
+      <c r="L16" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
12/13/16 General Capture, added DT-Automation Directory and contents
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-580" yWindow="120" windowWidth="27380" windowHeight="16440" tabRatio="498" firstSheet="24" activeTab="33"/>
+    <workbookView xWindow="31140" yWindow="-660" windowWidth="28800" windowHeight="15060" tabRatio="498" firstSheet="26" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="10.28" sheetId="45" r:id="rId32"/>
     <sheet name="Sheet1" sheetId="46" r:id="rId33"/>
     <sheet name="11.14" sheetId="47" r:id="rId34"/>
+    <sheet name="11.28" sheetId="48" r:id="rId35"/>
   </sheets>
   <definedNames>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="29">'10.12'!$A$1:$N$18</definedName>
@@ -48,6 +49,7 @@
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="31">'10.28'!$A$1:$N$19</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="28">'10.3'!$A$1:$N$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="33">'11.14'!$A$1:$N$19</definedName>
+    <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="34">'11.28'!$A$1:$L$18</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="7">'3.18'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="8">'3.18 ++'!$A$1:$L$16</definedName>
     <definedName name="MarkSonarQubeMuranoTestOutput" localSheetId="9">'3.25'!$A$1:$L$16</definedName>
@@ -193,26 +195,29 @@
   <connection id="35" name="Connection4" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/index/12800?metric=tests/profiles/changelog?key=xml-murano-services-xml-profile-81269&amp;since=2015-09-02T19%3A11%3A38%2B0000&amp;to=2016-01-14T22%3A14%3A37%2B0000" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="36" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="36" name="Connection40" type="4" refreshedVersion="0" background="1" saveData="1">
+    <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=8" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="37" name="Connection5" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="37" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="38" name="Connection6" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="38" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="39" name="Connection7" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="39" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="40" name="Connection8" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-msonaq1.dev.svbank.com:9000/dashboard/?did=5" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="40" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
+  <connection id="41" name="Connection9" type="4" refreshedVersion="0" background="1" saveData="1">
     <webPr url="http://sal-dvs-mjenk01.dev.svbank.com:8080/job/T2%20web-payment-test-master/lastBuild/consoleText" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="370">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1316,6 +1321,15 @@
   <si>
     <t>2016-22</t>
   </si>
+  <si>
+    <t xml:space="preserve">45min </t>
+  </si>
+  <si>
+    <t>2016 - 23</t>
+  </si>
+  <si>
+    <t>2016 - 24</t>
+  </si>
 </sst>
 </file>
 
@@ -1871,7 +1885,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="78">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1950,8 +1964,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2274,6 +2289,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2294,12 +2321,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="78">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2376,6 +2399,7 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2660,11 +2684,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2144292520"/>
-        <c:axId val="2144087144"/>
+        <c:axId val="2120112232"/>
+        <c:axId val="2120115352"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2144292520"/>
+        <c:axId val="2120112232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2673,7 +2697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144087144"/>
+        <c:crossAx val="2120115352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2681,7 +2705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144087144"/>
+        <c:axId val="2120115352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2692,14 +2716,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144292520"/>
+        <c:crossAx val="2120112232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2760,9 +2783,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:f>'11.14'!$R$48:$Y$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>16-Mar</c:v>
                 </c:pt>
@@ -2781,15 +2804,21 @@
                 <c:pt idx="5">
                   <c:v>2016-22</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016 - 23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016 - 24</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'11.14'!$R$52:$W$52</c:f>
+              <c:f>'11.14'!$R$52:$Y$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1216.0</c:v>
                 </c:pt>
@@ -2807,6 +2836,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>2131.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2152.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2139.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2828,9 +2863,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:f>'11.14'!$R$48:$Y$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>16-Mar</c:v>
                 </c:pt>
@@ -2849,15 +2884,21 @@
                 <c:pt idx="5">
                   <c:v>2016-22</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016 - 23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016 - 24</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'11.14'!$R$51:$W$51</c:f>
+              <c:f>'11.14'!$R$51:$Y$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>218.0</c:v>
                 </c:pt>
@@ -2875,6 +2916,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>193.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2896,9 +2943,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:f>'11.14'!$R$48:$Y$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>16-Mar</c:v>
                 </c:pt>
@@ -2917,15 +2964,21 @@
                 <c:pt idx="5">
                   <c:v>2016-22</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016 - 23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016 - 24</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'11.14'!$R$50:$W$50</c:f>
+              <c:f>'11.14'!$R$50:$Y$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>117.0</c:v>
                 </c:pt>
@@ -2943,6 +2996,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>203.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>203.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>201.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2964,9 +3023,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'11.14'!$R$48:$W$48</c:f>
+              <c:f>'11.14'!$R$48:$Y$48</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>16-Mar</c:v>
                 </c:pt>
@@ -2985,15 +3044,21 @@
                 <c:pt idx="5">
                   <c:v>2016-22</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016 - 23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016 - 24</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'11.14'!$R$49:$W$49</c:f>
+              <c:f>'11.14'!$R$49:$Y$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>163.0</c:v>
                 </c:pt>
@@ -3012,6 +3077,12 @@
                 <c:pt idx="5">
                   <c:v>223.0</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>224.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3024,11 +3095,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2146090136"/>
-        <c:axId val="2146333752"/>
+        <c:axId val="2121287096"/>
+        <c:axId val="2121290216"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2146090136"/>
+        <c:axId val="2121287096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3108,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146333752"/>
+        <c:crossAx val="2121290216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3045,7 +3116,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2146333752"/>
+        <c:axId val="2121290216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3056,7 +3127,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146090136"/>
+        <c:crossAx val="2121287096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3219,15 +3290,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3250,7 +3321,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3294,7 +3365,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3338,7 +3409,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="36" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MSN_MarkWebQueryTest" headers="0" connectionId="37" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3346,15 +3417,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="36" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9443,13 +9518,13 @@
       <c r="L4" s="35">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -9486,9 +9561,9 @@
       <c r="L5" s="35">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -10070,20 +10145,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -10546,13 +10621,13 @@
       <c r="L4" s="36">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -10589,9 +10664,9 @@
       <c r="L5" s="36">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -11173,20 +11248,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>12</v>
       </c>
@@ -11381,13 +11456,13 @@
       <c r="Q25" s="14"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
-      <c r="U25" s="160" t="s">
+      <c r="U25" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V25" s="161"/>
-      <c r="W25" s="161"/>
-      <c r="X25" s="161"/>
-      <c r="Y25" s="162"/>
+      <c r="V25" s="167"/>
+      <c r="W25" s="167"/>
+      <c r="X25" s="167"/>
+      <c r="Y25" s="168"/>
     </row>
     <row r="26" spans="2:25">
       <c r="N26" s="14">
@@ -11400,9 +11475,9 @@
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
-      <c r="U26" s="163"/>
-      <c r="V26" s="164"/>
-      <c r="W26" s="164"/>
+      <c r="U26" s="169"/>
+      <c r="V26" s="170"/>
+      <c r="W26" s="170"/>
       <c r="X26" s="37" t="s">
         <v>165</v>
       </c>
@@ -11796,13 +11871,13 @@
       <c r="L4" s="63">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -11839,9 +11914,9 @@
       <c r="L5" s="63">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -12431,20 +12506,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -12967,13 +13042,13 @@
       <c r="L4" s="65">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -13010,9 +13085,9 @@
       <c r="L5" s="65">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -13613,20 +13688,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -14171,13 +14246,13 @@
       <c r="L4" s="66">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="18" customHeight="1">
       <c r="A5" s="20"/>
@@ -14214,9 +14289,9 @@
       <c r="L5" s="66">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -14827,20 +14902,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -15377,13 +15452,13 @@
       <c r="L4" s="68">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -15420,9 +15495,9 @@
       <c r="L5" s="68">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -16033,20 +16108,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -16583,13 +16658,13 @@
       <c r="L4" s="67">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -16626,9 +16701,9 @@
       <c r="L5" s="67">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -17239,20 +17314,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -17789,13 +17864,13 @@
       <c r="L4" s="69">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -17832,9 +17907,9 @@
       <c r="L5" s="69">
         <v>1</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -18445,20 +18520,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>14</v>
       </c>
@@ -18998,13 +19073,13 @@
       <c r="L4" s="70">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -19041,9 +19116,9 @@
       <c r="L5" s="70">
         <v>1</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -19657,20 +19732,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -20147,13 +20222,13 @@
       <c r="L4" s="71">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -20190,9 +20265,9 @@
       <c r="L5" s="71">
         <v>1</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -20806,20 +20881,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>267</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -21961,13 +22036,13 @@
       <c r="L4" s="73">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="17" customHeight="1">
       <c r="A5" s="20"/>
@@ -22004,9 +22079,9 @@
       <c r="L5" s="73">
         <v>1</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -22620,20 +22695,20 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14" t="s">
         <v>263</v>
       </c>
@@ -23723,20 +23798,20 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="17" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14"/>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -24819,20 +24894,20 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="165" t="s">
         <v>270</v>
       </c>
-      <c r="B15" s="159"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
-      <c r="L15" s="159"/>
+      <c r="B15" s="165"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
+      <c r="L15" s="165"/>
       <c r="N15" s="14"/>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -26813,21 +26888,21 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
-      <c r="M16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
+      <c r="M16" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -27691,21 +27766,21 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
-      <c r="M16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
+      <c r="M16" s="165"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -28586,20 +28661,20 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
     <row r="22" spans="1:12" ht="15">
       <c r="A22" s="19"/>
@@ -30038,20 +30113,20 @@
       </c>
     </row>
     <row r="16" spans="1:20">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="O16" s="14"/>
       <c r="Q16" s="14"/>
       <c r="R16" s="14"/>
@@ -31085,20 +31160,20 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="159" t="s">
+      <c r="A17" s="165" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="159"/>
-      <c r="C17" s="159"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
-      <c r="K17" s="159"/>
-      <c r="L17" s="159"/>
+      <c r="B17" s="165"/>
+      <c r="C17" s="165"/>
+      <c r="D17" s="165"/>
+      <c r="E17" s="165"/>
+      <c r="F17" s="165"/>
+      <c r="G17" s="165"/>
+      <c r="H17" s="165"/>
+      <c r="I17" s="165"/>
+      <c r="J17" s="165"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="165"/>
     </row>
     <row r="18" spans="1:19" ht="15" thickBot="1">
       <c r="B18" t="s">
@@ -31109,13 +31184,13 @@
       <c r="B19" t="s">
         <v>273</v>
       </c>
-      <c r="O19" s="165" t="s">
+      <c r="O19" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="P19" s="166"/>
-      <c r="Q19" s="166"/>
-      <c r="R19" s="166"/>
-      <c r="S19" s="167"/>
+      <c r="P19" s="172"/>
+      <c r="Q19" s="172"/>
+      <c r="R19" s="172"/>
+      <c r="S19" s="173"/>
     </row>
     <row r="20" spans="1:19" ht="17" customHeight="1">
       <c r="O20" s="124"/>
@@ -32205,34 +32280,34 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="15" thickBot="1">
-      <c r="A18" s="159" t="s">
+      <c r="A18" s="165" t="s">
         <v>330</v>
       </c>
-      <c r="B18" s="159"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="159"/>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
-      <c r="L18" s="159"/>
-      <c r="M18" s="159"/>
-      <c r="N18" s="159"/>
+      <c r="B18" s="165"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
+      <c r="L18" s="165"/>
+      <c r="M18" s="165"/>
+      <c r="N18" s="165"/>
     </row>
     <row r="19" spans="1:21" ht="15" thickBot="1">
       <c r="B19" t="s">
         <v>272</v>
       </c>
-      <c r="Q19" s="165" t="s">
+      <c r="Q19" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="R19" s="166"/>
-      <c r="S19" s="166"/>
-      <c r="T19" s="166"/>
-      <c r="U19" s="167"/>
+      <c r="R19" s="172"/>
+      <c r="S19" s="172"/>
+      <c r="T19" s="172"/>
+      <c r="U19" s="173"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -34082,13 +34157,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="165" t="s">
+      <c r="Q22" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="166"/>
-      <c r="S22" s="166"/>
-      <c r="T22" s="166"/>
-      <c r="U22" s="167"/>
+      <c r="R22" s="172"/>
+      <c r="S22" s="172"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="173"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -35774,22 +35849,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="159" t="s">
+      <c r="A19" s="165" t="s">
         <v>352</v>
       </c>
-      <c r="B19" s="159"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -35802,13 +35877,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="165" t="s">
+      <c r="Q22" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="166"/>
-      <c r="S22" s="166"/>
-      <c r="T22" s="166"/>
-      <c r="U22" s="167"/>
+      <c r="R22" s="172"/>
+      <c r="S22" s="172"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="173"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -37069,22 +37144,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="159" t="s">
+      <c r="A19" s="165" t="s">
         <v>330</v>
       </c>
-      <c r="B19" s="159"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
     </row>
     <row r="20" spans="1:21">
       <c r="B20" t="s">
@@ -37097,13 +37172,13 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="15" thickBot="1">
-      <c r="Q22" s="165" t="s">
+      <c r="Q22" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="166"/>
-      <c r="S22" s="166"/>
-      <c r="T22" s="166"/>
-      <c r="U22" s="167"/>
+      <c r="R22" s="172"/>
+      <c r="S22" s="172"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="173"/>
     </row>
     <row r="23" spans="1:21">
       <c r="B23" t="s">
@@ -37427,13 +37502,13 @@
       </c>
     </row>
     <row r="52" spans="6:23">
-      <c r="R52" s="169">
+      <c r="R52" s="161">
         <v>42445</v>
       </c>
-      <c r="S52" s="169">
+      <c r="S52" s="161">
         <v>42476</v>
       </c>
-      <c r="T52" s="169">
+      <c r="T52" s="161">
         <v>42629</v>
       </c>
       <c r="U52" s="62" t="s">
@@ -38452,24 +38527,24 @@
       </c>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="159" t="s">
+      <c r="A19" s="165" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="159"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
-      <c r="O19" s="159"/>
-      <c r="P19" s="159"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
+      <c r="O19" s="165"/>
+      <c r="P19" s="165"/>
     </row>
     <row r="23" spans="1:16" ht="60">
       <c r="A23" s="18" t="s">
@@ -39270,20 +39345,20 @@
       </c>
     </row>
     <row r="43" spans="1:16">
-      <c r="A43" s="159" t="s">
+      <c r="A43" s="165" t="s">
         <v>357</v>
       </c>
-      <c r="B43" s="159"/>
-      <c r="C43" s="159"/>
-      <c r="D43" s="159"/>
-      <c r="E43" s="159"/>
-      <c r="F43" s="159"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="159"/>
-      <c r="I43" s="159"/>
-      <c r="J43" s="159"/>
-      <c r="K43" s="159"/>
-      <c r="L43" s="159"/>
+      <c r="B43" s="165"/>
+      <c r="C43" s="165"/>
+      <c r="D43" s="165"/>
+      <c r="E43" s="165"/>
+      <c r="F43" s="165"/>
+      <c r="G43" s="165"/>
+      <c r="H43" s="165"/>
+      <c r="I43" s="165"/>
+      <c r="J43" s="165"/>
+      <c r="K43" s="165"/>
+      <c r="L43" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -39363,10 +39438,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="R45" sqref="R45"/>
+    <sheetView tabSelected="1" topLeftCell="G20" workbookViewId="0">
+      <selection activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -39390,7 +39465,8 @@
     <col min="19" max="19" width="22.33203125" customWidth="1"/>
     <col min="20" max="20" width="19.1640625" customWidth="1"/>
     <col min="21" max="21" width="13.83203125" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="168"/>
+    <col min="24" max="24" width="10.83203125" style="160"/>
+    <col min="25" max="25" width="10.83203125" style="163"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45">
@@ -40300,22 +40376,22 @@
       <c r="T18" s="59"/>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="159" t="s">
+      <c r="A19" s="165" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="159"/>
-      <c r="C19" s="159"/>
-      <c r="D19" s="159"/>
-      <c r="E19" s="159"/>
-      <c r="F19" s="159"/>
-      <c r="G19" s="159"/>
-      <c r="H19" s="159"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
-      <c r="K19" s="159"/>
-      <c r="L19" s="159"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="159"/>
+      <c r="B19" s="165"/>
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="165"/>
+      <c r="F19" s="165"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="165"/>
+      <c r="I19" s="165"/>
+      <c r="J19" s="165"/>
+      <c r="K19" s="165"/>
+      <c r="L19" s="165"/>
+      <c r="M19" s="165"/>
+      <c r="N19" s="165"/>
     </row>
     <row r="20" spans="1:24">
       <c r="B20" t="s">
@@ -40328,19 +40404,19 @@
       </c>
     </row>
     <row r="22" spans="1:24" ht="15" thickBot="1">
-      <c r="Q22" s="165" t="s">
+      <c r="Q22" s="171" t="s">
         <v>164</v>
       </c>
-      <c r="R22" s="166"/>
-      <c r="S22" s="166"/>
-      <c r="T22" s="166"/>
-      <c r="U22" s="167"/>
-      <c r="W22">
-        <v>223</v>
-      </c>
-      <c r="X22" s="168">
+      <c r="R22" s="172"/>
+      <c r="S22" s="172"/>
+      <c r="T22" s="172"/>
+      <c r="U22" s="173"/>
+      <c r="W22" s="163">
+        <v>224</v>
+      </c>
+      <c r="X22" s="160">
         <f>W22/W$26</f>
-        <v>8.0885019949220163E-2</v>
+        <v>8.1247733043162865E-2</v>
       </c>
     </row>
     <row r="23" spans="1:24">
@@ -40365,12 +40441,12 @@
       <c r="U23" s="145" t="s">
         <v>356</v>
       </c>
-      <c r="W23">
-        <v>203</v>
-      </c>
-      <c r="X23" s="168">
+      <c r="W23" s="163">
+        <v>201</v>
+      </c>
+      <c r="X23" s="160">
         <f t="shared" ref="X23:X26" si="2">W23/W$26</f>
-        <v>7.3630758070366342E-2</v>
+        <v>7.2905331882480953E-2</v>
       </c>
     </row>
     <row r="24" spans="1:24">
@@ -40384,12 +40460,12 @@
         <v>2</v>
       </c>
       <c r="U24" s="146"/>
-      <c r="W24">
-        <v>200</v>
-      </c>
-      <c r="X24" s="168">
+      <c r="W24" s="163">
+        <v>193</v>
+      </c>
+      <c r="X24" s="160">
         <f t="shared" si="2"/>
-        <v>7.2542618788538266E-2</v>
+        <v>7.0003627130939425E-2</v>
       </c>
     </row>
     <row r="25" spans="1:24">
@@ -40418,12 +40494,12 @@
         <f>T25/$T$32</f>
         <v>8.0885019949220163E-2</v>
       </c>
-      <c r="W25">
-        <v>2131</v>
-      </c>
-      <c r="X25" s="168">
+      <c r="W25" s="163">
+        <v>2139</v>
+      </c>
+      <c r="X25" s="160">
         <f t="shared" si="2"/>
-        <v>0.77294160319187522</v>
+        <v>0.77584330794341672</v>
       </c>
     </row>
     <row r="26" spans="1:24">
@@ -40449,7 +40525,7 @@
         <f>SUM(W22:W25)</f>
         <v>2757</v>
       </c>
-      <c r="X26" s="168">
+      <c r="X26" s="160">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -40555,7 +40631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:25">
       <c r="B33" s="122" t="s">
         <v>276</v>
       </c>
@@ -40576,7 +40652,7 @@
       <c r="M33" s="122"/>
       <c r="N33" s="122"/>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:25">
       <c r="B34" t="s">
         <v>339</v>
       </c>
@@ -40590,12 +40666,12 @@
         <v>328</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:25">
       <c r="A36" s="62" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:25">
       <c r="A37" s="62" t="s">
         <v>343</v>
       </c>
@@ -40603,13 +40679,13 @@
         <v>341</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:25">
       <c r="A38" s="62"/>
       <c r="B38" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:25">
       <c r="A39" s="62" t="s">
         <v>344</v>
       </c>
@@ -40617,7 +40693,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:25">
       <c r="A40" s="62" t="s">
         <v>346</v>
       </c>
@@ -40625,20 +40701,20 @@
         <v>354</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:25">
       <c r="A41" s="62"/>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:25">
       <c r="A42" s="62"/>
     </row>
-    <row r="48" spans="1:23">
-      <c r="R48" s="169">
+    <row r="48" spans="1:25">
+      <c r="R48" s="161">
         <v>42445</v>
       </c>
-      <c r="S48" s="169">
+      <c r="S48" s="161">
         <v>42476</v>
       </c>
-      <c r="T48" s="169">
+      <c r="T48" s="161">
         <v>42629</v>
       </c>
       <c r="U48" s="62" t="s">
@@ -40650,8 +40726,14 @@
       <c r="W48" s="62" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="49" spans="17:23">
+      <c r="X48" s="62" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y48" s="164" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="49" spans="17:25">
       <c r="Q49" t="s">
         <v>360</v>
       </c>
@@ -40673,8 +40755,14 @@
       <c r="W49">
         <v>223</v>
       </c>
-    </row>
-    <row r="50" spans="17:23">
+      <c r="X49">
+        <v>223</v>
+      </c>
+      <c r="Y49" s="163">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="50" spans="17:25">
       <c r="Q50" t="s">
         <v>361</v>
       </c>
@@ -40696,8 +40784,14 @@
       <c r="W50">
         <v>203</v>
       </c>
-    </row>
-    <row r="51" spans="17:23">
+      <c r="X50">
+        <v>203</v>
+      </c>
+      <c r="Y50" s="163">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="51" spans="17:25">
       <c r="Q51" t="s">
         <v>362</v>
       </c>
@@ -40719,8 +40813,14 @@
       <c r="W51">
         <v>200</v>
       </c>
-    </row>
-    <row r="52" spans="17:23">
+      <c r="X51">
+        <v>196</v>
+      </c>
+      <c r="Y51" s="163">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="17:25">
       <c r="Q52" t="s">
         <v>363</v>
       </c>
@@ -40742,6 +40842,15 @@
       <c r="W52">
         <v>2131</v>
       </c>
+      <c r="X52">
+        <v>2152</v>
+      </c>
+      <c r="Y52" s="163">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="56" spans="17:25">
+      <c r="X56" s="162"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -40793,6 +40902,707 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="45">
+      <c r="A1" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="159">
+        <v>491</v>
+      </c>
+      <c r="D2" s="23">
+        <v>5271</v>
+      </c>
+      <c r="E2" s="159" t="s">
+        <v>367</v>
+      </c>
+      <c r="F2" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G2" s="25">
+        <v>0.92</v>
+      </c>
+      <c r="H2" s="25">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="I2" s="159">
+        <v>0</v>
+      </c>
+      <c r="J2" s="159">
+        <v>0</v>
+      </c>
+      <c r="K2" s="159">
+        <v>2</v>
+      </c>
+      <c r="L2" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15">
+      <c r="A3" s="20"/>
+      <c r="B3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="159">
+        <v>194</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1760</v>
+      </c>
+      <c r="E3" s="159" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="24">
+        <v>42695</v>
+      </c>
+      <c r="G3" s="25">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="I3" s="159">
+        <v>0</v>
+      </c>
+      <c r="J3" s="159">
+        <v>0</v>
+      </c>
+      <c r="K3" s="159">
+        <v>2</v>
+      </c>
+      <c r="L3" s="159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15">
+      <c r="A4" s="19"/>
+      <c r="B4" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="159">
+        <v>181</v>
+      </c>
+      <c r="D4" s="23">
+        <v>2270</v>
+      </c>
+      <c r="E4" s="159" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="24">
+        <v>42699</v>
+      </c>
+      <c r="G4" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="I4" s="159">
+        <v>0</v>
+      </c>
+      <c r="J4" s="159">
+        <v>0</v>
+      </c>
+      <c r="K4" s="159">
+        <v>2</v>
+      </c>
+      <c r="L4" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15">
+      <c r="A5" s="20"/>
+      <c r="B5" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="159">
+        <v>135</v>
+      </c>
+      <c r="D5" s="159">
+        <v>904</v>
+      </c>
+      <c r="E5" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G5" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="I5" s="159">
+        <v>0</v>
+      </c>
+      <c r="J5" s="159">
+        <v>0</v>
+      </c>
+      <c r="K5" s="159">
+        <v>1</v>
+      </c>
+      <c r="L5" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15">
+      <c r="A6" s="20"/>
+      <c r="B6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="159">
+        <v>114</v>
+      </c>
+      <c r="D6" s="23">
+        <v>1638</v>
+      </c>
+      <c r="E6" s="159" t="s">
+        <v>355</v>
+      </c>
+      <c r="F6" s="24">
+        <v>42676</v>
+      </c>
+      <c r="G6" s="25">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="I6" s="159">
+        <v>0</v>
+      </c>
+      <c r="J6" s="159">
+        <v>0</v>
+      </c>
+      <c r="K6" s="159">
+        <v>2</v>
+      </c>
+      <c r="L6" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15">
+      <c r="A7" s="19"/>
+      <c r="B7" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="159">
+        <v>83</v>
+      </c>
+      <c r="D7" s="159">
+        <v>680</v>
+      </c>
+      <c r="E7" s="159" t="s">
+        <v>351</v>
+      </c>
+      <c r="F7" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G7" s="25">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="H7" s="25">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="I7" s="159">
+        <v>0</v>
+      </c>
+      <c r="J7" s="159">
+        <v>0</v>
+      </c>
+      <c r="K7" s="159">
+        <v>1</v>
+      </c>
+      <c r="L7" s="159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15">
+      <c r="A8" s="20"/>
+      <c r="B8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="159">
+        <v>69</v>
+      </c>
+      <c r="D8" s="159">
+        <v>839</v>
+      </c>
+      <c r="E8" s="159" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8" s="24">
+        <v>42657</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="I8" s="159">
+        <v>0</v>
+      </c>
+      <c r="J8" s="159">
+        <v>0</v>
+      </c>
+      <c r="K8" s="159">
+        <v>2</v>
+      </c>
+      <c r="L8" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="159">
+        <v>61</v>
+      </c>
+      <c r="D9" s="159">
+        <v>693</v>
+      </c>
+      <c r="E9" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G9" s="25">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="I9" s="159">
+        <v>0</v>
+      </c>
+      <c r="J9" s="159">
+        <v>0</v>
+      </c>
+      <c r="K9" s="159">
+        <v>0</v>
+      </c>
+      <c r="L9" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15">
+      <c r="A10" s="20"/>
+      <c r="B10" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="159">
+        <v>59</v>
+      </c>
+      <c r="D10" s="159">
+        <v>344</v>
+      </c>
+      <c r="E10" s="159">
+        <v>0</v>
+      </c>
+      <c r="F10" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G10" s="25">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="I10" s="159">
+        <v>0</v>
+      </c>
+      <c r="J10" s="159">
+        <v>0</v>
+      </c>
+      <c r="K10" s="159">
+        <v>0</v>
+      </c>
+      <c r="L10" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15">
+      <c r="A11" s="20"/>
+      <c r="B11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="159">
+        <v>36</v>
+      </c>
+      <c r="D11" s="159">
+        <v>195</v>
+      </c>
+      <c r="E11" s="159">
+        <v>0</v>
+      </c>
+      <c r="F11" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G11" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H11" s="25">
+        <v>1</v>
+      </c>
+      <c r="I11" s="159">
+        <v>0</v>
+      </c>
+      <c r="J11" s="159">
+        <v>0</v>
+      </c>
+      <c r="K11" s="159">
+        <v>0</v>
+      </c>
+      <c r="L11" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="159">
+        <v>31</v>
+      </c>
+      <c r="D12" s="159">
+        <v>378</v>
+      </c>
+      <c r="E12" s="159" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G12" s="25">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="H12" s="25">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="I12" s="159">
+        <v>0</v>
+      </c>
+      <c r="J12" s="159">
+        <v>0</v>
+      </c>
+      <c r="K12" s="159">
+        <v>1</v>
+      </c>
+      <c r="L12" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C13" s="159">
+        <v>31</v>
+      </c>
+      <c r="D13" s="159">
+        <v>402</v>
+      </c>
+      <c r="E13" s="159" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="24">
+        <v>42695</v>
+      </c>
+      <c r="G13" s="25">
+        <v>0.76</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="I13" s="159">
+        <v>0</v>
+      </c>
+      <c r="J13" s="159">
+        <v>0</v>
+      </c>
+      <c r="K13" s="159">
+        <v>1</v>
+      </c>
+      <c r="L13" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="159">
+        <v>20</v>
+      </c>
+      <c r="D14" s="159">
+        <v>179</v>
+      </c>
+      <c r="E14" s="159">
+        <v>0</v>
+      </c>
+      <c r="F14" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G14" s="25">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="I14" s="159">
+        <v>0</v>
+      </c>
+      <c r="J14" s="159">
+        <v>0</v>
+      </c>
+      <c r="K14" s="159">
+        <v>0</v>
+      </c>
+      <c r="L14" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15">
+      <c r="A15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="159">
+        <v>17</v>
+      </c>
+      <c r="D15" s="159">
+        <v>261</v>
+      </c>
+      <c r="E15" s="159">
+        <v>0</v>
+      </c>
+      <c r="F15" s="24">
+        <v>42692</v>
+      </c>
+      <c r="G15" s="25">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I15" s="159">
+        <v>0</v>
+      </c>
+      <c r="J15" s="159">
+        <v>0</v>
+      </c>
+      <c r="K15" s="159">
+        <v>0</v>
+      </c>
+      <c r="L15" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15">
+      <c r="A16" s="20"/>
+      <c r="B16" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="23">
+        <v>3041</v>
+      </c>
+      <c r="E16" s="159">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24">
+        <v>42578</v>
+      </c>
+      <c r="G16" s="25">
+        <v>0.91700000000000004</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="I16" s="159">
+        <v>0</v>
+      </c>
+      <c r="J16" s="159">
+        <v>0</v>
+      </c>
+      <c r="K16" s="159">
+        <v>0</v>
+      </c>
+      <c r="L16" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15">
+      <c r="A17" s="20"/>
+      <c r="B17" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="23">
+        <v>10687</v>
+      </c>
+      <c r="E17" s="159" t="s">
+        <v>359</v>
+      </c>
+      <c r="F17" s="24">
+        <v>42689</v>
+      </c>
+      <c r="G17" s="25">
+        <v>0</v>
+      </c>
+      <c r="H17" s="31"/>
+      <c r="I17" s="159">
+        <v>0</v>
+      </c>
+      <c r="J17" s="159">
+        <v>0</v>
+      </c>
+      <c r="K17" s="159">
+        <v>2</v>
+      </c>
+      <c r="L17" s="159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="165" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" s="165"/>
+      <c r="C18" s="165"/>
+      <c r="D18" s="165"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
+      <c r="L18" s="165"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="L27">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="L28">
+        <v>768</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A18:L18"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" tooltip="The project status with regard to its quality gate." display="QG"/>
+    <hyperlink ref="B1" tooltip="Name" display="Name"/>
+    <hyperlink ref="C1" tooltip="Number of unit tests" display="UTs "/>
+    <hyperlink ref="D1" tooltip="Non Commenting Lines of Code" display="LOC"/>
+    <hyperlink ref="E1" tooltip="Total effort (in days) to fix all the issues on the component and therefore to comply to all the requirements." display="Technical Debt"/>
+    <hyperlink ref="F1" tooltip="Last Analysis" display="Last Analysis"/>
+    <hyperlink ref="G1" tooltip="Coverage by unit tests" display="Coverage"/>
+    <hyperlink ref="H1" tooltip="Condition coverage" display="Condition coverage"/>
+    <hyperlink ref="I1" tooltip="Blocker issues" display="Blocker issues"/>
+    <hyperlink ref="J1" tooltip="Critical issues" display="Critical issues"/>
+    <hyperlink ref="K1" tooltip="Major issues" display="Major issues"/>
+    <hyperlink ref="L1" tooltip="Minor issues" display="Minor issues"/>
+    <hyperlink ref="B2" r:id="rId1" tooltip="svb-service-payments"/>
+    <hyperlink ref="B3" r:id="rId2" tooltip="svb-service-entitlement"/>
+    <hyperlink ref="B4" r:id="rId3" tooltip="svb-service-ooba"/>
+    <hyperlink ref="B5" r:id="rId4" tooltip="mur-java-lib-httpclient"/>
+    <hyperlink ref="B6" r:id="rId5" tooltip="svb-scheduler-payments"/>
+    <hyperlink ref="B7" r:id="rId6" tooltip="mur-java-lib-auth"/>
+    <hyperlink ref="B8" r:id="rId7" tooltip="svb-service-accounts"/>
+    <hyperlink ref="B9" r:id="rId8" tooltip="svb-service-csrf"/>
+    <hyperlink ref="B10" r:id="rId9" tooltip="mur-java-lib-dbconnector"/>
+    <hyperlink ref="B11" r:id="rId10" tooltip="mur-java-lib-logger"/>
+    <hyperlink ref="B12" r:id="rId11" tooltip="mur-java-lib-monitoring"/>
+    <hyperlink ref="B13" r:id="rId12" tooltip="svb-service-client"/>
+    <hyperlink ref="B14" r:id="rId13" tooltip="mur-java-lib-exception"/>
+    <hyperlink ref="B15" r:id="rId14" tooltip="mur-java-lib-mappers"/>
+    <hyperlink ref="B16" r:id="rId15" tooltip="svb-web-core-ui"/>
+    <hyperlink ref="B17" r:id="rId16" tooltip="svb-web-payment"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
@@ -41316,20 +42126,20 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="B15" s="159"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
-      <c r="K15" s="159"/>
-      <c r="L15" s="159"/>
+      <c r="B15" s="165"/>
+      <c r="C15" s="165"/>
+      <c r="D15" s="165"/>
+      <c r="E15" s="165"/>
+      <c r="F15" s="165"/>
+      <c r="G15" s="165"/>
+      <c r="H15" s="165"/>
+      <c r="I15" s="165"/>
+      <c r="J15" s="165"/>
+      <c r="K15" s="165"/>
+      <c r="L15" s="165"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="B16" s="29">
@@ -41534,18 +42344,18 @@
       <c r="L39" s="21"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="159"/>
-      <c r="B40" s="159"/>
-      <c r="C40" s="159"/>
-      <c r="D40" s="159"/>
-      <c r="E40" s="159"/>
-      <c r="F40" s="159"/>
-      <c r="G40" s="159"/>
-      <c r="H40" s="159"/>
-      <c r="I40" s="159"/>
-      <c r="J40" s="159"/>
-      <c r="K40" s="159"/>
-      <c r="L40" s="159"/>
+      <c r="A40" s="165"/>
+      <c r="B40" s="165"/>
+      <c r="C40" s="165"/>
+      <c r="D40" s="165"/>
+      <c r="E40" s="165"/>
+      <c r="F40" s="165"/>
+      <c r="G40" s="165"/>
+      <c r="H40" s="165"/>
+      <c r="I40" s="165"/>
+      <c r="J40" s="165"/>
+      <c r="K40" s="165"/>
+      <c r="L40" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -42179,20 +42989,20 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
     <row r="17" ht="15" customHeight="1"/>
     <row r="34" spans="2:2">
@@ -42796,20 +43606,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -43419,20 +44229,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
     <row r="17" ht="14" customHeight="1"/>
     <row r="18" ht="14" customHeight="1"/>
@@ -43654,13 +44464,13 @@
       <c r="L4" s="33">
         <v>0</v>
       </c>
-      <c r="U4" s="160" t="s">
+      <c r="U4" s="166" t="s">
         <v>164</v>
       </c>
-      <c r="V4" s="161"/>
-      <c r="W4" s="161"/>
-      <c r="X4" s="161"/>
-      <c r="Y4" s="162"/>
+      <c r="V4" s="167"/>
+      <c r="W4" s="167"/>
+      <c r="X4" s="167"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1">
       <c r="A5" s="20"/>
@@ -43697,9 +44507,9 @@
       <c r="L5" s="33">
         <v>0</v>
       </c>
-      <c r="U5" s="163"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="170"/>
+      <c r="W5" s="170"/>
       <c r="X5" s="37" t="s">
         <v>165</v>
       </c>
@@ -44289,20 +45099,20 @@
       <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:25" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
       <c r="N16" s="14">
         <v>9</v>
       </c>
@@ -45083,20 +45893,20 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="159"/>
-      <c r="C16" s="159"/>
-      <c r="D16" s="159"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="159"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
-      <c r="K16" s="159"/>
-      <c r="L16" s="159"/>
+      <c r="B16" s="165"/>
+      <c r="C16" s="165"/>
+      <c r="D16" s="165"/>
+      <c r="E16" s="165"/>
+      <c r="F16" s="165"/>
+      <c r="G16" s="165"/>
+      <c r="H16" s="165"/>
+      <c r="I16" s="165"/>
+      <c r="J16" s="165"/>
+      <c r="K16" s="165"/>
+      <c r="L16" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
12/20/16 Adding Calc-v2 and working contents minus node_modules
</commit_message>
<xml_diff>
--- a/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
+++ b/DesktopShortcuts/Murano Web Payment Automation Test Metrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="31140" yWindow="-660" windowWidth="28800" windowHeight="15060" tabRatio="498" firstSheet="26" activeTab="33"/>
+    <workbookView xWindow="32300" yWindow="-2120" windowWidth="26080" windowHeight="15520" tabRatio="458" firstSheet="26" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="How To" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2779" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2791" uniqueCount="380">
   <si>
     <t xml:space="preserve">Murano Test Automation </t>
   </si>
@@ -1330,6 +1330,36 @@
   <si>
     <t>2016 - 24</t>
   </si>
+  <si>
+    <t>Dashboar</t>
+  </si>
+  <si>
+    <t>Automate E2E</t>
+  </si>
+  <si>
+    <t>Auto Api Serv/Comp</t>
+  </si>
+  <si>
+    <t>Auto UI Comp</t>
+  </si>
+  <si>
+    <t>Sprint 2016-20</t>
+  </si>
+  <si>
+    <t>Sprint 2016-21</t>
+  </si>
+  <si>
+    <t>Sprint 2016-22</t>
+  </si>
+  <si>
+    <t>Sprint 2016-23</t>
+  </si>
+  <si>
+    <t>Sprint 2016-24</t>
+  </si>
+  <si>
+    <t>UK Payments</t>
+  </si>
 </sst>
 </file>
 
@@ -1885,7 +1915,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1965,8 +1995,15 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2321,8 +2358,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="86">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2400,11 +2438,26 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF717E"/>
+      <color rgb="FFF7A400"/>
+      <color rgb="FF8DB7F6"/>
+      <color rgb="FFDF5D5A"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -2684,11 +2737,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120112232"/>
-        <c:axId val="2120115352"/>
+        <c:axId val="2118129880"/>
+        <c:axId val="2107449976"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2120112232"/>
+        <c:axId val="2118129880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,7 +2750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120115352"/>
+        <c:crossAx val="2107449976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2705,7 +2758,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2120115352"/>
+        <c:axId val="2107449976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2716,7 +2769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120112232"/>
+        <c:crossAx val="2118129880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2781,6 +2834,15 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="43000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
           <c:cat>
             <c:strRef>
               <c:f>'11.14'!$R$48:$Y$48</c:f>
@@ -3095,11 +3157,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121287096"/>
-        <c:axId val="2121290216"/>
+        <c:axId val="2038789928"/>
+        <c:axId val="2038793048"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2121287096"/>
+        <c:axId val="2038789928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3108,7 +3170,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121290216"/>
+        <c:crossAx val="2038793048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3116,7 +3178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121290216"/>
+        <c:axId val="2038793048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3127,7 +3189,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121287096"/>
+        <c:crossAx val="2038789928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3142,6 +3204,498 @@
           <c:y val="0.314047098279382"/>
           <c:w val="0.125214262600737"/>
           <c:h val="0.371905803441236"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$81</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unit Test</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$81:$W$81</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>274.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>688.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>569.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>536.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>541.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$82</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Auto UI Comp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF717E"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$82:$W$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Auto Api Serv/Comp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F7A400"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$83:$W$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$84</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Automate E2E</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$84:$W$84</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>124.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>131.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>132.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>132.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>132.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>163.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$85</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Manual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$85:$W$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>173.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>212.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>212.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'11.14'!$Q$86</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'11.14'!$R$80:$W$80</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Sep-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2016-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 2016-21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Sprint 2016-22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sprint 2016-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sprint 2016-24</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'11.14'!$R$86:$W$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2117373352"/>
+        <c:axId val="2108752024"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="-2117373352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2108752024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2108752024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2117373352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79972627865137"/>
+          <c:y val="0.310289051530702"/>
+          <c:w val="0.153129880249921"/>
+          <c:h val="0.296499751456964"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3317,11 +3871,41 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>127002</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>84667</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3365,7 +3949,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest_1" headers="0" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkWebQueryTest" headers="0" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3417,11 +4001,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput_1" headers="0" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MarkSonarQubeMuranoTestOutput" headers="0" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1"/>
 </file>
 
 <file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39438,10 +40022,10 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y56"/>
+  <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" workbookViewId="0">
-      <selection activeCell="Y38" sqref="Y38"/>
+    <sheetView tabSelected="1" topLeftCell="F87" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="U125" sqref="U125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -39462,11 +40046,13 @@
     <col min="16" max="16" width="5.5" customWidth="1"/>
     <col min="17" max="17" width="20.1640625" customWidth="1"/>
     <col min="18" max="18" width="17.1640625" customWidth="1"/>
-    <col min="19" max="19" width="22.33203125" customWidth="1"/>
-    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="19" max="19" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.5" customWidth="1"/>
     <col min="21" max="21" width="13.83203125" customWidth="1"/>
-    <col min="24" max="24" width="10.83203125" style="160"/>
-    <col min="25" max="25" width="10.83203125" style="163"/>
+    <col min="22" max="23" width="11.6640625" customWidth="1"/>
+    <col min="24" max="24" width="11.6640625" style="160" customWidth="1"/>
+    <col min="25" max="25" width="11.6640625" style="163" customWidth="1"/>
+    <col min="26" max="28" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="45">
@@ -40707,6 +41293,11 @@
     <row r="42" spans="1:25">
       <c r="A42" s="62"/>
     </row>
+    <row r="45" spans="1:25">
+      <c r="Q45" t="s">
+        <v>379</v>
+      </c>
+    </row>
     <row r="48" spans="1:25">
       <c r="R48" s="161">
         <v>42445</v>
@@ -40851,6 +41442,165 @@
     </row>
     <row r="56" spans="17:25">
       <c r="X56" s="162"/>
+    </row>
+    <row r="76" spans="17:25">
+      <c r="Q76" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="80" spans="17:25">
+      <c r="Q80" s="163"/>
+      <c r="R80" s="174">
+        <v>42614</v>
+      </c>
+      <c r="S80" s="163" t="s">
+        <v>374</v>
+      </c>
+      <c r="T80" s="163" t="s">
+        <v>375</v>
+      </c>
+      <c r="U80" s="163" t="s">
+        <v>376</v>
+      </c>
+      <c r="V80" s="163" t="s">
+        <v>377</v>
+      </c>
+      <c r="W80" s="163" t="s">
+        <v>378</v>
+      </c>
+      <c r="X80"/>
+      <c r="Y80"/>
+    </row>
+    <row r="81" spans="17:25">
+      <c r="Q81" t="s">
+        <v>363</v>
+      </c>
+      <c r="R81" s="163">
+        <v>274</v>
+      </c>
+      <c r="S81" s="163">
+        <v>688</v>
+      </c>
+      <c r="T81" s="163">
+        <v>569</v>
+      </c>
+      <c r="U81" s="163">
+        <v>540</v>
+      </c>
+      <c r="V81" s="163">
+        <v>536</v>
+      </c>
+      <c r="W81" s="163">
+        <v>541</v>
+      </c>
+      <c r="X81"/>
+      <c r="Y81"/>
+    </row>
+    <row r="82" spans="17:25">
+      <c r="Q82" t="s">
+        <v>373</v>
+      </c>
+      <c r="R82" s="163">
+        <v>0</v>
+      </c>
+      <c r="S82" s="163">
+        <v>0</v>
+      </c>
+      <c r="T82" s="163">
+        <v>53</v>
+      </c>
+      <c r="U82" s="163">
+        <v>53</v>
+      </c>
+      <c r="V82" s="163">
+        <v>53</v>
+      </c>
+      <c r="W82" s="163">
+        <v>53</v>
+      </c>
+      <c r="X82"/>
+      <c r="Y82"/>
+    </row>
+    <row r="83" spans="17:25">
+      <c r="Q83" t="s">
+        <v>372</v>
+      </c>
+      <c r="R83" s="163">
+        <v>0</v>
+      </c>
+      <c r="S83" s="163">
+        <v>0</v>
+      </c>
+      <c r="T83" s="163">
+        <v>16</v>
+      </c>
+      <c r="U83" s="163">
+        <v>16</v>
+      </c>
+      <c r="V83" s="163">
+        <v>16</v>
+      </c>
+      <c r="W83" s="163">
+        <v>16</v>
+      </c>
+      <c r="X83"/>
+      <c r="Y83"/>
+    </row>
+    <row r="84" spans="17:25">
+      <c r="Q84" t="s">
+        <v>371</v>
+      </c>
+      <c r="R84" s="163">
+        <v>124</v>
+      </c>
+      <c r="S84" s="163">
+        <v>131</v>
+      </c>
+      <c r="T84" s="163">
+        <v>132</v>
+      </c>
+      <c r="U84" s="163">
+        <v>132</v>
+      </c>
+      <c r="V84" s="163">
+        <v>132</v>
+      </c>
+      <c r="W84" s="163">
+        <v>163</v>
+      </c>
+      <c r="X84"/>
+      <c r="Y84"/>
+    </row>
+    <row r="85" spans="17:25">
+      <c r="Q85" t="s">
+        <v>360</v>
+      </c>
+      <c r="R85" s="163">
+        <v>173</v>
+      </c>
+      <c r="S85" s="163">
+        <v>212</v>
+      </c>
+      <c r="T85" s="163">
+        <v>212</v>
+      </c>
+      <c r="U85" s="163">
+        <v>212</v>
+      </c>
+      <c r="V85" s="163">
+        <v>212</v>
+      </c>
+      <c r="W85" s="163">
+        <v>212</v>
+      </c>
+      <c r="X85"/>
+      <c r="Y85"/>
+    </row>
+    <row r="86" spans="17:25">
+      <c r="U86" s="160"/>
+      <c r="V86" s="163"/>
+      <c r="X86"/>
+      <c r="Y86"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -40906,7 +41656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>

</xml_diff>